<commit_message>
superdataset 24 (single model, mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="mae" sheetId="1" r:id="rId1"/>
+    <sheet name="mse" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -43,6 +44,12 @@
   </si>
   <si>
     <t>Hybrid model 3 (superdataset-24.csv) balanced</t>
+  </si>
+  <si>
+    <t>train (MSE)</t>
+  </si>
+  <si>
+    <t>test (MSE)</t>
   </si>
 </sst>
 </file>
@@ -96,7 +103,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -105,6 +112,10 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -387,8 +398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2430,4 +2441,1004 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:J57"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O18" sqref="O18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="2"/>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="2">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>3.9012656255087122E-3</v>
+      </c>
+      <c r="E5" s="4">
+        <v>2.6872809770650489E-2</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <f>C5+1</f>
+        <v>2</v>
+      </c>
+      <c r="D6" s="4">
+        <v>3.8802144292124029E-3</v>
+      </c>
+      <c r="E6" s="4">
+        <v>2.8297882858074969E-2</v>
+      </c>
+      <c r="H6" s="2">
+        <f>H5+1</f>
+        <v>2</v>
+      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f t="shared" ref="C7:C54" si="0">C6+1</f>
+        <v>3</v>
+      </c>
+      <c r="D7" s="4">
+        <v>3.8304198092593668E-3</v>
+      </c>
+      <c r="E7" s="4">
+        <v>2.6811164812730631E-2</v>
+      </c>
+      <c r="H7" s="2">
+        <f t="shared" ref="H7:H54" si="1">H6+1</f>
+        <v>3</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D8" s="4">
+        <v>3.6859332530850609E-3</v>
+      </c>
+      <c r="E8" s="4">
+        <v>2.8402875125575131E-2</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>3.80306349724318E-3</v>
+      </c>
+      <c r="E9" s="4">
+        <v>2.5853134642315759E-2</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D10" s="4">
+        <v>3.768815482112625E-3</v>
+      </c>
+      <c r="E10" s="4">
+        <v>3.0369313080958471E-2</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3.8064013351161341E-3</v>
+      </c>
+      <c r="E11" s="4">
+        <v>2.9039274741696479E-2</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I11" s="4"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3.8383955338046928E-3</v>
+      </c>
+      <c r="E12" s="4">
+        <v>2.7928201559299069E-2</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3.8991542600385911E-3</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2.8141538016755889E-2</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3.8535817048818829E-3</v>
+      </c>
+      <c r="E14" s="4">
+        <v>2.687925624265711E-2</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3.8035737978991042E-3</v>
+      </c>
+      <c r="E15" s="4">
+        <v>2.882085174650945E-2</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3.7016948072582652E-3</v>
+      </c>
+      <c r="E16" s="4">
+        <v>2.975635506976828E-2</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3.7794792730085069E-3</v>
+      </c>
+      <c r="E17" s="4">
+        <v>2.734510818016956E-2</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3.9511753103124696E-3</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2.549298724019286E-2</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3.9310945414033054E-3</v>
+      </c>
+      <c r="E19" s="4">
+        <v>2.4181809072906651E-2</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3.8895802447439631E-3</v>
+      </c>
+      <c r="E20" s="4">
+        <v>2.5848474995463978E-2</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3.9347203993610304E-3</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2.6240046834724091E-2</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3.8073867233460409E-3</v>
+      </c>
+      <c r="E22" s="4">
+        <v>2.8783177102295769E-2</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3.905734568014658E-3</v>
+      </c>
+      <c r="E23" s="4">
+        <v>2.481079967838417E-2</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3.8327794613647959E-3</v>
+      </c>
+      <c r="E24" s="4">
+        <v>2.6490374757372689E-2</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I24" s="4"/>
+      <c r="J24" s="4"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3.7937332617988938E-3</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2.8047402593543391E-2</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I25" s="4"/>
+      <c r="J25" s="4"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3.8909347802066349E-3</v>
+      </c>
+      <c r="E26" s="4">
+        <v>2.5780589083182689E-2</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I26" s="4"/>
+      <c r="J26" s="4"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3.876071983761956E-3</v>
+      </c>
+      <c r="E27" s="4">
+        <v>2.5570233238790499E-2</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3.940080044885135E-3</v>
+      </c>
+      <c r="E28" s="4">
+        <v>2.8819020744889162E-2</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I28" s="4"/>
+      <c r="J28" s="4"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D29" s="4">
+        <v>3.783030765446027E-3</v>
+      </c>
+      <c r="E29" s="4">
+        <v>3.0057788823361881E-2</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D30" s="4">
+        <v>3.8163153264058592E-3</v>
+      </c>
+      <c r="E30" s="4">
+        <v>3.036462570137707E-2</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I30" s="4"/>
+      <c r="J30" s="4"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D31" s="4">
+        <v>3.9225142717788566E-3</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2.6176243985086022E-2</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="4"/>
+      <c r="J31" s="4"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D32" s="4">
+        <v>3.825211961441108E-3</v>
+      </c>
+      <c r="E32" s="4">
+        <v>2.77923234996077E-2</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I32" s="4"/>
+      <c r="J32" s="4"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D33" s="4">
+        <v>3.7196619024681249E-3</v>
+      </c>
+      <c r="E33" s="4">
+        <v>3.1133483508790579E-2</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D34" s="4">
+        <v>3.882863579783511E-3</v>
+      </c>
+      <c r="E34" s="4">
+        <v>2.667409849898604E-2</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I34" s="4"/>
+      <c r="J34" s="4"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D35" s="4">
+        <v>3.8561259247562869E-3</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2.6440087674392359E-2</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I35" s="4"/>
+      <c r="J35" s="4"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D36" s="4">
+        <v>3.87087215101141E-3</v>
+      </c>
+      <c r="E36" s="4">
+        <v>2.8551800829002751E-2</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I36" s="4"/>
+      <c r="J36" s="4"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D37" s="4">
+        <v>3.8285427536956982E-3</v>
+      </c>
+      <c r="E37" s="4">
+        <v>2.6971365282784019E-2</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D38" s="4">
+        <v>3.816965740176077E-3</v>
+      </c>
+      <c r="E38" s="4">
+        <v>2.8085421339488811E-2</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I38" s="4"/>
+      <c r="J38" s="4"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D39" s="4">
+        <v>3.8379187546036348E-3</v>
+      </c>
+      <c r="E39" s="4">
+        <v>2.77635868504937E-2</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I39" s="4"/>
+      <c r="J39" s="4"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D40" s="4">
+        <v>3.8568270057973589E-3</v>
+      </c>
+      <c r="E40" s="4">
+        <v>2.7218575965366941E-2</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I40" s="4"/>
+      <c r="J40" s="4"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D41" s="4">
+        <v>3.80889543350832E-3</v>
+      </c>
+      <c r="E41" s="4">
+        <v>2.9723421719144799E-2</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D42" s="4">
+        <v>4.0074705160596091E-3</v>
+      </c>
+      <c r="E42" s="4">
+        <v>2.5739825124919659E-2</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I42" s="4"/>
+      <c r="J42" s="4"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D43" s="4">
+        <v>3.8453490871246292E-3</v>
+      </c>
+      <c r="E43" s="4">
+        <v>2.6779323254488101E-2</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D44" s="4">
+        <v>3.8696770321489972E-3</v>
+      </c>
+      <c r="E44" s="4">
+        <v>2.401601120272474E-2</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I44" s="4"/>
+      <c r="J44" s="4"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D45" s="4">
+        <v>3.85987498298773E-3</v>
+      </c>
+      <c r="E45" s="4">
+        <v>2.8005137930539891E-2</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D46" s="4">
+        <v>3.709589710884737E-3</v>
+      </c>
+      <c r="E46" s="4">
+        <v>3.0798913894152791E-2</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D47" s="4">
+        <v>3.839143271601504E-3</v>
+      </c>
+      <c r="E47" s="4">
+        <v>2.8537236460197641E-2</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I47" s="4"/>
+      <c r="J47" s="4"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D48" s="4">
+        <v>3.7703139498748012E-3</v>
+      </c>
+      <c r="E48" s="4">
+        <v>2.8668062253393911E-2</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D49" s="4">
+        <v>3.8507157867619509E-3</v>
+      </c>
+      <c r="E49" s="4">
+        <v>2.8005740654497211E-2</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I49" s="4"/>
+      <c r="J49" s="4"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D50" s="4">
+        <v>3.8623685416919211E-3</v>
+      </c>
+      <c r="E50" s="4">
+        <v>2.612216900567654E-2</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D51" s="4">
+        <v>3.721545626216185E-3</v>
+      </c>
+      <c r="E51" s="4">
+        <v>2.9210147704990919E-2</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D52" s="4">
+        <v>3.7979591781253392E-3</v>
+      </c>
+      <c r="E52" s="4">
+        <v>2.8592664583893521E-2</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I52" s="4"/>
+      <c r="J52" s="4"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D53" s="4">
+        <v>3.8286546026109719E-3</v>
+      </c>
+      <c r="E53" s="4">
+        <v>2.8166956626693759E-2</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I53" s="4"/>
+      <c r="J53" s="4"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D54" s="4">
+        <v>3.7450634272971472E-3</v>
+      </c>
+      <c r="E54" s="4">
+        <v>2.8923390865649719E-2</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I54" s="4"/>
+      <c r="J54" s="4"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="I55" s="5"/>
+      <c r="J55" s="5"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D56" s="4">
+        <f>AVERAGE(D5:D54)</f>
+        <v>3.8367751082377033E-3</v>
+      </c>
+      <c r="E56" s="4">
+        <f>AVERAGE(E5:E54)</f>
+        <v>2.7662021688572166E-2</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I56" s="4" t="e">
+        <f>AVERAGE(I5:I54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J56" s="4" t="e">
+        <f>AVERAGE(J5:J54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" s="4">
+        <f>_xlfn.STDEV.S(D5:D54)</f>
+        <v>6.7713886455263164E-5</v>
+      </c>
+      <c r="E57" s="4">
+        <f>_xlfn.STDEV.S(E5:E54)</f>
+        <v>1.6698090965107128E-3</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I57" s="4" t="e">
+        <f>_xlfn.STDEV.S(I5:I54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J57" s="4" t="e">
+        <f>_xlfn.STDEV.S(J5:J54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
superdataset-24 - positive flow test
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="mae" sheetId="1" r:id="rId1"/>
-    <sheet name="mse" sheetId="2" r:id="rId2"/>
+    <sheet name="pos vs neg" sheetId="3" r:id="rId1"/>
+    <sheet name="mae" sheetId="1" r:id="rId2"/>
+    <sheet name="mse" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -102,6 +103,18 @@
   <si>
     <t>beforeschool</t>
   </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 (positive flow).csv)</t>
+  </si>
+  <si>
+    <t>positive flow</t>
+  </si>
+  <si>
+    <t>negative flow</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 (negative flow).csv)</t>
+  </si>
 </sst>
 </file>
 
@@ -160,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -179,6 +192,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -1374,10 +1388,1323 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C4:T58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="18" max="18" width="20.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.85546875" customWidth="1"/>
+    <col min="20" max="20" width="17.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="H4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C5" s="2"/>
+      <c r="D5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C6" s="2">
+        <v>1</v>
+      </c>
+      <c r="D6" s="3">
+        <v>55.788316221765918</v>
+      </c>
+      <c r="E6" s="3">
+        <v>153.6779098360656</v>
+      </c>
+      <c r="H6" s="2">
+        <v>1</v>
+      </c>
+      <c r="I6" s="3">
+        <v>55.788316221765918</v>
+      </c>
+      <c r="J6" s="3">
+        <v>153.6779098360656</v>
+      </c>
+      <c r="R6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0.25852249577887998</v>
+      </c>
+      <c r="T6" s="3"/>
+    </row>
+    <row r="7" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C7" s="2">
+        <f>C6+1</f>
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>53.338449691991791</v>
+      </c>
+      <c r="E7" s="3">
+        <v>179.17241803278691</v>
+      </c>
+      <c r="H7" s="2">
+        <f>H6+1</f>
+        <v>2</v>
+      </c>
+      <c r="I7" s="3">
+        <v>53.338449691991791</v>
+      </c>
+      <c r="J7" s="3">
+        <v>179.17241803278691</v>
+      </c>
+      <c r="R7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="S7" s="3">
+        <v>2.9128855552448121E-2</v>
+      </c>
+      <c r="T7" s="3"/>
+    </row>
+    <row r="8" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C8" s="2">
+        <f t="shared" ref="C8:C55" si="0">C7+1</f>
+        <v>3</v>
+      </c>
+      <c r="D8" s="3">
+        <v>54.543285420944549</v>
+      </c>
+      <c r="E8" s="3">
+        <v>148.6551639344263</v>
+      </c>
+      <c r="H8" s="2">
+        <f t="shared" ref="H8:H55" si="1">H7+1</f>
+        <v>3</v>
+      </c>
+      <c r="I8" s="3">
+        <v>54.543285420944549</v>
+      </c>
+      <c r="J8" s="3">
+        <v>148.6551639344263</v>
+      </c>
+      <c r="R8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="S8" s="3">
+        <v>4.4655059358944323E-2</v>
+      </c>
+      <c r="T8" s="3"/>
+    </row>
+    <row r="9" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D9" s="3">
+        <v>54.764691991786442</v>
+      </c>
+      <c r="E9" s="3">
+        <v>159.42118852459021</v>
+      </c>
+      <c r="H9" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="I9" s="3">
+        <v>54.764691991786442</v>
+      </c>
+      <c r="J9" s="3">
+        <v>159.42118852459021</v>
+      </c>
+      <c r="R9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="S9" s="3">
+        <v>3.4533933905929091E-2</v>
+      </c>
+      <c r="T9" s="3"/>
+    </row>
+    <row r="10" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D10" s="3">
+        <v>57.240513347022578</v>
+      </c>
+      <c r="E10" s="3">
+        <v>140.6745901639344</v>
+      </c>
+      <c r="H10" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="I10" s="3">
+        <v>57.240513347022578</v>
+      </c>
+      <c r="J10" s="3">
+        <v>140.6745901639344</v>
+      </c>
+      <c r="R10" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S10" s="3">
+        <v>5.1912290768252677E-2</v>
+      </c>
+      <c r="T10" s="3"/>
+    </row>
+    <row r="11" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D11" s="3">
+        <v>56.165903490759767</v>
+      </c>
+      <c r="E11" s="3">
+        <v>156.73520491803279</v>
+      </c>
+      <c r="H11" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="I11" s="3">
+        <v>56.165903490759767</v>
+      </c>
+      <c r="J11" s="3">
+        <v>156.73520491803279</v>
+      </c>
+      <c r="R11" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="S11" s="3">
+        <v>6.1876215419234312E-2</v>
+      </c>
+      <c r="T11" s="3"/>
+    </row>
+    <row r="12" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C12" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="D12" s="3">
+        <v>55.818049281314167</v>
+      </c>
+      <c r="E12" s="3">
+        <v>155.67159836065579</v>
+      </c>
+      <c r="H12" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="I12" s="3">
+        <v>55.818049281314167</v>
+      </c>
+      <c r="J12" s="3">
+        <v>155.67159836065579</v>
+      </c>
+      <c r="R12" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0.15274357333507019</v>
+      </c>
+      <c r="T12" s="3"/>
+    </row>
+    <row r="13" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D13" s="3">
+        <v>56.226232032854213</v>
+      </c>
+      <c r="E13" s="3">
+        <v>154.82508196721309</v>
+      </c>
+      <c r="H13" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="I13" s="3">
+        <v>56.226232032854213</v>
+      </c>
+      <c r="J13" s="3">
+        <v>154.82508196721309</v>
+      </c>
+      <c r="R13" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="S13" s="3">
+        <v>4.0969016499390998E-2</v>
+      </c>
+      <c r="T13" s="3"/>
+    </row>
+    <row r="14" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C14" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="D14" s="3">
+        <v>55.524517453798779</v>
+      </c>
+      <c r="E14" s="3">
+        <v>160.09938524590169</v>
+      </c>
+      <c r="H14" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="I14" s="3">
+        <v>55.524517453798779</v>
+      </c>
+      <c r="J14" s="3">
+        <v>160.09938524590169</v>
+      </c>
+      <c r="R14" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="S14" s="3">
+        <v>3.771698471518789E-2</v>
+      </c>
+      <c r="T14" s="3"/>
+    </row>
+    <row r="15" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C15" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="D15" s="3">
+        <v>56.176724845995892</v>
+      </c>
+      <c r="E15" s="3">
+        <v>145.51348360655729</v>
+      </c>
+      <c r="H15" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="I15" s="3">
+        <v>56.176724845995892</v>
+      </c>
+      <c r="J15" s="3">
+        <v>145.51348360655729</v>
+      </c>
+      <c r="R15" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S15" s="3">
+        <v>3.839653741383061E-2</v>
+      </c>
+      <c r="T15" s="3"/>
+    </row>
+    <row r="16" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C16" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="D16" s="3">
+        <v>56.98952772073924</v>
+      </c>
+      <c r="E16" s="3">
+        <v>140.51717213114759</v>
+      </c>
+      <c r="H16" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="I16" s="3">
+        <v>56.98952772073924</v>
+      </c>
+      <c r="J16" s="3">
+        <v>140.51717213114759</v>
+      </c>
+      <c r="R16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="S16" s="3">
+        <v>4.2972143084908702E-2</v>
+      </c>
+      <c r="T16" s="3"/>
+    </row>
+    <row r="17" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C17" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="D17" s="3">
+        <v>57.912607802874739</v>
+      </c>
+      <c r="E17" s="3">
+        <v>131.7270491803279</v>
+      </c>
+      <c r="H17" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="I17" s="3">
+        <v>57.912607802874739</v>
+      </c>
+      <c r="J17" s="3">
+        <v>131.7270491803279</v>
+      </c>
+      <c r="R17" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="S17" s="3">
+        <v>9.8865933722695101E-2</v>
+      </c>
+      <c r="T17" s="3"/>
+    </row>
+    <row r="18" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C18" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="3">
+        <v>55.247936344969212</v>
+      </c>
+      <c r="E18" s="3">
+        <v>151.11500000000001</v>
+      </c>
+      <c r="H18" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="I18" s="3">
+        <v>55.247936344969212</v>
+      </c>
+      <c r="J18" s="3">
+        <v>151.11500000000001</v>
+      </c>
+      <c r="R18" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="S18" s="3">
+        <v>2.8654657279261069E-2</v>
+      </c>
+      <c r="T18" s="3"/>
+    </row>
+    <row r="19" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C19" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>56.018305954825458</v>
+      </c>
+      <c r="E19" s="3">
+        <v>163.21016393442619</v>
+      </c>
+      <c r="H19" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="I19" s="3">
+        <v>56.018305954825458</v>
+      </c>
+      <c r="J19" s="3">
+        <v>163.21016393442619</v>
+      </c>
+      <c r="R19" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="S19" s="3">
+        <v>3.1342373340615473E-2</v>
+      </c>
+      <c r="T19" s="3"/>
+    </row>
+    <row r="20" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C20" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="D20" s="3">
+        <v>56.314825462012308</v>
+      </c>
+      <c r="E20" s="3">
+        <v>154.2882786885246</v>
+      </c>
+      <c r="H20" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="I20" s="3">
+        <v>56.314825462012308</v>
+      </c>
+      <c r="J20" s="3">
+        <v>154.2882786885246</v>
+      </c>
+      <c r="R20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="S20" s="3">
+        <v>4.7709929825351417E-2</v>
+      </c>
+      <c r="T20" s="3"/>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="D21" s="3">
+        <v>55.70534907597537</v>
+      </c>
+      <c r="E21" s="3">
+        <v>145.32852459016399</v>
+      </c>
+      <c r="H21" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="I21" s="3">
+        <v>55.70534907597537</v>
+      </c>
+      <c r="J21" s="3">
+        <v>145.32852459016399</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C22" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="D22" s="3">
+        <v>55.223798767967139</v>
+      </c>
+      <c r="E22" s="3">
+        <v>159.75368852459019</v>
+      </c>
+      <c r="H22" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="I22" s="3">
+        <v>55.223798767967139</v>
+      </c>
+      <c r="J22" s="3">
+        <v>159.75368852459019</v>
+      </c>
+      <c r="R22" s="6"/>
+    </row>
+    <row r="23" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C23" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="D23" s="3">
+        <v>56.688490759753613</v>
+      </c>
+      <c r="E23" s="3">
+        <v>148.3181557377049</v>
+      </c>
+      <c r="H23" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="I23" s="3">
+        <v>56.688490759753613</v>
+      </c>
+      <c r="J23" s="3">
+        <v>148.3181557377049</v>
+      </c>
+      <c r="R23" s="8"/>
+    </row>
+    <row r="24" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C24" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="D24" s="3">
+        <v>57.348377823408619</v>
+      </c>
+      <c r="E24" s="3">
+        <v>144.3418442622951</v>
+      </c>
+      <c r="H24" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="I24" s="3">
+        <v>57.348377823408619</v>
+      </c>
+      <c r="J24" s="3">
+        <v>144.3418442622951</v>
+      </c>
+    </row>
+    <row r="25" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C25" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="D25" s="3">
+        <v>56.506468172484603</v>
+      </c>
+      <c r="E25" s="3">
+        <v>146.62643442622951</v>
+      </c>
+      <c r="H25" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="I25" s="3">
+        <v>56.506468172484603</v>
+      </c>
+      <c r="J25" s="3">
+        <v>146.62643442622951</v>
+      </c>
+    </row>
+    <row r="26" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C26" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="D26" s="3">
+        <v>55.195338809034922</v>
+      </c>
+      <c r="E26" s="3">
+        <v>144.581762295082</v>
+      </c>
+      <c r="H26" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="I26" s="3">
+        <v>55.195338809034922</v>
+      </c>
+      <c r="J26" s="3">
+        <v>144.581762295082</v>
+      </c>
+    </row>
+    <row r="27" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C27" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="D27" s="3">
+        <v>54.922843942505132</v>
+      </c>
+      <c r="E27" s="3">
+        <v>160.34065573770491</v>
+      </c>
+      <c r="H27" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="I27" s="3">
+        <v>54.922843942505132</v>
+      </c>
+      <c r="J27" s="3">
+        <v>160.34065573770491</v>
+      </c>
+    </row>
+    <row r="28" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C28" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="D28" s="3">
+        <v>53.736314168377831</v>
+      </c>
+      <c r="E28" s="3">
+        <v>171.64590163934429</v>
+      </c>
+      <c r="H28" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="I28" s="3">
+        <v>53.736314168377831</v>
+      </c>
+      <c r="J28" s="3">
+        <v>171.64590163934429</v>
+      </c>
+    </row>
+    <row r="29" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C29" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="D29" s="3">
+        <v>55.846683778234087</v>
+      </c>
+      <c r="E29" s="3">
+        <v>155.17307377049181</v>
+      </c>
+      <c r="H29" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="I29" s="3">
+        <v>55.846683778234087</v>
+      </c>
+      <c r="J29" s="3">
+        <v>155.17307377049181</v>
+      </c>
+    </row>
+    <row r="30" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C30" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="D30" s="3">
+        <v>56.90160164271046</v>
+      </c>
+      <c r="E30" s="3">
+        <v>154.92442622950821</v>
+      </c>
+      <c r="H30" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="I30" s="3">
+        <v>56.90160164271046</v>
+      </c>
+      <c r="J30" s="3">
+        <v>154.92442622950821</v>
+      </c>
+    </row>
+    <row r="31" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C31" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>57.720297741273093</v>
+      </c>
+      <c r="E31" s="3">
+        <v>131.96454918032791</v>
+      </c>
+      <c r="H31" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="I31" s="3">
+        <v>57.720297741273093</v>
+      </c>
+      <c r="J31" s="3">
+        <v>131.96454918032791</v>
+      </c>
+    </row>
+    <row r="32" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C32" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="D32" s="3">
+        <v>54.252772073921967</v>
+      </c>
+      <c r="E32" s="3">
+        <v>164.648155737705</v>
+      </c>
+      <c r="H32" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="I32" s="3">
+        <v>54.252772073921967</v>
+      </c>
+      <c r="J32" s="3">
+        <v>164.648155737705</v>
+      </c>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C33" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="D33" s="3">
+        <v>56.885503080082131</v>
+      </c>
+      <c r="E33" s="3">
+        <v>159.35274590163939</v>
+      </c>
+      <c r="H33" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="I33" s="3">
+        <v>56.885503080082131</v>
+      </c>
+      <c r="J33" s="3">
+        <v>159.35274590163939</v>
+      </c>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C34" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="D34" s="3">
+        <v>55.655472279260778</v>
+      </c>
+      <c r="E34" s="3">
+        <v>152.5567213114754</v>
+      </c>
+      <c r="H34" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I34" s="3">
+        <v>55.655472279260778</v>
+      </c>
+      <c r="J34" s="3">
+        <v>152.5567213114754</v>
+      </c>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C35" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="D35" s="3">
+        <v>53.900913757700224</v>
+      </c>
+      <c r="E35" s="3">
+        <v>160.3526639344262</v>
+      </c>
+      <c r="H35" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="I35" s="3">
+        <v>53.900913757700224</v>
+      </c>
+      <c r="J35" s="3">
+        <v>160.3526639344262</v>
+      </c>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C36" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="D36" s="3">
+        <v>55.648809034907607</v>
+      </c>
+      <c r="E36" s="3">
+        <v>151.47782786885239</v>
+      </c>
+      <c r="H36" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="I36" s="3">
+        <v>55.648809034907607</v>
+      </c>
+      <c r="J36" s="3">
+        <v>151.47782786885239</v>
+      </c>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C37" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="D37" s="3">
+        <v>55.96349075975359</v>
+      </c>
+      <c r="E37" s="3">
+        <v>148.7710245901639</v>
+      </c>
+      <c r="H37" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="I37" s="3">
+        <v>55.96349075975359</v>
+      </c>
+      <c r="J37" s="3">
+        <v>148.7710245901639</v>
+      </c>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C38" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="D38" s="3">
+        <v>53.455236139630379</v>
+      </c>
+      <c r="E38" s="3">
+        <v>159.43995901639349</v>
+      </c>
+      <c r="H38" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="I38" s="3">
+        <v>53.455236139630379</v>
+      </c>
+      <c r="J38" s="3">
+        <v>159.43995901639349</v>
+      </c>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C39" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="D39" s="3">
+        <v>55.007207392197131</v>
+      </c>
+      <c r="E39" s="3">
+        <v>164.4861885245902</v>
+      </c>
+      <c r="H39" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="I39" s="3">
+        <v>55.007207392197131</v>
+      </c>
+      <c r="J39" s="3">
+        <v>164.4861885245902</v>
+      </c>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C40" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="D40" s="3">
+        <v>55.486478439425049</v>
+      </c>
+      <c r="E40" s="3">
+        <v>158.6072540983607</v>
+      </c>
+      <c r="H40" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="I40" s="3">
+        <v>55.486478439425049</v>
+      </c>
+      <c r="J40" s="3">
+        <v>158.6072540983607</v>
+      </c>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C41" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="D41" s="3">
+        <v>55.499178644763859</v>
+      </c>
+      <c r="E41" s="3">
+        <v>156.53709016393441</v>
+      </c>
+      <c r="H41" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="I41" s="3">
+        <v>55.499178644763859</v>
+      </c>
+      <c r="J41" s="3">
+        <v>156.53709016393441</v>
+      </c>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C42" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="D42" s="3">
+        <v>55.933121149897339</v>
+      </c>
+      <c r="E42" s="3">
+        <v>145.6338524590164</v>
+      </c>
+      <c r="H42" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="I42" s="3">
+        <v>55.933121149897339</v>
+      </c>
+      <c r="J42" s="3">
+        <v>145.6338524590164</v>
+      </c>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C43" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="D43" s="3">
+        <v>55.354999999999997</v>
+      </c>
+      <c r="E43" s="3">
+        <v>163.1984836065574</v>
+      </c>
+      <c r="H43" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="I43" s="3">
+        <v>55.354999999999997</v>
+      </c>
+      <c r="J43" s="3">
+        <v>163.1984836065574</v>
+      </c>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C44" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="D44" s="3">
+        <v>58.014702258726899</v>
+      </c>
+      <c r="E44" s="3">
+        <v>135.29864754098361</v>
+      </c>
+      <c r="H44" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="I44" s="3">
+        <v>58.014702258726899</v>
+      </c>
+      <c r="J44" s="3">
+        <v>135.29864754098361</v>
+      </c>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C45" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="D45" s="3">
+        <v>57.835903490759762</v>
+      </c>
+      <c r="E45" s="3">
+        <v>139.25954918032781</v>
+      </c>
+      <c r="H45" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="I45" s="3">
+        <v>57.835903490759762</v>
+      </c>
+      <c r="J45" s="3">
+        <v>139.25954918032781</v>
+      </c>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C46" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="D46" s="3">
+        <v>53.766950718685841</v>
+      </c>
+      <c r="E46" s="3">
+        <v>175.01897540983609</v>
+      </c>
+      <c r="H46" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="I46" s="3">
+        <v>53.766950718685841</v>
+      </c>
+      <c r="J46" s="3">
+        <v>175.01897540983609</v>
+      </c>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C47" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="D47" s="3">
+        <v>55.056180698151962</v>
+      </c>
+      <c r="E47" s="3">
+        <v>151.0440573770492</v>
+      </c>
+      <c r="H47" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="I47" s="3">
+        <v>55.056180698151962</v>
+      </c>
+      <c r="J47" s="3">
+        <v>151.0440573770492</v>
+      </c>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C48" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="D48" s="3">
+        <v>56.164537987679687</v>
+      </c>
+      <c r="E48" s="3">
+        <v>145.84540983606561</v>
+      </c>
+      <c r="H48" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="I48" s="3">
+        <v>56.164537987679687</v>
+      </c>
+      <c r="J48" s="3">
+        <v>145.84540983606561</v>
+      </c>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C49" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="D49" s="3">
+        <v>57.091468172484603</v>
+      </c>
+      <c r="E49" s="3">
+        <v>135.55102459016391</v>
+      </c>
+      <c r="H49" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="I49" s="3">
+        <v>57.091468172484603</v>
+      </c>
+      <c r="J49" s="3">
+        <v>135.55102459016391</v>
+      </c>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C50" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="D50" s="3">
+        <v>56.354876796714571</v>
+      </c>
+      <c r="E50" s="3">
+        <v>160.80495901639341</v>
+      </c>
+      <c r="H50" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="I50" s="3">
+        <v>56.354876796714571</v>
+      </c>
+      <c r="J50" s="3">
+        <v>160.80495901639341</v>
+      </c>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C51" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="D51" s="3">
+        <v>53.998850102669422</v>
+      </c>
+      <c r="E51" s="3">
+        <v>160.4527868852459</v>
+      </c>
+      <c r="H51" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="I51" s="3">
+        <v>53.998850102669422</v>
+      </c>
+      <c r="J51" s="3">
+        <v>160.4527868852459</v>
+      </c>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C52" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="D52" s="3">
+        <v>55.114948665297753</v>
+      </c>
+      <c r="E52" s="3">
+        <v>152.68799180327869</v>
+      </c>
+      <c r="H52" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="I52" s="3">
+        <v>55.114948665297753</v>
+      </c>
+      <c r="J52" s="3">
+        <v>152.68799180327869</v>
+      </c>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C53" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="D53" s="3">
+        <v>55.575585215605763</v>
+      </c>
+      <c r="E53" s="3">
+        <v>162.6149180327869</v>
+      </c>
+      <c r="H53" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="I53" s="3">
+        <v>55.575585215605763</v>
+      </c>
+      <c r="J53" s="3">
+        <v>162.6149180327869</v>
+      </c>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C54" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="D54" s="3">
+        <v>54.782505133470238</v>
+      </c>
+      <c r="E54" s="3">
+        <v>169.36680327868851</v>
+      </c>
+      <c r="H54" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="I54" s="3">
+        <v>54.782505133470238</v>
+      </c>
+      <c r="J54" s="3">
+        <v>169.36680327868851</v>
+      </c>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C55" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="D55" s="3">
+        <v>57.475030800821379</v>
+      </c>
+      <c r="E55" s="3">
+        <v>128.9006147540984</v>
+      </c>
+      <c r="H55" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I55" s="3">
+        <v>57.475030800821379</v>
+      </c>
+      <c r="J55" s="3">
+        <v>128.9006147540984</v>
+      </c>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D57" s="3">
+        <f>AVERAGE(D6:D55)</f>
+        <v>55.762803490759751</v>
+      </c>
+      <c r="E57" s="3">
+        <f>AVERAGE(E6:E55)</f>
+        <v>153.20420819672134</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I57" s="3">
+        <f>AVERAGE(I6:I55)</f>
+        <v>55.762803490759751</v>
+      </c>
+      <c r="J57" s="3">
+        <f>AVERAGE(J6:J55)</f>
+        <v>153.20420819672134</v>
+      </c>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D58" s="3">
+        <f>_xlfn.STDEV.S(D6:D55)</f>
+        <v>1.1892357812622139</v>
+      </c>
+      <c r="E58" s="3">
+        <f>_xlfn.STDEV.S(E6:E55)</f>
+        <v>11.009852940109267</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I58" s="3">
+        <f>_xlfn.STDEV.S(I6:I55)</f>
+        <v>1.1892357812622139</v>
+      </c>
+      <c r="J58" s="3">
+        <f>_xlfn.STDEV.S(J6:J55)</f>
+        <v>11.009852940109267</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:E57"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3421,11 +4748,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
superdataset-24 negative flow test
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -11,6 +11,53 @@
     <sheet name="mae" sheetId="1" r:id="rId2"/>
     <sheet name="mse" sheetId="2" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">'pos vs neg'!$S$5</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">'pos vs neg'!$T$5</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -153,12 +200,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -173,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -193,6 +246,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -211,6 +273,520 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="ru-RU"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pos vs neg'!$S$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>positive flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent1"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent1"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pos vs neg'!$R$6:$R$20</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pos vs neg'!$S$6:$S$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.25852249577887998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.9128855552448121E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.4655059358944323E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.4533933905929091E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.1912290768252677E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.1876215419234312E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15274357333507019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.0969016499390998E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.771698471518789E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.839653741383061E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>4.2972143084908702E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.8865933722695101E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.8654657279261069E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>3.1342373340615473E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.7709929825351417E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-487F-4CE1-9032-2C723789062B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'pos vs neg'!$T$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>negative flow</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:pattFill prst="narHorz">
+              <a:fgClr>
+                <a:schemeClr val="accent2"/>
+              </a:fgClr>
+              <a:bgClr>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="20000"/>
+                  <a:lumOff val="80000"/>
+                </a:schemeClr>
+              </a:bgClr>
+            </a:pattFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:innerShdw blurRad="114300">
+                <a:schemeClr val="accent2"/>
+              </a:innerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'pos vs neg'!$R$6:$R$20</c:f>
+              <c:strCache>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>popsize</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>avgemployers</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>avgsalary</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>shoparea</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>foodseats</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>retailturnover</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>livarea</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>sportsvenue</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>servicesnum</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>roadslen</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>livestock</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>harvest</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>agrprod</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>hospitals</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>beforeschool</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'pos vs neg'!$T$6:$T$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>0.23728358919337381</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.5864048553715892E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9461133981485038E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4314090393932047E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0473514598308238E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.7618113073030561E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.8594960965908457E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2126834968642772E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.8406796292098262E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.0411832324806868E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.8504335319464841E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.2575489899654979E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.2782165333528653E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.7013107286034382E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.1045699878160153</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-487F-4CE1-9032-2C723789062B}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="164"/>
+        <c:overlap val="-22"/>
+        <c:axId val="1429664111"/>
+        <c:axId val="1429660367"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1429664111"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1100" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1429660367"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1429660367"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="95000"/>
+                    <a:lumOff val="5000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mj-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="ru-RU"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1429664111"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="t"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="95000"/>
+                  <a:lumOff val="5000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mj-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="ru-RU"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="ru-RU"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -532,6 +1108,46 @@
 </file>
 
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1090,7 +1706,561 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="203">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:pattFill prst="narHorz">
+        <a:fgClr>
+          <a:schemeClr val="phClr"/>
+        </a:fgClr>
+        <a:bgClr>
+          <a:schemeClr val="phClr">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:bgClr>
+      </a:pattFill>
+      <a:effectLst>
+        <a:innerShdw blurRad="114300">
+          <a:schemeClr val="phClr"/>
+        </a:innerShdw>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="50000"/>
+        <a:lumOff val="50000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1800" b="1" kern="1200" cap="all" spc="150" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600073</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>47626</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Диаграмма 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1390,8 +2560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
+      <selection activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1454,10 +2624,10 @@
         <v>1</v>
       </c>
       <c r="I6" s="3">
-        <v>55.788316221765918</v>
+        <v>27.436200396825399</v>
       </c>
       <c r="J6" s="3">
-        <v>153.6779098360656</v>
+        <v>74.471417244796811</v>
       </c>
       <c r="R6" s="6" t="s">
         <v>12</v>
@@ -1465,7 +2635,9 @@
       <c r="S6" s="3">
         <v>0.25852249577887998</v>
       </c>
-      <c r="T6" s="3"/>
+      <c r="T6" s="3">
+        <v>0.23728358919337381</v>
+      </c>
     </row>
     <row r="7" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
@@ -1483,18 +2655,20 @@
         <v>2</v>
       </c>
       <c r="I7" s="3">
-        <v>53.338449691991791</v>
+        <v>27.2718576388889</v>
       </c>
       <c r="J7" s="3">
-        <v>179.17241803278691</v>
-      </c>
-      <c r="R7" s="6" t="s">
+        <v>75.89561942517345</v>
+      </c>
+      <c r="R7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="S7" s="3">
+      <c r="S7" s="10">
         <v>2.9128855552448121E-2</v>
       </c>
-      <c r="T7" s="3"/>
+      <c r="T7" s="10">
+        <v>5.5864048553715892E-2</v>
+      </c>
     </row>
     <row r="8" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
@@ -1512,10 +2686,10 @@
         <v>3</v>
       </c>
       <c r="I8" s="3">
-        <v>54.543285420944549</v>
+        <v>27.179312996031751</v>
       </c>
       <c r="J8" s="3">
-        <v>148.6551639344263</v>
+        <v>76.855213082259667</v>
       </c>
       <c r="R8" s="6" t="s">
         <v>14</v>
@@ -1523,7 +2697,9 @@
       <c r="S8" s="3">
         <v>4.4655059358944323E-2</v>
       </c>
-      <c r="T8" s="3"/>
+      <c r="T8" s="3">
+        <v>5.9461133981485038E-2</v>
+      </c>
     </row>
     <row r="9" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
@@ -1541,10 +2717,10 @@
         <v>4</v>
       </c>
       <c r="I9" s="3">
-        <v>54.764691991786442</v>
+        <v>27.291279761904772</v>
       </c>
       <c r="J9" s="3">
-        <v>159.42118852459021</v>
+        <v>73.658176412289407</v>
       </c>
       <c r="R9" s="6" t="s">
         <v>15</v>
@@ -1552,7 +2728,9 @@
       <c r="S9" s="3">
         <v>3.4533933905929091E-2</v>
       </c>
-      <c r="T9" s="3"/>
+      <c r="T9" s="3">
+        <v>4.4314090393932047E-2</v>
+      </c>
     </row>
     <row r="10" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
@@ -1570,10 +2748,10 @@
         <v>5</v>
       </c>
       <c r="I10" s="3">
-        <v>57.240513347022578</v>
+        <v>27.58789930555556</v>
       </c>
       <c r="J10" s="3">
-        <v>140.6745901639344</v>
+        <v>70.873221010901887</v>
       </c>
       <c r="R10" s="6" t="s">
         <v>16</v>
@@ -1581,7 +2759,9 @@
       <c r="S10" s="3">
         <v>5.1912290768252677E-2</v>
       </c>
-      <c r="T10" s="3"/>
+      <c r="T10" s="3">
+        <v>4.0473514598308238E-2</v>
+      </c>
     </row>
     <row r="11" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
@@ -1599,10 +2779,10 @@
         <v>6</v>
       </c>
       <c r="I11" s="3">
-        <v>56.165903490759767</v>
+        <v>27.141101190476199</v>
       </c>
       <c r="J11" s="3">
-        <v>156.73520491803279</v>
+        <v>76.649801783944511</v>
       </c>
       <c r="R11" s="6" t="s">
         <v>17</v>
@@ -1610,7 +2790,9 @@
       <c r="S11" s="3">
         <v>6.1876215419234312E-2</v>
       </c>
-      <c r="T11" s="3"/>
+      <c r="T11" s="3">
+        <v>6.7618113073030561E-2</v>
+      </c>
     </row>
     <row r="12" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
@@ -1628,18 +2810,20 @@
         <v>7</v>
       </c>
       <c r="I12" s="3">
-        <v>55.818049281314167</v>
+        <v>27.327021329365081</v>
       </c>
       <c r="J12" s="3">
-        <v>155.67159836065579</v>
-      </c>
-      <c r="R12" s="6" t="s">
+        <v>73.891407333994039</v>
+      </c>
+      <c r="R12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="S12" s="3">
+      <c r="S12" s="10">
         <v>0.15274357333507019</v>
       </c>
-      <c r="T12" s="3"/>
+      <c r="T12" s="10">
+        <v>4.8594960965908457E-2</v>
+      </c>
     </row>
     <row r="13" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
@@ -1657,10 +2841,10 @@
         <v>8</v>
       </c>
       <c r="I13" s="3">
-        <v>56.226232032854213</v>
+        <v>27.1418253968254</v>
       </c>
       <c r="J13" s="3">
-        <v>154.82508196721309</v>
+        <v>74.903240832507436</v>
       </c>
       <c r="R13" s="6" t="s">
         <v>19</v>
@@ -1668,7 +2852,9 @@
       <c r="S13" s="3">
         <v>4.0969016499390998E-2</v>
       </c>
-      <c r="T13" s="3"/>
+      <c r="T13" s="3">
+        <v>4.2126834968642772E-2</v>
+      </c>
     </row>
     <row r="14" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
@@ -1686,10 +2872,10 @@
         <v>9</v>
       </c>
       <c r="I14" s="3">
-        <v>55.524517453798779</v>
+        <v>27.03370535714286</v>
       </c>
       <c r="J14" s="3">
-        <v>160.09938524590169</v>
+        <v>76.365678889990093</v>
       </c>
       <c r="R14" s="6" t="s">
         <v>20</v>
@@ -1697,7 +2883,9 @@
       <c r="S14" s="3">
         <v>3.771698471518789E-2</v>
       </c>
-      <c r="T14" s="3"/>
+      <c r="T14" s="3">
+        <v>3.8406796292098262E-2</v>
+      </c>
     </row>
     <row r="15" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
@@ -1715,10 +2903,10 @@
         <v>10</v>
       </c>
       <c r="I15" s="3">
-        <v>56.176724845995892</v>
+        <v>27.2882886904762</v>
       </c>
       <c r="J15" s="3">
-        <v>145.51348360655729</v>
+        <v>74.862596630327062</v>
       </c>
       <c r="R15" s="6" t="s">
         <v>21</v>
@@ -1726,7 +2914,9 @@
       <c r="S15" s="3">
         <v>3.839653741383061E-2</v>
       </c>
-      <c r="T15" s="3"/>
+      <c r="T15" s="3">
+        <v>6.0411832324806868E-2</v>
+      </c>
     </row>
     <row r="16" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
@@ -1744,10 +2934,10 @@
         <v>11</v>
       </c>
       <c r="I16" s="3">
-        <v>56.98952772073924</v>
+        <v>27.15534970238096</v>
       </c>
       <c r="J16" s="3">
-        <v>140.51717213114759</v>
+        <v>74.863191278493559</v>
       </c>
       <c r="R16" s="6" t="s">
         <v>22</v>
@@ -1755,7 +2945,9 @@
       <c r="S16" s="3">
         <v>4.2972143084908702E-2</v>
       </c>
-      <c r="T16" s="3"/>
+      <c r="T16" s="3">
+        <v>5.8504335319464841E-2</v>
+      </c>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
@@ -1773,18 +2965,20 @@
         <v>12</v>
       </c>
       <c r="I17" s="3">
-        <v>57.912607802874739</v>
+        <v>27.07872023809524</v>
       </c>
       <c r="J17" s="3">
-        <v>131.7270491803279</v>
-      </c>
-      <c r="R17" s="6" t="s">
+        <v>76.777730426164524</v>
+      </c>
+      <c r="R17" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="S17" s="3">
+      <c r="S17" s="10">
         <v>9.8865933722695101E-2</v>
       </c>
-      <c r="T17" s="3"/>
+      <c r="T17" s="10">
+        <v>5.2575489899654979E-2</v>
+      </c>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
@@ -1802,10 +2996,10 @@
         <v>13</v>
       </c>
       <c r="I18" s="3">
-        <v>55.247936344969212</v>
+        <v>27.695736607142859</v>
       </c>
       <c r="J18" s="3">
-        <v>151.11500000000001</v>
+        <v>72.855173439048556</v>
       </c>
       <c r="R18" s="6" t="s">
         <v>24</v>
@@ -1813,7 +3007,9 @@
       <c r="S18" s="3">
         <v>2.8654657279261069E-2</v>
       </c>
-      <c r="T18" s="3"/>
+      <c r="T18" s="3">
+        <v>4.2782165333528653E-2</v>
+      </c>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
@@ -1831,10 +3027,10 @@
         <v>14</v>
       </c>
       <c r="I19" s="3">
-        <v>56.018305954825458</v>
+        <v>27.61394841269842</v>
       </c>
       <c r="J19" s="3">
-        <v>163.21016393442619</v>
+        <v>73.418126858275528</v>
       </c>
       <c r="R19" s="6" t="s">
         <v>25</v>
@@ -1842,7 +3038,9 @@
       <c r="S19" s="3">
         <v>3.1342373340615473E-2</v>
       </c>
-      <c r="T19" s="3"/>
+      <c r="T19" s="3">
+        <v>4.7013107286034382E-2</v>
+      </c>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
@@ -1860,18 +3058,20 @@
         <v>15</v>
       </c>
       <c r="I20" s="3">
-        <v>56.314825462012308</v>
+        <v>27.594047619047629</v>
       </c>
       <c r="J20" s="3">
-        <v>154.2882786885246</v>
-      </c>
-      <c r="R20" s="7" t="s">
+        <v>73.463597621407331</v>
+      </c>
+      <c r="R20" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="S20" s="3">
+      <c r="S20" s="10">
         <v>4.7709929825351417E-2</v>
       </c>
-      <c r="T20" s="3"/>
+      <c r="T20" s="10">
+        <v>0.1045699878160153</v>
+      </c>
     </row>
     <row r="21" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -1889,10 +3089,10 @@
         <v>16</v>
       </c>
       <c r="I21" s="3">
-        <v>55.70534907597537</v>
+        <v>27.63276041666667</v>
       </c>
       <c r="J21" s="3">
-        <v>145.32852459016399</v>
+        <v>73.536848364717542</v>
       </c>
     </row>
     <row r="22" spans="3:20" x14ac:dyDescent="0.25">
@@ -1911,10 +3111,10 @@
         <v>17</v>
       </c>
       <c r="I22" s="3">
-        <v>55.223798767967139</v>
+        <v>27.395121527777789</v>
       </c>
       <c r="J22" s="3">
-        <v>159.75368852459019</v>
+        <v>76.376511397423201</v>
       </c>
       <c r="R22" s="6"/>
     </row>
@@ -1934,10 +3134,10 @@
         <v>18</v>
       </c>
       <c r="I23" s="3">
-        <v>56.688490759753613</v>
+        <v>27.309097222222231</v>
       </c>
       <c r="J23" s="3">
-        <v>148.3181557377049</v>
+        <v>78.468880079286421</v>
       </c>
       <c r="R23" s="8"/>
     </row>
@@ -1957,10 +3157,10 @@
         <v>19</v>
       </c>
       <c r="I24" s="3">
-        <v>57.348377823408619</v>
+        <v>27.114685019841271</v>
       </c>
       <c r="J24" s="3">
-        <v>144.3418442622951</v>
+        <v>75.140495540138758</v>
       </c>
     </row>
     <row r="25" spans="3:20" x14ac:dyDescent="0.25">
@@ -1979,10 +3179,10 @@
         <v>20</v>
       </c>
       <c r="I25" s="3">
-        <v>56.506468172484603</v>
+        <v>27.4622197420635</v>
       </c>
       <c r="J25" s="3">
-        <v>146.62643442622951</v>
+        <v>74.922745292368688</v>
       </c>
     </row>
     <row r="26" spans="3:20" x14ac:dyDescent="0.25">
@@ -2001,10 +3201,10 @@
         <v>21</v>
       </c>
       <c r="I26" s="3">
-        <v>55.195338809034922</v>
+        <v>27.68507440476191</v>
       </c>
       <c r="J26" s="3">
-        <v>144.581762295082</v>
+        <v>72.981754212091175</v>
       </c>
     </row>
     <row r="27" spans="3:20" x14ac:dyDescent="0.25">
@@ -2023,10 +3223,10 @@
         <v>22</v>
       </c>
       <c r="I27" s="3">
-        <v>54.922843942505132</v>
+        <v>27.586810515873019</v>
       </c>
       <c r="J27" s="3">
-        <v>160.34065573770491</v>
+        <v>72.908949454905851</v>
       </c>
     </row>
     <row r="28" spans="3:20" x14ac:dyDescent="0.25">
@@ -2045,10 +3245,10 @@
         <v>23</v>
       </c>
       <c r="I28" s="3">
-        <v>53.736314168377831</v>
+        <v>27.37615823412699</v>
       </c>
       <c r="J28" s="3">
-        <v>171.64590163934429</v>
+        <v>74.654380574826561</v>
       </c>
     </row>
     <row r="29" spans="3:20" x14ac:dyDescent="0.25">
@@ -2067,10 +3267,10 @@
         <v>24</v>
       </c>
       <c r="I29" s="3">
-        <v>55.846683778234087</v>
+        <v>27.532425595238099</v>
       </c>
       <c r="J29" s="3">
-        <v>155.17307377049181</v>
+        <v>72.230396432111007</v>
       </c>
     </row>
     <row r="30" spans="3:20" x14ac:dyDescent="0.25">
@@ -2089,10 +3289,10 @@
         <v>25</v>
       </c>
       <c r="I30" s="3">
-        <v>56.90160164271046</v>
+        <v>27.546073908730161</v>
       </c>
       <c r="J30" s="3">
-        <v>154.92442622950821</v>
+        <v>72.579048562933593</v>
       </c>
     </row>
     <row r="31" spans="3:20" x14ac:dyDescent="0.25">
@@ -2111,10 +3311,10 @@
         <v>26</v>
       </c>
       <c r="I31" s="3">
-        <v>57.720297741273093</v>
+        <v>27.293943452380962</v>
       </c>
       <c r="J31" s="3">
-        <v>131.96454918032791</v>
+        <v>79.23398414271557</v>
       </c>
     </row>
     <row r="32" spans="3:20" x14ac:dyDescent="0.25">
@@ -2133,10 +3333,10 @@
         <v>27</v>
       </c>
       <c r="I32" s="3">
-        <v>54.252772073921967</v>
+        <v>27.61683283730159</v>
       </c>
       <c r="J32" s="3">
-        <v>164.648155737705</v>
+        <v>70.615044598612499</v>
       </c>
     </row>
     <row r="33" spans="3:10" x14ac:dyDescent="0.25">
@@ -2155,10 +3355,10 @@
         <v>28</v>
       </c>
       <c r="I33" s="3">
-        <v>56.885503080082131</v>
+        <v>27.203303571428581</v>
       </c>
       <c r="J33" s="3">
-        <v>159.35274590163939</v>
+        <v>77.619167492566902</v>
       </c>
     </row>
     <row r="34" spans="3:10" x14ac:dyDescent="0.25">
@@ -2177,10 +3377,10 @@
         <v>29</v>
       </c>
       <c r="I34" s="3">
-        <v>55.655472279260778</v>
+        <v>27.577571924603181</v>
       </c>
       <c r="J34" s="3">
-        <v>152.5567213114754</v>
+        <v>71.939038652130833</v>
       </c>
     </row>
     <row r="35" spans="3:10" x14ac:dyDescent="0.25">
@@ -2199,10 +3399,10 @@
         <v>30</v>
       </c>
       <c r="I35" s="3">
-        <v>53.900913757700224</v>
+        <v>27.296178075396831</v>
       </c>
       <c r="J35" s="3">
-        <v>160.3526639344262</v>
+        <v>75.326382556987141</v>
       </c>
     </row>
     <row r="36" spans="3:10" x14ac:dyDescent="0.25">
@@ -2221,10 +3421,10 @@
         <v>31</v>
       </c>
       <c r="I36" s="3">
-        <v>55.648809034907607</v>
+        <v>27.433335813492072</v>
       </c>
       <c r="J36" s="3">
-        <v>151.47782786885239</v>
+        <v>75.346105054509422</v>
       </c>
     </row>
     <row r="37" spans="3:10" x14ac:dyDescent="0.25">
@@ -2243,10 +3443,10 @@
         <v>32</v>
       </c>
       <c r="I37" s="3">
-        <v>55.96349075975359</v>
+        <v>27.221165674603181</v>
       </c>
       <c r="J37" s="3">
-        <v>148.7710245901639</v>
+        <v>75.932418235877122</v>
       </c>
     </row>
     <row r="38" spans="3:10" x14ac:dyDescent="0.25">
@@ -2265,10 +3465,10 @@
         <v>33</v>
       </c>
       <c r="I38" s="3">
-        <v>53.455236139630379</v>
+        <v>27.420198412698429</v>
       </c>
       <c r="J38" s="3">
-        <v>159.43995901639349</v>
+        <v>75.917205153617445</v>
       </c>
     </row>
     <row r="39" spans="3:10" x14ac:dyDescent="0.25">
@@ -2287,10 +3487,10 @@
         <v>34</v>
       </c>
       <c r="I39" s="3">
-        <v>55.007207392197131</v>
+        <v>27.590071924603169</v>
       </c>
       <c r="J39" s="3">
-        <v>164.4861885245902</v>
+        <v>72.912447968285434</v>
       </c>
     </row>
     <row r="40" spans="3:10" x14ac:dyDescent="0.25">
@@ -2309,10 +3509,10 @@
         <v>35</v>
       </c>
       <c r="I40" s="3">
-        <v>55.486478439425049</v>
+        <v>27.547710813492071</v>
       </c>
       <c r="J40" s="3">
-        <v>158.6072540983607</v>
+        <v>72.331655104063429</v>
       </c>
     </row>
     <row r="41" spans="3:10" x14ac:dyDescent="0.25">
@@ -2331,10 +3531,10 @@
         <v>36</v>
       </c>
       <c r="I41" s="3">
-        <v>55.499178644763859</v>
+        <v>28.041842757936521</v>
       </c>
       <c r="J41" s="3">
-        <v>156.53709016393441</v>
+        <v>69.965520317145689</v>
       </c>
     </row>
     <row r="42" spans="3:10" x14ac:dyDescent="0.25">
@@ -2353,10 +3553,10 @@
         <v>37</v>
       </c>
       <c r="I42" s="3">
-        <v>55.933121149897339</v>
+        <v>27.521778273809531</v>
       </c>
       <c r="J42" s="3">
-        <v>145.6338524590164</v>
+        <v>73.415559960356788</v>
       </c>
     </row>
     <row r="43" spans="3:10" x14ac:dyDescent="0.25">
@@ -2375,10 +3575,10 @@
         <v>38</v>
       </c>
       <c r="I43" s="3">
-        <v>55.354999999999997</v>
+        <v>27.46375744047619</v>
       </c>
       <c r="J43" s="3">
-        <v>163.1984836065574</v>
+        <v>73.793894945490592</v>
       </c>
     </row>
     <row r="44" spans="3:10" x14ac:dyDescent="0.25">
@@ -2397,10 +3597,10 @@
         <v>39</v>
       </c>
       <c r="I44" s="3">
-        <v>58.014702258726899</v>
+        <v>27.55360863095239</v>
       </c>
       <c r="J44" s="3">
-        <v>135.29864754098361</v>
+        <v>72.311060455896921</v>
       </c>
     </row>
     <row r="45" spans="3:10" x14ac:dyDescent="0.25">
@@ -2419,10 +3619,10 @@
         <v>40</v>
       </c>
       <c r="I45" s="3">
-        <v>57.835903490759762</v>
+        <v>27.165111607142869</v>
       </c>
       <c r="J45" s="3">
-        <v>139.25954918032781</v>
+        <v>73.68607532210109</v>
       </c>
     </row>
     <row r="46" spans="3:10" x14ac:dyDescent="0.25">
@@ -2441,10 +3641,10 @@
         <v>41</v>
       </c>
       <c r="I46" s="3">
-        <v>53.766950718685841</v>
+        <v>27.161230158730159</v>
       </c>
       <c r="J46" s="3">
-        <v>175.01897540983609</v>
+        <v>77.852616451932604</v>
       </c>
     </row>
     <row r="47" spans="3:10" x14ac:dyDescent="0.25">
@@ -2463,10 +3663,10 @@
         <v>42</v>
       </c>
       <c r="I47" s="3">
-        <v>55.056180698151962</v>
+        <v>27.0398759920635</v>
       </c>
       <c r="J47" s="3">
-        <v>151.0440573770492</v>
+        <v>75.420624380574822</v>
       </c>
     </row>
     <row r="48" spans="3:10" x14ac:dyDescent="0.25">
@@ -2485,10 +3685,10 @@
         <v>43</v>
       </c>
       <c r="I48" s="3">
-        <v>56.164537987679687</v>
+        <v>27.465243055555561</v>
       </c>
       <c r="J48" s="3">
-        <v>145.84540983606561</v>
+        <v>73.300426164519322</v>
       </c>
     </row>
     <row r="49" spans="3:10" x14ac:dyDescent="0.25">
@@ -2507,10 +3707,10 @@
         <v>44</v>
       </c>
       <c r="I49" s="3">
-        <v>57.091468172484603</v>
+        <v>27.339786706349209</v>
       </c>
       <c r="J49" s="3">
-        <v>135.55102459016391</v>
+        <v>76.893181367690786</v>
       </c>
     </row>
     <row r="50" spans="3:10" x14ac:dyDescent="0.25">
@@ -2529,10 +3729,10 @@
         <v>45</v>
       </c>
       <c r="I50" s="3">
-        <v>56.354876796714571</v>
+        <v>27.806413690476202</v>
       </c>
       <c r="J50" s="3">
-        <v>160.80495901639341</v>
+        <v>70.35185332011892</v>
       </c>
     </row>
     <row r="51" spans="3:10" x14ac:dyDescent="0.25">
@@ -2551,10 +3751,10 @@
         <v>46</v>
       </c>
       <c r="I51" s="3">
-        <v>53.998850102669422</v>
+        <v>27.672224702380959</v>
       </c>
       <c r="J51" s="3">
-        <v>160.4527868852459</v>
+        <v>73.273201189296344</v>
       </c>
     </row>
     <row r="52" spans="3:10" x14ac:dyDescent="0.25">
@@ -2573,10 +3773,10 @@
         <v>47</v>
       </c>
       <c r="I52" s="3">
-        <v>55.114948665297753</v>
+        <v>27.12560267857144</v>
       </c>
       <c r="J52" s="3">
-        <v>152.68799180327869</v>
+        <v>79.661655104063442</v>
       </c>
     </row>
     <row r="53" spans="3:10" x14ac:dyDescent="0.25">
@@ -2595,10 +3795,10 @@
         <v>48</v>
       </c>
       <c r="I53" s="3">
-        <v>55.575585215605763</v>
+        <v>27.450977182539681</v>
       </c>
       <c r="J53" s="3">
-        <v>162.6149180327869</v>
+        <v>75.433002973240846</v>
       </c>
     </row>
     <row r="54" spans="3:10" x14ac:dyDescent="0.25">
@@ -2617,10 +3817,10 @@
         <v>49</v>
       </c>
       <c r="I54" s="3">
-        <v>54.782505133470238</v>
+        <v>27.55211805555556</v>
       </c>
       <c r="J54" s="3">
-        <v>169.36680327868851</v>
+        <v>72.68617443012883</v>
       </c>
     </row>
     <row r="55" spans="3:10" x14ac:dyDescent="0.25">
@@ -2639,10 +3839,10 @@
         <v>50</v>
       </c>
       <c r="I55" s="3">
-        <v>57.475030800821379</v>
+        <v>27.45905753968254</v>
       </c>
       <c r="J55" s="3">
-        <v>128.9006147540984</v>
+        <v>73.422041625371648</v>
       </c>
     </row>
     <row r="57" spans="3:10" x14ac:dyDescent="0.25">
@@ -2662,11 +3862,11 @@
       </c>
       <c r="I57" s="3">
         <f>AVERAGE(I6:I55)</f>
-        <v>55.762803490759751</v>
+        <v>27.409913244047626</v>
       </c>
       <c r="J57" s="3">
         <f>AVERAGE(J6:J55)</f>
-        <v>153.20420819672134</v>
+        <v>74.444890782953422</v>
       </c>
     </row>
     <row r="58" spans="3:10" x14ac:dyDescent="0.25">
@@ -2686,16 +3886,17 @@
       </c>
       <c r="I58" s="3">
         <f>_xlfn.STDEV.S(I6:I55)</f>
-        <v>1.1892357812622139</v>
+        <v>0.21713983736784781</v>
       </c>
       <c r="J58" s="3">
         <f>_xlfn.STDEV.S(J6:J55)</f>
-        <v>11.009852940109267</v>
+        <v>2.2077219445700469</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
test 13 on new version of 24 negative superdataset
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -4,60 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pos vs neg" sheetId="3" r:id="rId1"/>
-    <sheet name="mae" sheetId="1" r:id="rId2"/>
-    <sheet name="mse" sheetId="2" r:id="rId3"/>
+    <sheet name="Лист1" sheetId="4" r:id="rId2"/>
+    <sheet name="mae" sheetId="1" r:id="rId3"/>
+    <sheet name="mse" sheetId="2" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">'pos vs neg'!$R$6:$R$20</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">'pos vs neg'!$S$5</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">'pos vs neg'!$S$6:$S$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">'pos vs neg'!$T$5</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">'pos vs neg'!$T$6:$T$20</definedName>
-  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -68,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="33">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -161,6 +115,12 @@
   </si>
   <si>
     <t>Random Forest-100 (superdataset-24 (negative flow).csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24-2 (positive flow).csv)</t>
+  </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24-2 (negative flow).csv)</t>
   </si>
 </sst>
 </file>
@@ -2560,8 +2520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C4:T58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C10" workbookViewId="0">
-      <selection activeCell="W30" sqref="W30"/>
+    <sheetView topLeftCell="A19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K55" sqref="K55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3901,6 +3861,1318 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:S56"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.85546875" customWidth="1"/>
+    <col min="18" max="18" width="15.85546875" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="1"/>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3">
+        <v>55.788316221765918</v>
+      </c>
+      <c r="D4" s="3">
+        <v>153.6779098360656</v>
+      </c>
+      <c r="G4" s="2">
+        <v>1</v>
+      </c>
+      <c r="H4" s="3">
+        <v>28.72156417398757</v>
+      </c>
+      <c r="I4" s="3">
+        <v>74.245921165381318</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3">
+        <v>0.21160587297740199</v>
+      </c>
+    </row>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <f>B4+1</f>
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>53.338449691991791</v>
+      </c>
+      <c r="D5" s="3">
+        <v>179.17241803278691</v>
+      </c>
+      <c r="G5" s="2">
+        <f>G4+1</f>
+        <v>2</v>
+      </c>
+      <c r="H5" s="3">
+        <v>28.311814870366401</v>
+      </c>
+      <c r="I5" s="3">
+        <v>76.821636675235652</v>
+      </c>
+      <c r="Q5" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10">
+        <v>5.8974021768202517E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:B53" si="0">B5+1</f>
+        <v>3</v>
+      </c>
+      <c r="C6" s="3">
+        <v>54.543285420944549</v>
+      </c>
+      <c r="D6" s="3">
+        <v>148.6551639344263</v>
+      </c>
+      <c r="G6" s="2">
+        <f t="shared" ref="G6:G53" si="1">G5+1</f>
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>28.834557531604879</v>
+      </c>
+      <c r="I6" s="3">
+        <v>76.951619537275079</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3">
+        <v>6.4580675206569071E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C7" s="3">
+        <v>54.764691991786442</v>
+      </c>
+      <c r="D7" s="3">
+        <v>159.42118852459021</v>
+      </c>
+      <c r="G7" s="2">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H7" s="3">
+        <v>28.457422326976641</v>
+      </c>
+      <c r="I7" s="3">
+        <v>75.231199657240793</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3">
+        <v>4.2514693155637433E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C8" s="3">
+        <v>57.240513347022578</v>
+      </c>
+      <c r="D8" s="3">
+        <v>140.6745901639344</v>
+      </c>
+      <c r="G8" s="2">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="H8" s="3">
+        <v>28.74610027855153</v>
+      </c>
+      <c r="I8" s="3">
+        <v>74.391876606683823</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3">
+        <v>4.3130944637673183E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C9" s="3">
+        <v>56.165903490759767</v>
+      </c>
+      <c r="D9" s="3">
+        <v>156.73520491803279</v>
+      </c>
+      <c r="G9" s="2">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H9" s="3">
+        <v>28.16415041782729</v>
+      </c>
+      <c r="I9" s="3">
+        <v>78.039700085689816</v>
+      </c>
+      <c r="Q9" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3">
+        <v>6.3206726900651239E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>55.818049281314167</v>
+      </c>
+      <c r="D10" s="3">
+        <v>155.67159836065579</v>
+      </c>
+      <c r="G10" s="2">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="H10" s="3">
+        <v>28.275731733447611</v>
+      </c>
+      <c r="I10" s="3">
+        <v>77.76393316195373</v>
+      </c>
+      <c r="Q10" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="R10" s="10"/>
+      <c r="S10" s="10">
+        <v>5.1093829662679911E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C11" s="3">
+        <v>56.226232032854213</v>
+      </c>
+      <c r="D11" s="3">
+        <v>154.82508196721309</v>
+      </c>
+      <c r="G11" s="2">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="H11" s="3">
+        <v>27.91671952003427</v>
+      </c>
+      <c r="I11" s="3">
+        <v>81.519725792630666</v>
+      </c>
+      <c r="Q11" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3">
+        <v>4.472767472121357E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C12" s="3">
+        <v>55.524517453798779</v>
+      </c>
+      <c r="D12" s="3">
+        <v>160.09938524590169</v>
+      </c>
+      <c r="G12" s="2">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="H12" s="3">
+        <v>28.095348189415041</v>
+      </c>
+      <c r="I12" s="3">
+        <v>79.009965724078839</v>
+      </c>
+      <c r="Q12" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="R12" s="3"/>
+      <c r="S12" s="3">
+        <v>3.7525436140557138E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C13" s="3">
+        <v>56.176724845995892</v>
+      </c>
+      <c r="D13" s="3">
+        <v>145.51348360655729</v>
+      </c>
+      <c r="G13" s="2">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="H13" s="3">
+        <v>28.646074566102421</v>
+      </c>
+      <c r="I13" s="3">
+        <v>73.64679520137102</v>
+      </c>
+      <c r="Q13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="R13" s="3"/>
+      <c r="S13" s="3">
+        <v>5.624668466067631E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C14" s="3">
+        <v>56.98952772073924</v>
+      </c>
+      <c r="D14" s="3">
+        <v>140.51717213114759</v>
+      </c>
+      <c r="G14" s="2">
+        <f t="shared" si="1"/>
+        <v>11</v>
+      </c>
+      <c r="H14" s="3">
+        <v>28.714216841654171</v>
+      </c>
+      <c r="I14" s="3">
+        <v>72.082733504712948</v>
+      </c>
+      <c r="Q14" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3">
+        <v>5.7359101157341198E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C15" s="3">
+        <v>57.912607802874739</v>
+      </c>
+      <c r="D15" s="3">
+        <v>131.7270491803279</v>
+      </c>
+      <c r="G15" s="2">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="H15" s="3">
+        <v>28.447426612384831</v>
+      </c>
+      <c r="I15" s="3">
+        <v>76.143059125964015</v>
+      </c>
+      <c r="Q15" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="R15" s="10"/>
+      <c r="S15" s="10">
+        <v>5.027624395645338E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C16" s="3">
+        <v>55.247936344969212</v>
+      </c>
+      <c r="D16" s="3">
+        <v>151.11500000000001</v>
+      </c>
+      <c r="G16" s="2">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="H16" s="3">
+        <v>28.341446325262471</v>
+      </c>
+      <c r="I16" s="3">
+        <v>78.16999143101971</v>
+      </c>
+      <c r="Q16" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="R16" s="3"/>
+      <c r="S16" s="3">
+        <v>4.4020107049946168E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C17" s="3">
+        <v>56.018305954825458</v>
+      </c>
+      <c r="D17" s="3">
+        <v>163.21016393442619</v>
+      </c>
+      <c r="G17" s="2">
+        <f t="shared" si="1"/>
+        <v>14</v>
+      </c>
+      <c r="H17" s="3">
+        <v>27.888133704735381</v>
+      </c>
+      <c r="I17" s="3">
+        <v>80.585715509854325</v>
+      </c>
+      <c r="Q17" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R17" s="3"/>
+      <c r="S17" s="3">
+        <v>4.6357086128139907E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <v>56.314825462012308</v>
+      </c>
+      <c r="D18" s="3">
+        <v>154.2882786885246</v>
+      </c>
+      <c r="G18" s="2">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="H18" s="3">
+        <v>28.201658452967639</v>
+      </c>
+      <c r="I18" s="3">
+        <v>77.04346186803771</v>
+      </c>
+      <c r="Q18" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="R18" s="10"/>
+      <c r="S18" s="10">
+        <v>0.128380901876857</v>
+      </c>
+    </row>
+    <row r="19" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C19" s="3">
+        <v>55.70534907597537</v>
+      </c>
+      <c r="D19" s="3">
+        <v>145.32852459016399</v>
+      </c>
+      <c r="G19" s="2">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="H19" s="3">
+        <v>28.30121491322048</v>
+      </c>
+      <c r="I19" s="3">
+        <v>75.047403598971727</v>
+      </c>
+    </row>
+    <row r="20" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C20" s="3">
+        <v>55.223798767967139</v>
+      </c>
+      <c r="D20" s="3">
+        <v>159.75368852459019</v>
+      </c>
+      <c r="G20" s="2">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="H20" s="3">
+        <v>28.557610884936789</v>
+      </c>
+      <c r="I20" s="3">
+        <v>75.241388174807199</v>
+      </c>
+      <c r="Q20" s="6"/>
+    </row>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <v>56.688490759753613</v>
+      </c>
+      <c r="D21" s="3">
+        <v>148.3181557377049</v>
+      </c>
+      <c r="G21" s="2">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="H21" s="3">
+        <v>28.20127490893508</v>
+      </c>
+      <c r="I21" s="3">
+        <v>76.981276778063418</v>
+      </c>
+      <c r="Q21" s="8"/>
+    </row>
+    <row r="22" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C22" s="3">
+        <v>57.348377823408619</v>
+      </c>
+      <c r="D22" s="3">
+        <v>144.3418442622951</v>
+      </c>
+      <c r="G22" s="2">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="H22" s="3">
+        <v>28.346968073709011</v>
+      </c>
+      <c r="I22" s="3">
+        <v>75.001131105398471</v>
+      </c>
+    </row>
+    <row r="23" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C23" s="3">
+        <v>56.506468172484603</v>
+      </c>
+      <c r="D23" s="3">
+        <v>146.62643442622951</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="H23" s="3">
+        <v>28.039136490250691</v>
+      </c>
+      <c r="I23" s="3">
+        <v>78.832793487574975</v>
+      </c>
+    </row>
+    <row r="24" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C24" s="3">
+        <v>55.195338809034922</v>
+      </c>
+      <c r="D24" s="3">
+        <v>144.581762295082</v>
+      </c>
+      <c r="G24" s="2">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="H24" s="3">
+        <v>28.349989286479541</v>
+      </c>
+      <c r="I24" s="3">
+        <v>75.781182519280208</v>
+      </c>
+    </row>
+    <row r="25" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C25" s="3">
+        <v>54.922843942505132</v>
+      </c>
+      <c r="D25" s="3">
+        <v>160.34065573770491</v>
+      </c>
+      <c r="G25" s="2">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="H25" s="3">
+        <v>28.825558174416109</v>
+      </c>
+      <c r="I25" s="3">
+        <v>73.807754927163671</v>
+      </c>
+    </row>
+    <row r="26" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C26" s="3">
+        <v>53.736314168377831</v>
+      </c>
+      <c r="D26" s="3">
+        <v>171.64590163934429</v>
+      </c>
+      <c r="G26" s="2">
+        <f t="shared" si="1"/>
+        <v>23</v>
+      </c>
+      <c r="H26" s="3">
+        <v>28.412185558174421</v>
+      </c>
+      <c r="I26" s="3">
+        <v>77.834481576692383</v>
+      </c>
+    </row>
+    <row r="27" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C27" s="3">
+        <v>55.846683778234087</v>
+      </c>
+      <c r="D27" s="3">
+        <v>155.17307377049181</v>
+      </c>
+      <c r="G27" s="2">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="H27" s="3">
+        <v>28.42605956717377</v>
+      </c>
+      <c r="I27" s="3">
+        <v>78.10454155955442</v>
+      </c>
+    </row>
+    <row r="28" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C28" s="3">
+        <v>56.90160164271046</v>
+      </c>
+      <c r="D28" s="3">
+        <v>154.92442622950821</v>
+      </c>
+      <c r="G28" s="2">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="H28" s="3">
+        <v>28.45665952431969</v>
+      </c>
+      <c r="I28" s="3">
+        <v>75.399631533847469</v>
+      </c>
+    </row>
+    <row r="29" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C29" s="3">
+        <v>57.720297741273093</v>
+      </c>
+      <c r="D29" s="3">
+        <v>131.96454918032791</v>
+      </c>
+      <c r="G29" s="2">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="H29" s="3">
+        <v>28.3578680094279</v>
+      </c>
+      <c r="I29" s="3">
+        <v>74.72246786632391</v>
+      </c>
+    </row>
+    <row r="30" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C30" s="3">
+        <v>54.252772073921967</v>
+      </c>
+      <c r="D30" s="3">
+        <v>164.648155737705</v>
+      </c>
+      <c r="G30" s="2">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="H30" s="3">
+        <v>28.629217913006212</v>
+      </c>
+      <c r="I30" s="3">
+        <v>76.491713796058278</v>
+      </c>
+    </row>
+    <row r="31" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C31" s="3">
+        <v>56.885503080082131</v>
+      </c>
+      <c r="D31" s="3">
+        <v>159.35274590163939</v>
+      </c>
+      <c r="G31" s="2">
+        <f t="shared" si="1"/>
+        <v>28</v>
+      </c>
+      <c r="H31" s="3">
+        <v>27.95733019070066</v>
+      </c>
+      <c r="I31" s="3">
+        <v>78.162167952013718</v>
+      </c>
+    </row>
+    <row r="32" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="B32" s="2">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C32" s="3">
+        <v>55.655472279260778</v>
+      </c>
+      <c r="D32" s="3">
+        <v>152.5567213114754</v>
+      </c>
+      <c r="G32" s="2">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="H32" s="3">
+        <v>28.297955860295691</v>
+      </c>
+      <c r="I32" s="3">
+        <v>79.027703513281907</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C33" s="3">
+        <v>53.900913757700224</v>
+      </c>
+      <c r="D33" s="3">
+        <v>160.3526639344262</v>
+      </c>
+      <c r="G33" s="2">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="H33" s="3">
+        <v>28.740717805871011</v>
+      </c>
+      <c r="I33" s="3">
+        <v>73.726615252784939</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C34" s="3">
+        <v>55.648809034907607</v>
+      </c>
+      <c r="D34" s="3">
+        <v>151.47782786885239</v>
+      </c>
+      <c r="G34" s="2">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
+      <c r="H34" s="3">
+        <v>28.279772873366191</v>
+      </c>
+      <c r="I34" s="3">
+        <v>77.486752356469594</v>
+      </c>
+    </row>
+    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B35" s="2">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C35" s="3">
+        <v>55.96349075975359</v>
+      </c>
+      <c r="D35" s="3">
+        <v>148.7710245901639</v>
+      </c>
+      <c r="G35" s="2">
+        <f t="shared" si="1"/>
+        <v>32</v>
+      </c>
+      <c r="H35" s="3">
+        <v>27.888521534176132</v>
+      </c>
+      <c r="I35" s="3">
+        <v>78.632253641816618</v>
+      </c>
+    </row>
+    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B36" s="2">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C36" s="3">
+        <v>53.455236139630379</v>
+      </c>
+      <c r="D36" s="3">
+        <v>159.43995901639349</v>
+      </c>
+      <c r="G36" s="2">
+        <f t="shared" si="1"/>
+        <v>33</v>
+      </c>
+      <c r="H36" s="3">
+        <v>28.60212770516392</v>
+      </c>
+      <c r="I36" s="3">
+        <v>74.289991431019715</v>
+      </c>
+    </row>
+    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B37" s="2">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C37" s="3">
+        <v>55.007207392197131</v>
+      </c>
+      <c r="D37" s="3">
+        <v>164.4861885245902</v>
+      </c>
+      <c r="G37" s="2">
+        <f t="shared" si="1"/>
+        <v>34</v>
+      </c>
+      <c r="H37" s="3">
+        <v>28.376125991000631</v>
+      </c>
+      <c r="I37" s="3">
+        <v>76.924413024850054</v>
+      </c>
+    </row>
+    <row r="38" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B38" s="2">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C38" s="3">
+        <v>55.486478439425049</v>
+      </c>
+      <c r="D38" s="3">
+        <v>158.6072540983607</v>
+      </c>
+      <c r="G38" s="2">
+        <f t="shared" si="1"/>
+        <v>35</v>
+      </c>
+      <c r="H38" s="3">
+        <v>28.183970430683519</v>
+      </c>
+      <c r="I38" s="3">
+        <v>79.015115681233937</v>
+      </c>
+    </row>
+    <row r="39" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B39" s="2">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C39" s="3">
+        <v>55.499178644763859</v>
+      </c>
+      <c r="D39" s="3">
+        <v>156.53709016393441</v>
+      </c>
+      <c r="G39" s="2">
+        <f t="shared" si="1"/>
+        <v>36</v>
+      </c>
+      <c r="H39" s="3">
+        <v>28.23765373901864</v>
+      </c>
+      <c r="I39" s="3">
+        <v>79.154378748928877</v>
+      </c>
+    </row>
+    <row r="40" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B40" s="2">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C40" s="3">
+        <v>55.933121149897339</v>
+      </c>
+      <c r="D40" s="3">
+        <v>145.6338524590164</v>
+      </c>
+      <c r="G40" s="2">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="H40" s="3">
+        <v>28.27595671737733</v>
+      </c>
+      <c r="I40" s="3">
+        <v>75.408860325621248</v>
+      </c>
+    </row>
+    <row r="41" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B41" s="2">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C41" s="3">
+        <v>55.354999999999997</v>
+      </c>
+      <c r="D41" s="3">
+        <v>163.1984836065574</v>
+      </c>
+      <c r="G41" s="2">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
+      <c r="H41" s="3">
+        <v>28.569297193057629</v>
+      </c>
+      <c r="I41" s="3">
+        <v>72.763787489288788</v>
+      </c>
+    </row>
+    <row r="42" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B42" s="2">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C42" s="3">
+        <v>58.014702258726899</v>
+      </c>
+      <c r="D42" s="3">
+        <v>135.29864754098361</v>
+      </c>
+      <c r="G42" s="2">
+        <f t="shared" si="1"/>
+        <v>39</v>
+      </c>
+      <c r="H42" s="3">
+        <v>28.271667023784019</v>
+      </c>
+      <c r="I42" s="3">
+        <v>77.937403598971727</v>
+      </c>
+    </row>
+    <row r="43" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B43" s="2">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C43" s="3">
+        <v>57.835903490759762</v>
+      </c>
+      <c r="D43" s="3">
+        <v>139.25954918032781</v>
+      </c>
+      <c r="G43" s="2">
+        <f t="shared" si="1"/>
+        <v>40</v>
+      </c>
+      <c r="H43" s="3">
+        <v>28.04858581529891</v>
+      </c>
+      <c r="I43" s="3">
+        <v>80.903993144815772</v>
+      </c>
+    </row>
+    <row r="44" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B44" s="2">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C44" s="3">
+        <v>53.766950718685841</v>
+      </c>
+      <c r="D44" s="3">
+        <v>175.01897540983609</v>
+      </c>
+      <c r="G44" s="2">
+        <f t="shared" si="1"/>
+        <v>41</v>
+      </c>
+      <c r="H44" s="3">
+        <v>28.140051424898221</v>
+      </c>
+      <c r="I44" s="3">
+        <v>77.879674378748945</v>
+      </c>
+    </row>
+    <row r="45" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B45" s="2">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C45" s="3">
+        <v>55.056180698151962</v>
+      </c>
+      <c r="D45" s="3">
+        <v>151.0440573770492</v>
+      </c>
+      <c r="G45" s="2">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="H45" s="3">
+        <v>28.554926076708799</v>
+      </c>
+      <c r="I45" s="3">
+        <v>74.75144815766923</v>
+      </c>
+    </row>
+    <row r="46" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B46" s="2">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C46" s="3">
+        <v>56.164537987679687</v>
+      </c>
+      <c r="D46" s="3">
+        <v>145.84540983606561</v>
+      </c>
+      <c r="G46" s="2">
+        <f t="shared" si="1"/>
+        <v>43</v>
+      </c>
+      <c r="H46" s="3">
+        <v>28.95710520677094</v>
+      </c>
+      <c r="I46" s="3">
+        <v>74.33588688946017</v>
+      </c>
+    </row>
+    <row r="47" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B47" s="2">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C47" s="3">
+        <v>57.091468172484603</v>
+      </c>
+      <c r="D47" s="3">
+        <v>135.55102459016391</v>
+      </c>
+      <c r="G47" s="2">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="H47" s="3">
+        <v>28.490409256481669</v>
+      </c>
+      <c r="I47" s="3">
+        <v>77.826829477292208</v>
+      </c>
+    </row>
+    <row r="48" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B48" s="2">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C48" s="3">
+        <v>56.354876796714571</v>
+      </c>
+      <c r="D48" s="3">
+        <v>160.80495901639341</v>
+      </c>
+      <c r="G48" s="2">
+        <f t="shared" si="1"/>
+        <v>45</v>
+      </c>
+      <c r="H48" s="3">
+        <v>28.22432826226698</v>
+      </c>
+      <c r="I48" s="3">
+        <v>77.406709511568124</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B49" s="2">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C49" s="3">
+        <v>53.998850102669422</v>
+      </c>
+      <c r="D49" s="3">
+        <v>160.4527868852459</v>
+      </c>
+      <c r="G49" s="2">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="H49" s="3">
+        <v>28.323409042211271</v>
+      </c>
+      <c r="I49" s="3">
+        <v>77.954584404455872</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B50" s="2">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C50" s="3">
+        <v>55.114948665297753</v>
+      </c>
+      <c r="D50" s="3">
+        <v>152.68799180327869</v>
+      </c>
+      <c r="G50" s="2">
+        <f t="shared" si="1"/>
+        <v>47</v>
+      </c>
+      <c r="H50" s="3">
+        <v>28.18232269123634</v>
+      </c>
+      <c r="I50" s="3">
+        <v>77.394755784061701</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B51" s="2">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C51" s="3">
+        <v>55.575585215605763</v>
+      </c>
+      <c r="D51" s="3">
+        <v>162.6149180327869</v>
+      </c>
+      <c r="G51" s="2">
+        <f t="shared" si="1"/>
+        <v>48</v>
+      </c>
+      <c r="H51" s="3">
+        <v>28.92028283694021</v>
+      </c>
+      <c r="I51" s="3">
+        <v>72.815604113110552</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B52" s="2">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C52" s="3">
+        <v>54.782505133470238</v>
+      </c>
+      <c r="D52" s="3">
+        <v>169.36680327868851</v>
+      </c>
+      <c r="G52" s="2">
+        <f t="shared" si="1"/>
+        <v>49</v>
+      </c>
+      <c r="H52" s="3">
+        <v>28.052659095778871</v>
+      </c>
+      <c r="I52" s="3">
+        <v>78.476341045415609</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B53" s="2">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C53" s="3">
+        <v>57.475030800821379</v>
+      </c>
+      <c r="D53" s="3">
+        <v>128.9006147540984</v>
+      </c>
+      <c r="G53" s="2">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="H53" s="3">
+        <v>28.267090207842291</v>
+      </c>
+      <c r="I53" s="3">
+        <v>76.570616966580971</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C55" s="3">
+        <f>AVERAGE(C4:C53)</f>
+        <v>55.762803490759751</v>
+      </c>
+      <c r="D55" s="3">
+        <f>AVERAGE(D4:D53)</f>
+        <v>153.20420819672134</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H55" s="3">
+        <f>AVERAGE(H4:H53)</f>
+        <v>28.370167516605946</v>
+      </c>
+      <c r="I55" s="3">
+        <f>AVERAGE(I4:I53)</f>
+        <v>76.674779777206496</v>
+      </c>
+    </row>
+    <row r="56" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C56" s="3">
+        <f>_xlfn.STDEV.S(C4:C53)</f>
+        <v>1.1892357812622139</v>
+      </c>
+      <c r="D56" s="3">
+        <f>_xlfn.STDEV.S(D4:D53)</f>
+        <v>11.009852940109267</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H56" s="3">
+        <f>_xlfn.STDEV.S(H4:H53)</f>
+        <v>0.26694218585547402</v>
+      </c>
+      <c r="I56" s="3">
+        <f>_xlfn.STDEV.S(I4:I53)</f>
+        <v>2.1716324788976622</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>
@@ -5949,7 +7221,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:P57"/>
   <sheetViews>

</xml_diff>

<commit_message>
hybrid3 corr superdataset24 mse
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pos vs neg" sheetId="3" r:id="rId1"/>
-    <sheet name="Лист1" sheetId="4" r:id="rId2"/>
+    <sheet name="pos vs neg 2" sheetId="4" r:id="rId2"/>
     <sheet name="mae" sheetId="1" r:id="rId3"/>
     <sheet name="mse" sheetId="2" r:id="rId4"/>
   </sheets>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -128,6 +128,9 @@
   <si>
     <t>Hybrid model 3 (superdataset-24-2.csv) balanced</t>
   </si>
+  <si>
+    <t>значимость balanced</t>
+  </si>
 </sst>
 </file>
 
@@ -192,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -224,6 +227,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -858,7 +862,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$R$4:$R$18</c:f>
+              <c:f>'pos vs neg 2'!$R$4:$R$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -999,7 +1003,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$S$4:$S$18</c:f>
+              <c:f>'pos vs neg 2'!$S$4:$S$18</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1268,7 +1272,17 @@
   <c:chart>
     <c:autoTitleDeleted val="1"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="7.1987985584740621E-2"/>
+          <c:y val="5.3723884514435695E-2"/>
+          <c:w val="0.92801201441525938"/>
+          <c:h val="0.74388271466066747"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -1278,7 +1292,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>mse!$P$4</c:f>
+              <c:f>mse!$AK$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1311,7 +1325,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>mse!$O$5:$O$19</c:f>
+              <c:f>mse!$AJ$5:$AJ$19</c:f>
               <c:strCache>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
@@ -1364,54 +1378,54 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>mse!$P$5:$P$19</c:f>
+              <c:f>mse!$AK$5:$AK$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>0.1954810928473423</c:v>
+                  <c:v>5.9078100942579592E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.4358248277851462E-2</c:v>
+                  <c:v>7.1747256485430747E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.0599889488889417E-2</c:v>
+                  <c:v>6.6021581284767011E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.6428044164823457E-2</c:v>
+                  <c:v>5.5989218607260152E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.6617541924901152E-2</c:v>
+                  <c:v>5.5925742131122301E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.6836034630361155E-2</c:v>
+                  <c:v>6.0536211694503163E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.1722452539209198E-2</c:v>
+                  <c:v>6.8679703265968825E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.9690340947174017E-2</c:v>
+                  <c:v>5.9051485991428877E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.443875125164393E-2</c:v>
+                  <c:v>6.1267950411860672E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.0003604342054961E-2</c:v>
+                  <c:v>6.4912499247150993E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>9.0600699378861518E-2</c:v>
+                  <c:v>7.1630954289568616E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>9.0496081779026766E-2</c:v>
+                  <c:v>6.1602652905225853E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4.695592267015105E-2</c:v>
+                  <c:v>6.3823501920893019E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.6855187840790009E-2</c:v>
+                  <c:v>0.11197281737261031</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.8916107916919543E-2</c:v>
+                  <c:v>6.7760323449629817E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3326,16 +3340,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>304799</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>291192</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>141514</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>43</xdr:col>
+      <xdr:colOff>327932</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>46264</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4966,7 +4980,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:S56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
@@ -6309,7 +6323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:Z57"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AB35" sqref="AB35"/>
     </sheetView>
   </sheetViews>
@@ -9746,10 +9760,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:P57"/>
+  <dimension ref="C3:AL57"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AA51" sqref="AA51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9758,11 +9772,18 @@
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
     <col min="9" max="9" width="12.85546875" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="15" max="15" width="15.5703125" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" customWidth="1"/>
+    <col min="15" max="15" width="12.85546875" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="19" max="19" width="10.7109375" customWidth="1"/>
+    <col min="20" max="20" width="9.7109375" customWidth="1"/>
+    <col min="21" max="21" width="13" customWidth="1"/>
+    <col min="22" max="22" width="13.42578125" customWidth="1"/>
+    <col min="36" max="36" width="16.140625" customWidth="1"/>
+    <col min="37" max="37" width="15.85546875" customWidth="1"/>
+    <col min="38" max="38" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
@@ -9771,8 +9792,16 @@
         <v>6</v>
       </c>
       <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V3" s="1"/>
+    </row>
+    <row r="4" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>8</v>
@@ -9790,14 +9819,37 @@
       <c r="K4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="N4" s="2"/>
       <c r="O4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="T4" s="2"/>
+      <c r="U4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="AK4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AL4" s="13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -9819,14 +9871,32 @@
       <c r="K5" s="3">
         <v>0.91938997821350776</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="4">
+        <v>2.1725117709742079E-3</v>
+      </c>
+      <c r="P5" s="4">
+        <v>3.088210903187608E-2</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>0.60493827160493829</v>
+      </c>
+      <c r="T5" s="2">
+        <v>1</v>
+      </c>
+      <c r="U5" s="4"/>
+      <c r="V5" s="4"/>
+      <c r="W5" s="3"/>
+      <c r="AJ5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="P5" s="3">
-        <v>0.1954810928473423</v>
-      </c>
-    </row>
-    <row r="6" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK5" s="3">
+        <v>5.9078100942579592E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -9850,14 +9920,34 @@
       <c r="K6" s="3">
         <v>0.86877828054298634</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="N6" s="2">
+        <f>N5+1</f>
+        <v>2</v>
+      </c>
+      <c r="O6" s="4">
+        <v>2.1883201027737931E-3</v>
+      </c>
+      <c r="P6" s="4">
+        <v>3.1058769672208681E-2</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>0.61507128309572301</v>
+      </c>
+      <c r="T6" s="2">
+        <f>T5+1</f>
+        <v>2</v>
+      </c>
+      <c r="U6" s="4"/>
+      <c r="V6" s="4"/>
+      <c r="W6" s="3"/>
+      <c r="AJ6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="P6" s="3">
-        <v>5.4358248277851462E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK6" s="3">
+        <v>7.1747256485430747E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -9881,14 +9971,34 @@
       <c r="K7" s="3">
         <v>0.91150442477876115</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="N7" s="2">
+        <f t="shared" ref="N7:N54" si="2">N6+1</f>
+        <v>3</v>
+      </c>
+      <c r="O7" s="4">
+        <v>2.205789034642761E-3</v>
+      </c>
+      <c r="P7" s="4">
+        <v>2.9514170046507519E-2</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.63008130081300817</v>
+      </c>
+      <c r="T7" s="2">
+        <f t="shared" ref="T7:T54" si="3">T6+1</f>
+        <v>3</v>
+      </c>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="3"/>
+      <c r="AJ7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="P7" s="3">
-        <v>5.0599889488889417E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK7" s="3">
+        <v>6.6021581284767011E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -9912,14 +10022,34 @@
       <c r="K8" s="3">
         <v>0.90308370044052877</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="N8" s="2">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O8" s="4">
+        <v>2.2418560823625512E-3</v>
+      </c>
+      <c r="P8" s="4">
+        <v>2.802567116669933E-2</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>0.60493827160493829</v>
+      </c>
+      <c r="T8" s="2">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="3"/>
+      <c r="AJ8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="P8" s="3">
-        <v>5.6428044164823457E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK8" s="3">
+        <v>5.5989218607260152E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -9943,14 +10073,34 @@
       <c r="K9" s="3">
         <v>0.89977728285077951</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="N9" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="O9" s="4">
+        <v>2.172093048609157E-3</v>
+      </c>
+      <c r="P9" s="4">
+        <v>3.1378881144606227E-2</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>0.58158995815899572</v>
+      </c>
+      <c r="T9" s="2">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+      <c r="U9" s="4"/>
+      <c r="V9" s="4"/>
+      <c r="W9" s="3"/>
+      <c r="AJ9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P9" s="3">
-        <v>3.6617541924901152E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK9" s="3">
+        <v>5.5925742131122301E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -9974,14 +10124,34 @@
       <c r="K10" s="3">
         <v>0.91352549889135259</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="N10" s="2">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="O10" s="4">
+        <v>2.190430055483924E-3</v>
+      </c>
+      <c r="P10" s="4">
+        <v>3.2334151378565587E-2</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>0.55072463768115942</v>
+      </c>
+      <c r="T10" s="2">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+      <c r="U10" s="4"/>
+      <c r="V10" s="4"/>
+      <c r="W10" s="3"/>
+      <c r="AJ10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="3">
-        <v>6.6836034630361155E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK10" s="3">
+        <v>6.0536211694503163E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -10005,14 +10175,34 @@
       <c r="K11" s="3">
         <v>0.92341356673960617</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="N11" s="2">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="O11" s="4">
+        <v>2.1649445616542672E-3</v>
+      </c>
+      <c r="P11" s="4">
+        <v>3.1336272549952228E-2</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.54623655913978486</v>
+      </c>
+      <c r="T11" s="2">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+      <c r="U11" s="4"/>
+      <c r="V11" s="4"/>
+      <c r="W11" s="3"/>
+      <c r="AJ11" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P11" s="3">
-        <v>4.1722452539209198E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK11" s="3">
+        <v>6.8679703265968825E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -10036,14 +10226,34 @@
       <c r="K12" s="3">
         <v>0.89485458612975399</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="N12" s="2">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="O12" s="4">
+        <v>2.2328104576801312E-3</v>
+      </c>
+      <c r="P12" s="4">
+        <v>2.89893210565631E-2</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.56475583864118895</v>
+      </c>
+      <c r="T12" s="2">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+      <c r="U12" s="4"/>
+      <c r="V12" s="4"/>
+      <c r="W12" s="3"/>
+      <c r="AJ12" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="P12" s="3">
-        <v>3.9690340947174017E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK12" s="3">
+        <v>5.9051485991428877E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -10067,14 +10277,34 @@
       <c r="K13" s="3">
         <v>0.89686098654708535</v>
       </c>
-      <c r="O13" s="6" t="s">
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="O13" s="4">
+        <v>2.2059788587199059E-3</v>
+      </c>
+      <c r="P13" s="4">
+        <v>3.5278863736186432E-2</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>0.57928118393234673</v>
+      </c>
+      <c r="T13" s="2">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+      <c r="U13" s="4"/>
+      <c r="V13" s="4"/>
+      <c r="W13" s="3"/>
+      <c r="AJ13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="P13" s="3">
-        <v>6.443875125164393E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK13" s="3">
+        <v>6.1267950411860672E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -10098,14 +10328,34 @@
       <c r="K14" s="3">
         <v>0.92872570194384452</v>
       </c>
-      <c r="O14" s="6" t="s">
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="O14" s="4">
+        <v>2.1049612445523079E-3</v>
+      </c>
+      <c r="P14" s="4">
+        <v>3.4770514525747843E-2</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>0.61632653061224496</v>
+      </c>
+      <c r="T14" s="2">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="U14" s="4"/>
+      <c r="V14" s="4"/>
+      <c r="W14" s="3"/>
+      <c r="AJ14" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P14" s="3">
-        <v>5.0003604342054961E-2</v>
-      </c>
-    </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK14" s="3">
+        <v>6.4912499247150993E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -10129,14 +10379,34 @@
       <c r="K15" s="3">
         <v>0.88487584650112872</v>
       </c>
-      <c r="O15" s="6" t="s">
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="O15" s="4">
+        <v>2.216441972778988E-3</v>
+      </c>
+      <c r="P15" s="4">
+        <v>2.9328559724642E-2</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>0.63052208835341372</v>
+      </c>
+      <c r="T15" s="2">
+        <f t="shared" si="3"/>
+        <v>11</v>
+      </c>
+      <c r="U15" s="4"/>
+      <c r="V15" s="4"/>
+      <c r="W15" s="3"/>
+      <c r="AJ15" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="P15" s="3">
-        <v>9.0600699378861518E-2</v>
-      </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK15" s="3">
+        <v>7.1630954289568616E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -10160,14 +10430,34 @@
       <c r="K16" s="3">
         <v>0.90380313199105144</v>
       </c>
-      <c r="O16" s="6" t="s">
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="O16" s="4">
+        <v>2.231150061003041E-3</v>
+      </c>
+      <c r="P16" s="4">
+        <v>2.7825355207568171E-2</v>
+      </c>
+      <c r="Q16" s="3">
+        <v>0.62833675564681724</v>
+      </c>
+      <c r="T16" s="2">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="3"/>
+      <c r="AJ16" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="P16" s="3">
-        <v>9.0496081779026766E-2</v>
-      </c>
-    </row>
-    <row r="17" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK16" s="3">
+        <v>6.1602652905225853E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -10191,14 +10481,34 @@
       <c r="K17" s="3">
         <v>0.8868778280542986</v>
       </c>
-      <c r="O17" s="6" t="s">
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="O17" s="4">
+        <v>2.2070409143103982E-3</v>
+      </c>
+      <c r="P17" s="4">
+        <v>3.14153673982965E-2</v>
+      </c>
+      <c r="Q17" s="3">
+        <v>0.56302521008403361</v>
+      </c>
+      <c r="T17" s="2">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+      <c r="U17" s="4"/>
+      <c r="V17" s="4"/>
+      <c r="W17" s="3"/>
+      <c r="AJ17" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="P17" s="3">
-        <v>4.695592267015105E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK17" s="3">
+        <v>6.3823501920893019E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -10222,14 +10532,34 @@
       <c r="K18" s="3">
         <v>0.90350877192982448</v>
       </c>
-      <c r="O18" s="6" t="s">
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="O18" s="4">
+        <v>2.2176850946951298E-3</v>
+      </c>
+      <c r="P18" s="4">
+        <v>2.875799324924562E-2</v>
+      </c>
+      <c r="Q18" s="3">
+        <v>0.61349693251533743</v>
+      </c>
+      <c r="T18" s="2">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+      <c r="U18" s="4"/>
+      <c r="V18" s="4"/>
+      <c r="W18" s="3"/>
+      <c r="AJ18" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P18" s="3">
-        <v>5.6855187840790009E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK18" s="3">
+        <v>0.11197281737261031</v>
+      </c>
+    </row>
+    <row r="19" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -10253,14 +10583,34 @@
       <c r="K19" s="3">
         <v>0.90350877192982448</v>
       </c>
-      <c r="O19" s="7" t="s">
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="O19" s="4">
+        <v>2.1340337516804488E-3</v>
+      </c>
+      <c r="P19" s="4">
+        <v>3.3674465558096119E-2</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0.59793814432989689</v>
+      </c>
+      <c r="T19" s="2">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+      <c r="U19" s="4"/>
+      <c r="V19" s="4"/>
+      <c r="W19" s="3"/>
+      <c r="AJ19" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="P19" s="3">
-        <v>5.8916107916919543E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="AK19" s="3">
+        <v>6.7760323449629817E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -10284,8 +10634,28 @@
       <c r="K20" s="3">
         <v>0.90869565217391302</v>
       </c>
-    </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="O20" s="4">
+        <v>2.1730541557602079E-3</v>
+      </c>
+      <c r="P20" s="4">
+        <v>2.8677798665624411E-2</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.58872651356993733</v>
+      </c>
+      <c r="T20" s="2">
+        <f t="shared" si="3"/>
+        <v>16</v>
+      </c>
+      <c r="U20" s="4"/>
+      <c r="V20" s="4"/>
+      <c r="W20" s="3"/>
+    </row>
+    <row r="21" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -10309,10 +10679,28 @@
       <c r="K21" s="3">
         <v>0.92747252747252751</v>
       </c>
-      <c r="O21" s="6"/>
-      <c r="P21" s="3"/>
-    </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="O21" s="4">
+        <v>2.1411171313397231E-3</v>
+      </c>
+      <c r="P21" s="4">
+        <v>3.025679365803809E-2</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>0.59917355371900827</v>
+      </c>
+      <c r="T21" s="2">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+      <c r="U21" s="4"/>
+      <c r="V21" s="4"/>
+      <c r="W21" s="3"/>
+    </row>
+    <row r="22" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -10336,8 +10724,28 @@
       <c r="K22" s="3">
         <v>0.90380313199105144</v>
       </c>
-    </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N22" s="2">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="O22" s="4">
+        <v>2.2121124353672861E-3</v>
+      </c>
+      <c r="P22" s="4">
+        <v>2.9720702855517148E-2</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>0.58649789029535859</v>
+      </c>
+      <c r="T22" s="2">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+      <c r="U22" s="4"/>
+      <c r="V22" s="4"/>
+      <c r="W22" s="3"/>
+    </row>
+    <row r="23" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -10361,8 +10769,28 @@
       <c r="K23" s="3">
         <v>0.89795918367346927</v>
       </c>
-    </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N23" s="2">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="O23" s="4">
+        <v>2.193153403465182E-3</v>
+      </c>
+      <c r="P23" s="4">
+        <v>3.033707022856021E-2</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>0.59548254620123209</v>
+      </c>
+      <c r="T23" s="2">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+      <c r="U23" s="4"/>
+      <c r="V23" s="4"/>
+      <c r="W23" s="3"/>
+    </row>
+    <row r="24" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -10386,8 +10814,28 @@
       <c r="K24" s="3">
         <v>0.8928571428571429</v>
       </c>
-    </row>
-    <row r="25" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N24" s="2">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="O24" s="4">
+        <v>2.202728094446198E-3</v>
+      </c>
+      <c r="P24" s="4">
+        <v>3.0208728167133169E-2</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>0.56431535269709543</v>
+      </c>
+      <c r="T24" s="2">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+      <c r="U24" s="4"/>
+      <c r="V24" s="4"/>
+      <c r="W24" s="3"/>
+    </row>
+    <row r="25" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -10411,8 +10859,28 @@
       <c r="K25" s="3">
         <v>0.91973969631236441</v>
       </c>
-    </row>
-    <row r="26" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N25" s="2">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="O25" s="4">
+        <v>2.159377273960129E-3</v>
+      </c>
+      <c r="P25" s="4">
+        <v>3.0378932697091549E-2</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>0.56289978678038377</v>
+      </c>
+      <c r="T25" s="2">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+      <c r="U25" s="4"/>
+      <c r="V25" s="4"/>
+      <c r="W25" s="3"/>
+    </row>
+    <row r="26" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -10436,8 +10904,28 @@
       <c r="K26" s="3">
         <v>0.93275488069414314</v>
       </c>
-    </row>
-    <row r="27" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N26" s="2">
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="O26" s="4">
+        <v>2.1976001333872072E-3</v>
+      </c>
+      <c r="P26" s="4">
+        <v>3.3745484687675617E-2</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>0.58486707566462171</v>
+      </c>
+      <c r="T26" s="2">
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+      <c r="U26" s="4"/>
+      <c r="V26" s="4"/>
+      <c r="W26" s="3"/>
+    </row>
+    <row r="27" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -10461,8 +10949,28 @@
       <c r="K27" s="3">
         <v>0.9111111111111112</v>
       </c>
-    </row>
-    <row r="28" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N27" s="2">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="O27" s="4">
+        <v>2.1241938503473012E-3</v>
+      </c>
+      <c r="P27" s="4">
+        <v>3.3269885375841142E-2</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>0.52813852813852813</v>
+      </c>
+      <c r="T27" s="2">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="3"/>
+    </row>
+    <row r="28" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -10486,8 +10994,28 @@
       <c r="K28" s="3">
         <v>0.91703056768558955</v>
       </c>
-    </row>
-    <row r="29" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N28" s="2">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="O28" s="4">
+        <v>2.207660182027294E-3</v>
+      </c>
+      <c r="P28" s="4">
+        <v>3.2872394336821237E-2</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>0.5641025641025641</v>
+      </c>
+      <c r="T28" s="2">
+        <f t="shared" si="3"/>
+        <v>24</v>
+      </c>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="3"/>
+    </row>
+    <row r="29" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -10511,8 +11039,28 @@
       <c r="K29" s="3">
         <v>0.9126637554585153</v>
       </c>
-    </row>
-    <row r="30" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N29" s="2">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="O29" s="4">
+        <v>2.2463117240311189E-3</v>
+      </c>
+      <c r="P29" s="4">
+        <v>2.8319380947523759E-2</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>0.60251046025104604</v>
+      </c>
+      <c r="T29" s="2">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="3"/>
+    </row>
+    <row r="30" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -10536,8 +11084,28 @@
       <c r="K30" s="3">
         <v>0.89342403628117906</v>
       </c>
-    </row>
-    <row r="31" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N30" s="2">
+        <f t="shared" si="2"/>
+        <v>26</v>
+      </c>
+      <c r="O30" s="4">
+        <v>2.1668073590391059E-3</v>
+      </c>
+      <c r="P30" s="4">
+        <v>3.3208450346997251E-2</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>0.60041407867494823</v>
+      </c>
+      <c r="T30" s="2">
+        <f t="shared" si="3"/>
+        <v>26</v>
+      </c>
+      <c r="U30" s="4"/>
+      <c r="V30" s="4"/>
+      <c r="W30" s="3"/>
+    </row>
+    <row r="31" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -10561,8 +11129,28 @@
       <c r="K31" s="3">
         <v>0.90909090909090906</v>
       </c>
-    </row>
-    <row r="32" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="N31" s="2">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+      <c r="O31" s="4">
+        <v>2.219101759425671E-3</v>
+      </c>
+      <c r="P31" s="4">
+        <v>3.070137723210193E-2</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>0.60692464358452136</v>
+      </c>
+      <c r="T31" s="2">
+        <f t="shared" si="3"/>
+        <v>27</v>
+      </c>
+      <c r="U31" s="4"/>
+      <c r="V31" s="4"/>
+      <c r="W31" s="3"/>
+    </row>
+    <row r="32" spans="3:37" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -10586,8 +11174,28 @@
       <c r="K32" s="3">
         <v>0.90507726269315669</v>
       </c>
-    </row>
-    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N32" s="2">
+        <f t="shared" si="2"/>
+        <v>28</v>
+      </c>
+      <c r="O32" s="4">
+        <v>2.1667665687289178E-3</v>
+      </c>
+      <c r="P32" s="4">
+        <v>2.9531981782549611E-2</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>0.61443298969072169</v>
+      </c>
+      <c r="T32" s="2">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+      <c r="U32" s="4"/>
+      <c r="V32" s="4"/>
+      <c r="W32" s="3"/>
+    </row>
+    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -10611,8 +11219,28 @@
       <c r="K33" s="3">
         <v>0.8783783783783784</v>
       </c>
-    </row>
-    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N33" s="2">
+        <f t="shared" si="2"/>
+        <v>29</v>
+      </c>
+      <c r="O33" s="4">
+        <v>2.1881356960659838E-3</v>
+      </c>
+      <c r="P33" s="4">
+        <v>3.1414036663573938E-2</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>0.5967078189300411</v>
+      </c>
+      <c r="T33" s="2">
+        <f t="shared" si="3"/>
+        <v>29</v>
+      </c>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="3"/>
+    </row>
+    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -10636,8 +11264,28 @@
       <c r="K34" s="3">
         <v>0.90949227373068431</v>
       </c>
-    </row>
-    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N34" s="2">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="O34" s="4">
+        <v>2.213604252536157E-3</v>
+      </c>
+      <c r="P34" s="4">
+        <v>3.1997519892149433E-2</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>0.61349693251533743</v>
+      </c>
+      <c r="T34" s="2">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="U34" s="4"/>
+      <c r="V34" s="4"/>
+      <c r="W34" s="3"/>
+    </row>
+    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -10661,8 +11309,28 @@
       <c r="K35" s="3">
         <v>0.91428571428571437</v>
       </c>
-    </row>
-    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N35" s="2">
+        <f t="shared" si="2"/>
+        <v>31</v>
+      </c>
+      <c r="O35" s="4">
+        <v>2.2957592801928751E-3</v>
+      </c>
+      <c r="P35" s="4">
+        <v>2.6765811819423349E-2</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>0.61475409836065575</v>
+      </c>
+      <c r="T35" s="2">
+        <f t="shared" si="3"/>
+        <v>31</v>
+      </c>
+      <c r="U35" s="4"/>
+      <c r="V35" s="4"/>
+      <c r="W35" s="3"/>
+    </row>
+    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -10686,8 +11354,28 @@
       <c r="K36" s="3">
         <v>0.8928571428571429</v>
       </c>
-    </row>
-    <row r="37" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N36" s="2">
+        <f t="shared" si="2"/>
+        <v>32</v>
+      </c>
+      <c r="O36" s="4">
+        <v>2.273142470180733E-3</v>
+      </c>
+      <c r="P36" s="4">
+        <v>3.019052346529973E-2</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>0.58316221765913756</v>
+      </c>
+      <c r="T36" s="2">
+        <f t="shared" si="3"/>
+        <v>32</v>
+      </c>
+      <c r="U36" s="4"/>
+      <c r="V36" s="4"/>
+      <c r="W36" s="3"/>
+    </row>
+    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -10711,8 +11399,28 @@
       <c r="K37" s="3">
         <v>0.91390728476821192</v>
       </c>
-    </row>
-    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N37" s="2">
+        <f t="shared" si="2"/>
+        <v>33</v>
+      </c>
+      <c r="O37" s="4">
+        <v>2.2030967118388109E-3</v>
+      </c>
+      <c r="P37" s="4">
+        <v>3.0096736305791121E-2</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>0.6262626262626263</v>
+      </c>
+      <c r="T37" s="2">
+        <f t="shared" si="3"/>
+        <v>33</v>
+      </c>
+      <c r="U37" s="4"/>
+      <c r="V37" s="4"/>
+      <c r="W37" s="3"/>
+    </row>
+    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -10736,8 +11444,28 @@
       <c r="K38" s="3">
         <v>0.88741721854304645</v>
       </c>
-    </row>
-    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N38" s="2">
+        <f t="shared" si="2"/>
+        <v>34</v>
+      </c>
+      <c r="O38" s="4">
+        <v>2.223258825862582E-3</v>
+      </c>
+      <c r="P38" s="4">
+        <v>3.0716777631687359E-2</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>0.59336099585062241</v>
+      </c>
+      <c r="T38" s="2">
+        <f t="shared" si="3"/>
+        <v>34</v>
+      </c>
+      <c r="U38" s="4"/>
+      <c r="V38" s="4"/>
+      <c r="W38" s="3"/>
+    </row>
+    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -10761,8 +11489,28 @@
       <c r="K39" s="3">
         <v>0.8868778280542986</v>
       </c>
-    </row>
-    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N39" s="2">
+        <f t="shared" si="2"/>
+        <v>35</v>
+      </c>
+      <c r="O39" s="4">
+        <v>2.2203428498830048E-3</v>
+      </c>
+      <c r="P39" s="4">
+        <v>2.973368092717921E-2</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>0.62248995983935751</v>
+      </c>
+      <c r="T39" s="2">
+        <f t="shared" si="3"/>
+        <v>35</v>
+      </c>
+      <c r="U39" s="4"/>
+      <c r="V39" s="4"/>
+      <c r="W39" s="3"/>
+    </row>
+    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -10786,8 +11534,28 @@
       <c r="K40" s="3">
         <v>0.88392857142857129</v>
       </c>
-    </row>
-    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N40" s="2">
+        <f t="shared" si="2"/>
+        <v>36</v>
+      </c>
+      <c r="O40" s="4">
+        <v>2.2130193717266279E-3</v>
+      </c>
+      <c r="P40" s="4">
+        <v>3.0267145014937141E-2</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>0.5950413223140496</v>
+      </c>
+      <c r="T40" s="2">
+        <f t="shared" si="3"/>
+        <v>36</v>
+      </c>
+      <c r="U40" s="4"/>
+      <c r="V40" s="4"/>
+      <c r="W40" s="3"/>
+    </row>
+    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -10811,8 +11579,28 @@
       <c r="K41" s="3">
         <v>0.89485458612975399</v>
       </c>
-    </row>
-    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N41" s="2">
+        <f t="shared" si="2"/>
+        <v>37</v>
+      </c>
+      <c r="O41" s="4">
+        <v>2.228591407074005E-3</v>
+      </c>
+      <c r="P41" s="4">
+        <v>2.644646603433469E-2</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>0.66011787819253431</v>
+      </c>
+      <c r="T41" s="2">
+        <f t="shared" si="3"/>
+        <v>37</v>
+      </c>
+      <c r="U41" s="4"/>
+      <c r="V41" s="4"/>
+      <c r="W41" s="3"/>
+    </row>
+    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -10836,8 +11624,28 @@
       <c r="K42" s="3">
         <v>0.92810457516339873</v>
       </c>
-    </row>
-    <row r="43" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N42" s="2">
+        <f t="shared" si="2"/>
+        <v>38</v>
+      </c>
+      <c r="O42" s="4">
+        <v>2.1679989820132918E-3</v>
+      </c>
+      <c r="P42" s="4">
+        <v>3.2042046580432797E-2</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>0.58436213991769548</v>
+      </c>
+      <c r="T42" s="2">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+      <c r="U42" s="4"/>
+      <c r="V42" s="4"/>
+      <c r="W42" s="3"/>
+    </row>
+    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -10861,8 +11669,28 @@
       <c r="K43" s="3">
         <v>0.90134529147982068</v>
       </c>
-    </row>
-    <row r="44" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N43" s="2">
+        <f t="shared" si="2"/>
+        <v>39</v>
+      </c>
+      <c r="O43" s="4">
+        <v>2.19316404238811E-3</v>
+      </c>
+      <c r="P43" s="4">
+        <v>2.6770752144825931E-2</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>0.61728395061728392</v>
+      </c>
+      <c r="T43" s="2">
+        <f t="shared" si="3"/>
+        <v>39</v>
+      </c>
+      <c r="U43" s="4"/>
+      <c r="V43" s="4"/>
+      <c r="W43" s="3"/>
+    </row>
+    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -10886,8 +11714,28 @@
       <c r="K44" s="3">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="45" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N44" s="2">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="4">
+        <v>2.1364530792186281E-3</v>
+      </c>
+      <c r="P44" s="4">
+        <v>3.3779903022816693E-2</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>0.5967078189300411</v>
+      </c>
+      <c r="T44" s="2">
+        <f t="shared" si="3"/>
+        <v>40</v>
+      </c>
+      <c r="U44" s="4"/>
+      <c r="V44" s="4"/>
+      <c r="W44" s="3"/>
+    </row>
+    <row r="45" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -10911,8 +11759,28 @@
       <c r="K45" s="3">
         <v>0.89438202247191023</v>
       </c>
-    </row>
-    <row r="46" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N45" s="2">
+        <f t="shared" si="2"/>
+        <v>41</v>
+      </c>
+      <c r="O45" s="4">
+        <v>2.11306975233339E-3</v>
+      </c>
+      <c r="P45" s="4">
+        <v>3.3748707063649727E-2</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>0.59789473684210526</v>
+      </c>
+      <c r="T45" s="2">
+        <f t="shared" si="3"/>
+        <v>41</v>
+      </c>
+      <c r="U45" s="4"/>
+      <c r="V45" s="4"/>
+      <c r="W45" s="3"/>
+    </row>
+    <row r="46" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -10936,8 +11804,28 @@
       <c r="K46" s="3">
         <v>0.8669724770642202</v>
       </c>
-    </row>
-    <row r="47" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N46" s="2">
+        <f t="shared" si="2"/>
+        <v>42</v>
+      </c>
+      <c r="O46" s="4">
+        <v>2.16531176191017E-3</v>
+      </c>
+      <c r="P46" s="4">
+        <v>2.9218207779042629E-2</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>0.58467741935483875</v>
+      </c>
+      <c r="T46" s="2">
+        <f t="shared" si="3"/>
+        <v>42</v>
+      </c>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="3"/>
+    </row>
+    <row r="47" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -10961,8 +11849,28 @@
       <c r="K47" s="3">
         <v>0.92841648590021697</v>
       </c>
-    </row>
-    <row r="48" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N47" s="2">
+        <f t="shared" si="2"/>
+        <v>43</v>
+      </c>
+      <c r="O47" s="4">
+        <v>2.1851579391022218E-3</v>
+      </c>
+      <c r="P47" s="4">
+        <v>3.0709032050495091E-2</v>
+      </c>
+      <c r="Q47" s="3">
+        <v>0.62576687116564422</v>
+      </c>
+      <c r="T47" s="2">
+        <f t="shared" si="3"/>
+        <v>43</v>
+      </c>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="3"/>
+    </row>
+    <row r="48" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -10986,8 +11894,28 @@
       <c r="K48" s="3">
         <v>0.91228070175438603</v>
       </c>
-    </row>
-    <row r="49" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N48" s="2">
+        <f t="shared" si="2"/>
+        <v>44</v>
+      </c>
+      <c r="O48" s="4">
+        <v>2.115813907309192E-3</v>
+      </c>
+      <c r="P48" s="4">
+        <v>3.5847612255756639E-2</v>
+      </c>
+      <c r="Q48" s="3">
+        <v>0.57387580299785856</v>
+      </c>
+      <c r="T48" s="2">
+        <f t="shared" si="3"/>
+        <v>44</v>
+      </c>
+      <c r="U48" s="4"/>
+      <c r="V48" s="4"/>
+      <c r="W48" s="3"/>
+    </row>
+    <row r="49" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -11011,8 +11939,28 @@
       <c r="K49" s="3">
         <v>0.88127853881278551</v>
       </c>
-    </row>
-    <row r="50" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N49" s="2">
+        <f t="shared" si="2"/>
+        <v>45</v>
+      </c>
+      <c r="O49" s="4">
+        <v>2.184954829423112E-3</v>
+      </c>
+      <c r="P49" s="4">
+        <v>3.4065672177002258E-2</v>
+      </c>
+      <c r="Q49" s="3">
+        <v>0.60323886639676105</v>
+      </c>
+      <c r="T49" s="2">
+        <f t="shared" si="3"/>
+        <v>45</v>
+      </c>
+      <c r="U49" s="4"/>
+      <c r="V49" s="4"/>
+      <c r="W49" s="3"/>
+    </row>
+    <row r="50" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -11036,8 +11984,28 @@
       <c r="K50" s="3">
         <v>0.92139737991266379</v>
       </c>
-    </row>
-    <row r="51" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N50" s="2">
+        <f t="shared" si="2"/>
+        <v>46</v>
+      </c>
+      <c r="O50" s="4">
+        <v>2.2465926082326062E-3</v>
+      </c>
+      <c r="P50" s="4">
+        <v>2.6763167253955611E-2</v>
+      </c>
+      <c r="Q50" s="3">
+        <v>0.64372469635627527</v>
+      </c>
+      <c r="T50" s="2">
+        <f t="shared" si="3"/>
+        <v>46</v>
+      </c>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
+      <c r="W50" s="3"/>
+    </row>
+    <row r="51" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -11061,8 +12029,28 @@
       <c r="K51" s="3">
         <v>0.89333333333333331</v>
       </c>
-    </row>
-    <row r="52" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N51" s="2">
+        <f t="shared" si="2"/>
+        <v>47</v>
+      </c>
+      <c r="O51" s="4">
+        <v>2.1594137804813872E-3</v>
+      </c>
+      <c r="P51" s="4">
+        <v>3.2357381538423068E-2</v>
+      </c>
+      <c r="Q51" s="3">
+        <v>0.62348178137651811</v>
+      </c>
+      <c r="T51" s="2">
+        <f t="shared" si="3"/>
+        <v>47</v>
+      </c>
+      <c r="U51" s="4"/>
+      <c r="V51" s="4"/>
+      <c r="W51" s="3"/>
+    </row>
+    <row r="52" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -11086,8 +12074,28 @@
       <c r="K52" s="3">
         <v>0.90423162583518935</v>
       </c>
-    </row>
-    <row r="53" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N52" s="2">
+        <f t="shared" si="2"/>
+        <v>48</v>
+      </c>
+      <c r="O52" s="4">
+        <v>2.1835109027562609E-3</v>
+      </c>
+      <c r="P52" s="4">
+        <v>3.0305959939055251E-2</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>0.58506224066390045</v>
+      </c>
+      <c r="T52" s="2">
+        <f t="shared" si="3"/>
+        <v>48</v>
+      </c>
+      <c r="U52" s="4"/>
+      <c r="V52" s="4"/>
+      <c r="W52" s="3"/>
+    </row>
+    <row r="53" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -11111,8 +12119,28 @@
       <c r="K53" s="3">
         <v>0.90748898678414092</v>
       </c>
-    </row>
-    <row r="54" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N53" s="2">
+        <f t="shared" si="2"/>
+        <v>49</v>
+      </c>
+      <c r="O53" s="4">
+        <v>2.2082425121197069E-3</v>
+      </c>
+      <c r="P53" s="4">
+        <v>3.0705264643286229E-2</v>
+      </c>
+      <c r="Q53" s="3">
+        <v>0.59043659043659047</v>
+      </c>
+      <c r="T53" s="2">
+        <f t="shared" si="3"/>
+        <v>49</v>
+      </c>
+      <c r="U53" s="4"/>
+      <c r="V53" s="4"/>
+      <c r="W53" s="3"/>
+    </row>
+    <row r="54" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -11136,14 +12164,38 @@
       <c r="K54" s="3">
         <v>0.89639639639639634</v>
       </c>
-    </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N54" s="2">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="O54" s="4">
+        <v>2.2090955605758031E-3</v>
+      </c>
+      <c r="P54" s="4">
+        <v>2.9282327574135798E-2</v>
+      </c>
+      <c r="Q54" s="3">
+        <v>0.59514170040485825</v>
+      </c>
+      <c r="T54" s="2">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="U54" s="4"/>
+      <c r="V54" s="4"/>
+      <c r="W54" s="3"/>
+    </row>
+    <row r="55" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="I55" s="5"/>
       <c r="J55" s="5"/>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="O55" s="5"/>
+      <c r="P55" s="5"/>
+      <c r="U55" s="5"/>
+      <c r="V55" s="5"/>
+    </row>
+    <row r="56" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -11170,8 +12222,38 @@
         <f>AVERAGE(K5:K54)</f>
         <v>0.90376923389460639</v>
       </c>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="N56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="O56" s="4">
+        <f>AVERAGE(O5:O54)</f>
+        <v>2.1924752321294204E-3</v>
+      </c>
+      <c r="P56" s="4">
+        <f>AVERAGE(P5:P54)</f>
+        <v>3.0780483564109805E-2</v>
+      </c>
+      <c r="Q56" s="3">
+        <f>AVERAGE(Q5:Q54)</f>
+        <v>0.59705594829937059</v>
+      </c>
+      <c r="T56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U56" s="4" t="e">
+        <f>AVERAGE(U5:U54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V56" s="4" t="e">
+        <f>AVERAGE(V5:V54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W56" s="3" t="e">
+        <f>AVERAGE(W5:W54)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="57" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -11197,6 +12279,36 @@
       <c r="K57" s="3">
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>1.5395698477376924E-2</v>
+      </c>
+      <c r="N57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O57" s="4">
+        <f>_xlfn.STDEV.S(O5:O54)</f>
+        <v>3.9655871667715098E-5</v>
+      </c>
+      <c r="P57" s="4">
+        <f>_xlfn.STDEV.S(P5:P54)</f>
+        <v>2.2554860774544171E-3</v>
+      </c>
+      <c r="Q57" s="3">
+        <f>_xlfn.STDEV.S(Q5:Q54)</f>
+        <v>2.5586981934371929E-2</v>
+      </c>
+      <c r="T57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="U57" s="4" t="e">
+        <f>_xlfn.STDEV.S(U5:U54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="V57" s="4" t="e">
+        <f>_xlfn.STDEV.S(V5:V54)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="W57" s="3" t="e">
+        <f>_xlfn.STDEV.S(W5:W54)</f>
+        <v>#DIV/0!</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
single model on balanced dataset (mae)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -131,6 +131,9 @@
   <si>
     <t>значимость balanced</t>
   </si>
+  <si>
+    <t>Random Forest-100 (superdataset-24 balanced.csv)</t>
+  </si>
 </sst>
 </file>
 
@@ -169,7 +172,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -179,6 +182,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +204,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -228,6 +237,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -6320,10 +6341,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:Z57"/>
+  <dimension ref="C3:AD57"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AB19" sqref="AB19"/>
+      <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6337,21 +6358,28 @@
     <col min="20" max="20" width="10.42578125" customWidth="1"/>
     <col min="24" max="24" width="14.28515625" customWidth="1"/>
     <col min="25" max="25" width="12.85546875" customWidth="1"/>
+    <col min="29" max="29" width="14.42578125" customWidth="1"/>
+    <col min="30" max="30" width="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="M3" s="1" t="s">
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="15"/>
+      <c r="M3" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="N3" s="15"/>
+      <c r="O3" s="14"/>
+      <c r="P3" s="15"/>
       <c r="R3" s="1" t="s">
         <v>33</v>
       </c>
@@ -6360,8 +6388,12 @@
         <v>34</v>
       </c>
       <c r="Y3" s="1"/>
-    </row>
-    <row r="4" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AD3" s="1"/>
+    </row>
+    <row r="4" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
         <v>0</v>
@@ -6369,24 +6401,25 @@
       <c r="E4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2" t="s">
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
+      <c r="N4" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="O4" s="2" t="s">
+      <c r="O4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="P4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="R4" s="2"/>
@@ -6409,8 +6442,15 @@
       <c r="Z4" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB4" s="2"/>
+      <c r="AC4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C5" s="2">
         <v>1</v>
       </c>
@@ -6420,28 +6460,29 @@
       <c r="E5" s="3">
         <v>94.979852249832092</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="16">
         <v>1</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5" s="17">
         <v>32.942101898101903</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5" s="17">
         <v>97.66714057507987</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="17">
         <v>0.88487584650112872</v>
       </c>
-      <c r="M5" s="2">
+      <c r="L5" s="15"/>
+      <c r="M5" s="16">
         <v>1</v>
       </c>
-      <c r="N5" s="3">
+      <c r="N5" s="17">
         <v>42.156040061633277</v>
       </c>
-      <c r="O5" s="3">
+      <c r="O5" s="17">
         <v>118.4294866529774</v>
       </c>
-      <c r="P5" s="3">
+      <c r="P5" s="17">
         <v>0.9494949494949495</v>
       </c>
       <c r="R5" s="2">
@@ -6468,8 +6509,17 @@
       <c r="Z5" s="3">
         <v>0.75766871165644178</v>
       </c>
-    </row>
-    <row r="6" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>43.430745052386499</v>
+      </c>
+      <c r="AD5" s="3">
+        <v>118.2650852713178</v>
+      </c>
+    </row>
+    <row r="6" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C6" s="2">
         <f>C5+1</f>
         <v>2</v>
@@ -6480,30 +6530,31 @@
       <c r="E6" s="3">
         <v>96.483243787777027</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="16">
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6" s="17">
         <v>32.700607392607402</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6" s="17">
         <v>98.875822683706076</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="17">
         <v>0.90748898678414092</v>
       </c>
-      <c r="M6" s="2">
+      <c r="L6" s="15"/>
+      <c r="M6" s="16">
         <f>M5+1</f>
         <v>2</v>
       </c>
-      <c r="N6" s="3">
+      <c r="N6" s="17">
         <v>41.041515151515163</v>
       </c>
-      <c r="O6" s="3">
+      <c r="O6" s="17">
         <v>140.79283367556471</v>
       </c>
-      <c r="P6" s="3">
+      <c r="P6" s="17">
         <v>0.91428571428571437</v>
       </c>
       <c r="R6" s="2">
@@ -6532,8 +6583,18 @@
       <c r="Z6" s="3">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="7" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB6" s="2">
+        <f>AB5+1</f>
+        <v>2</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>43.84987582460225</v>
+      </c>
+      <c r="AD6" s="3">
+        <v>110.7233953488372</v>
+      </c>
+    </row>
+    <row r="7" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C7" s="2">
         <f t="shared" ref="C7:C54" si="0">C6+1</f>
         <v>3</v>
@@ -6544,30 +6605,31 @@
       <c r="E7" s="3">
         <v>97.748844862323708</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="16">
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7" s="17">
         <v>32.987240759240763</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7" s="17">
         <v>103.0479712460064</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="17">
         <v>0.87584650112866824</v>
       </c>
-      <c r="M7" s="2">
+      <c r="L7" s="15"/>
+      <c r="M7" s="16">
         <f t="shared" ref="M7:M54" si="2">M6+1</f>
         <v>3</v>
       </c>
-      <c r="N7" s="3">
+      <c r="N7" s="17">
         <v>41.159727786337967</v>
       </c>
-      <c r="O7" s="3">
+      <c r="O7" s="17">
         <v>120.0490349075975</v>
       </c>
-      <c r="P7" s="3">
+      <c r="P7" s="17">
         <v>0.95061728395061729</v>
       </c>
       <c r="R7" s="2">
@@ -6596,8 +6658,18 @@
       <c r="Z7" s="3">
         <v>0.80573248407643294</v>
       </c>
-    </row>
-    <row r="8" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB7" s="2">
+        <f t="shared" ref="AB7:AB54" si="5">AB6+1</f>
+        <v>3</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>43.367605743112136</v>
+      </c>
+      <c r="AD7" s="3">
+        <v>115.12675968992249</v>
+      </c>
+    </row>
+    <row r="8" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C8" s="2">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -6608,30 +6680,31 @@
       <c r="E8" s="3">
         <v>97.348623237071862</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8" s="17">
         <v>32.953482517482513</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8" s="17">
         <v>98.090311501597455</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="17">
         <v>0.8868778280542986</v>
       </c>
-      <c r="M8" s="2">
+      <c r="L8" s="15"/>
+      <c r="M8" s="16">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="N8" s="3">
+      <c r="N8" s="17">
         <v>41.271597329224463</v>
       </c>
-      <c r="O8" s="3">
+      <c r="O8" s="17">
         <v>127.1847022587269</v>
       </c>
-      <c r="P8" s="3">
+      <c r="P8" s="17">
         <v>0.94989979959919846</v>
       </c>
       <c r="R8" s="2">
@@ -6660,8 +6733,18 @@
       <c r="Z8" s="3">
         <v>0.80499219968798741</v>
       </c>
-    </row>
-    <row r="9" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB8" s="2">
+        <f t="shared" si="5"/>
+        <v>4</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>43.189930151338757</v>
+      </c>
+      <c r="AD8" s="3">
+        <v>117.7471937984496</v>
+      </c>
+    </row>
+    <row r="9" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C9" s="2">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -6672,30 +6755,31 @@
       <c r="E9" s="3">
         <v>99.289751511081249</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="16">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9" s="17">
         <v>33.234569430569437</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9" s="17">
         <v>97.241238019169344</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="17">
         <v>0.88888888888888884</v>
       </c>
-      <c r="M9" s="2">
+      <c r="L9" s="15"/>
+      <c r="M9" s="16">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="N9" s="3">
+      <c r="N9" s="17">
         <v>41.256096558808423</v>
       </c>
-      <c r="O9" s="3">
+      <c r="O9" s="17">
         <v>126.5131416837782</v>
       </c>
-      <c r="P9" s="3">
+      <c r="P9" s="17">
         <v>0.94802494802494808</v>
       </c>
       <c r="R9" s="2">
@@ -6724,8 +6808,18 @@
       <c r="Z9" s="3">
         <v>0.76650563607085342</v>
       </c>
-    </row>
-    <row r="10" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB9" s="2">
+        <f t="shared" si="5"/>
+        <v>5</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>43.840911913077207</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>111.750465116279</v>
+      </c>
+    </row>
+    <row r="10" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C10" s="2">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -6736,30 +6830,31 @@
       <c r="E10" s="3">
         <v>93.387716588314291</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="16">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10" s="17">
         <v>32.402823176823183</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10" s="17">
         <v>102.5543849840256</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="17">
         <v>0.8868778280542986</v>
       </c>
-      <c r="M10" s="2">
+      <c r="L10" s="15"/>
+      <c r="M10" s="16">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="N10" s="3">
+      <c r="N10" s="17">
         <v>41.587688751926031</v>
       </c>
-      <c r="O10" s="3">
+      <c r="O10" s="17">
         <v>128.54032854209439</v>
       </c>
-      <c r="P10" s="3">
+      <c r="P10" s="17">
         <v>0.94545454545454544</v>
       </c>
       <c r="R10" s="2">
@@ -6788,8 +6883,18 @@
       <c r="Z10" s="3">
         <v>0.80059084194977848</v>
       </c>
-    </row>
-    <row r="11" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB10" s="2">
+        <f t="shared" si="5"/>
+        <v>6</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>43.716612339930137</v>
+      </c>
+      <c r="AD10" s="3">
+        <v>115.0925891472868</v>
+      </c>
+    </row>
+    <row r="11" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C11" s="2">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -6800,30 +6905,31 @@
       <c r="E11" s="3">
         <v>100.25349227669579</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="16">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11" s="17">
         <v>32.976533466533468</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11" s="17">
         <v>99.219776357827485</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="17">
         <v>0.89578713968957857</v>
       </c>
-      <c r="M11" s="2">
+      <c r="L11" s="15"/>
+      <c r="M11" s="16">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="N11" s="3">
+      <c r="N11" s="17">
         <v>41.25715459681561</v>
       </c>
-      <c r="O11" s="3">
+      <c r="O11" s="17">
         <v>138.1483162217659</v>
       </c>
-      <c r="P11" s="3">
+      <c r="P11" s="17">
         <v>0.93927125506072873</v>
       </c>
       <c r="R11" s="2">
@@ -6852,8 +6958,18 @@
       <c r="Z11" s="3">
         <v>0.80188679245283023</v>
       </c>
-    </row>
-    <row r="12" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB11" s="2">
+        <f t="shared" si="5"/>
+        <v>7</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>43.896332945285216</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>117.8104031007752</v>
+      </c>
+    </row>
+    <row r="12" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C12" s="2">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -6864,30 +6980,31 @@
       <c r="E12" s="3">
         <v>98.036111484217571</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="16">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12" s="17">
         <v>32.838163836163837</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12" s="17">
         <v>101.45865015974439</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="17">
         <v>0.88839285714285721</v>
       </c>
-      <c r="M12" s="2">
+      <c r="L12" s="15"/>
+      <c r="M12" s="16">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="N12" s="3">
+      <c r="N12" s="17">
         <v>40.385418592706728</v>
       </c>
-      <c r="O12" s="3">
+      <c r="O12" s="17">
         <v>144.55636550308009</v>
       </c>
-      <c r="P12" s="3">
+      <c r="P12" s="17">
         <v>0.94523326572008126</v>
       </c>
       <c r="R12" s="2">
@@ -6916,8 +7033,18 @@
       <c r="Z12" s="3">
         <v>0.83911671924290221</v>
       </c>
-    </row>
-    <row r="13" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB12" s="2">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>43.378051998447802</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>121.8953178294574</v>
+      </c>
+    </row>
+    <row r="13" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C13" s="2">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -6928,30 +7055,31 @@
       <c r="E13" s="3">
         <v>98.474016118200126</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="16">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13" s="17">
         <v>33.456141858141862</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13" s="17">
         <v>92.46848242811501</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="17">
         <v>0.92511013215859017</v>
       </c>
-      <c r="M13" s="2">
+      <c r="L13" s="15"/>
+      <c r="M13" s="16">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="N13" s="3">
+      <c r="N13" s="17">
         <v>42.129157678479707</v>
       </c>
-      <c r="O13" s="3">
+      <c r="O13" s="17">
         <v>127.748295687885</v>
       </c>
-      <c r="P13" s="3">
+      <c r="P13" s="17">
         <v>0.93951612903225801</v>
       </c>
       <c r="R13" s="2">
@@ -6980,8 +7108,18 @@
       <c r="Z13" s="3">
         <v>0.79876160990712064</v>
       </c>
-    </row>
-    <row r="14" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB13" s="2">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>43.226383391540551</v>
+      </c>
+      <c r="AD13" s="3">
+        <v>119.88533333333331</v>
+      </c>
+    </row>
+    <row r="14" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C14" s="2">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -6992,30 +7130,31 @@
       <c r="E14" s="3">
         <v>100.2977165883143</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14" s="17">
         <v>33.232537462537472</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14" s="17">
         <v>94.10614217252396</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="17">
         <v>0.88789237668161436</v>
       </c>
-      <c r="M14" s="2">
+      <c r="L14" s="15"/>
+      <c r="M14" s="16">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="N14" s="3">
+      <c r="N14" s="17">
         <v>41.979013867488447</v>
       </c>
-      <c r="O14" s="3">
+      <c r="O14" s="17">
         <v>129.21012320328541</v>
       </c>
-      <c r="P14" s="3">
+      <c r="P14" s="17">
         <v>0.94715447154471533</v>
       </c>
       <c r="R14" s="2">
@@ -7044,8 +7183,18 @@
       <c r="Z14" s="3">
         <v>0.80511182108626211</v>
       </c>
-    </row>
-    <row r="15" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB14" s="2">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>43.931276678308123</v>
+      </c>
+      <c r="AD14" s="3">
+        <v>118.51361240310079</v>
+      </c>
+    </row>
+    <row r="15" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C15" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -7056,30 +7205,31 @@
       <c r="E15" s="3">
         <v>102.08296171927471</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="16">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15" s="17">
         <v>33.096939060939071</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15" s="17">
         <v>98.108650159744414</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="17">
         <v>0.87471526195899763</v>
       </c>
-      <c r="M15" s="2">
+      <c r="L15" s="15"/>
+      <c r="M15" s="16">
         <f t="shared" si="2"/>
         <v>11</v>
       </c>
-      <c r="N15" s="3">
+      <c r="N15" s="17">
         <v>42.531468926553671</v>
       </c>
-      <c r="O15" s="3">
+      <c r="O15" s="17">
         <v>123.785749486653</v>
       </c>
-      <c r="P15" s="3">
+      <c r="P15" s="17">
         <v>0.94589178356713421</v>
       </c>
       <c r="R15" s="2">
@@ -7108,8 +7258,18 @@
       <c r="Z15" s="3">
         <v>0.81470137825421141</v>
       </c>
-    </row>
-    <row r="16" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB15" s="2">
+        <f t="shared" si="5"/>
+        <v>11</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>43.18726038028715</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>119.2350542635659</v>
+      </c>
+    </row>
+    <row r="16" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -7120,30 +7280,31 @@
       <c r="E16" s="3">
         <v>96.635708529214241</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16" s="17">
         <v>32.98412987012987</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16" s="17">
         <v>97.907891373801917</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="17">
         <v>0.89485458612975399</v>
       </c>
-      <c r="M16" s="2">
+      <c r="L16" s="15"/>
+      <c r="M16" s="16">
         <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N16" s="3">
+      <c r="N16" s="17">
         <v>42.618834103749371</v>
       </c>
-      <c r="O16" s="3">
+      <c r="O16" s="17">
         <v>125.76353182751539</v>
       </c>
-      <c r="P16" s="3">
+      <c r="P16" s="17">
         <v>0.93951612903225801</v>
       </c>
       <c r="R16" s="2">
@@ -7172,8 +7333,18 @@
       <c r="Z16" s="3">
         <v>0.79204892966360874</v>
       </c>
-    </row>
-    <row r="17" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB16" s="2">
+        <f t="shared" si="5"/>
+        <v>12</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>43.213519596429947</v>
+      </c>
+      <c r="AD16" s="3">
+        <v>117.029488372093</v>
+      </c>
+    </row>
+    <row r="17" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -7184,30 +7355,31 @@
       <c r="E17" s="3">
         <v>94.58910006715918</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="16">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17" s="17">
         <v>32.950975024975023</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17" s="17">
         <v>101.5547124600639</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="17">
         <v>0.89038031319910516</v>
       </c>
-      <c r="M17" s="2">
+      <c r="L17" s="15"/>
+      <c r="M17" s="16">
         <f t="shared" si="2"/>
         <v>13</v>
       </c>
-      <c r="N17" s="3">
+      <c r="N17" s="17">
         <v>40.913528505392918</v>
       </c>
-      <c r="O17" s="3">
+      <c r="O17" s="17">
         <v>134.98281314168381</v>
       </c>
-      <c r="P17" s="3">
+      <c r="P17" s="17">
         <v>0.9346938775510204</v>
       </c>
       <c r="R17" s="2">
@@ -7236,8 +7408,18 @@
       <c r="Z17" s="3">
         <v>0.79233226837060711</v>
       </c>
-    </row>
-    <row r="18" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB17" s="2">
+        <f t="shared" si="5"/>
+        <v>13</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>43.269957314707007</v>
+      </c>
+      <c r="AD17" s="3">
+        <v>115.0801240310077</v>
+      </c>
+    </row>
+    <row r="18" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -7248,30 +7430,31 @@
       <c r="E18" s="3">
         <v>97.300141034251169</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="16">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18" s="17">
         <v>32.537346653346653</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="17">
         <v>100.5431948881789</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="17">
         <v>0.89438202247191023</v>
       </c>
-      <c r="M18" s="2">
+      <c r="L18" s="15"/>
+      <c r="M18" s="16">
         <f t="shared" si="2"/>
         <v>14</v>
       </c>
-      <c r="N18" s="3">
+      <c r="N18" s="17">
         <v>42.678947098099641</v>
       </c>
-      <c r="O18" s="3">
+      <c r="O18" s="17">
         <v>123.9367761806981</v>
       </c>
-      <c r="P18" s="3">
+      <c r="P18" s="17">
         <v>0.93117408906882582</v>
       </c>
       <c r="R18" s="2">
@@ -7300,8 +7483,18 @@
       <c r="Z18" s="3">
         <v>0.76650563607085342</v>
       </c>
-    </row>
-    <row r="19" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB18" s="2">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>43.404780752813338</v>
+      </c>
+      <c r="AD18" s="3">
+        <v>119.0241550387597</v>
+      </c>
+    </row>
+    <row r="19" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -7312,30 +7505,31 @@
       <c r="E19" s="3">
         <v>94.231511081262582</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="16">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="3">
+      <c r="I19" s="17">
         <v>33.070477522477518</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="17">
         <v>98.380335463258774</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="17">
         <v>0.8977777777777779</v>
       </c>
-      <c r="M19" s="2">
+      <c r="L19" s="15"/>
+      <c r="M19" s="16">
         <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="N19" s="3">
+      <c r="N19" s="17">
         <v>42.005788392398571</v>
       </c>
-      <c r="O19" s="3">
+      <c r="O19" s="17">
         <v>123.8722381930185</v>
       </c>
-      <c r="P19" s="3">
+      <c r="P19" s="17">
         <v>0.95757575757575741</v>
       </c>
       <c r="R19" s="2">
@@ -7364,8 +7558,18 @@
       <c r="Z19" s="3">
         <v>0.80547112462006076</v>
       </c>
-    </row>
-    <row r="20" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB19" s="2">
+        <f t="shared" si="5"/>
+        <v>15</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>43.039433449747762</v>
+      </c>
+      <c r="AD19" s="3">
+        <v>119.8191782945736</v>
+      </c>
+    </row>
+    <row r="20" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -7376,30 +7580,31 @@
       <c r="E20" s="3">
         <v>103.1834654130289</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="16">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="3">
+      <c r="I20" s="17">
         <v>32.74853746253747</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="17">
         <v>101.4435862619808</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="17">
         <v>0.89342403628117906</v>
       </c>
-      <c r="M20" s="2">
+      <c r="L20" s="15"/>
+      <c r="M20" s="16">
         <f t="shared" si="2"/>
         <v>16</v>
       </c>
-      <c r="N20" s="3">
+      <c r="N20" s="17">
         <v>43.04824858757064</v>
       </c>
-      <c r="O20" s="3">
+      <c r="O20" s="17">
         <v>119.2666119096509</v>
       </c>
-      <c r="P20" s="3">
+      <c r="P20" s="17">
         <v>0.94969818913480886</v>
       </c>
       <c r="R20" s="2">
@@ -7428,8 +7633,18 @@
       <c r="Z20" s="3">
         <v>0.79937304075235105</v>
       </c>
-    </row>
-    <row r="21" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB20" s="2">
+        <f t="shared" si="5"/>
+        <v>16</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>43.959666278618542</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>112.06438759689919</v>
+      </c>
+    </row>
+    <row r="21" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -7440,30 +7655,31 @@
       <c r="E21" s="3">
         <v>93.387662860980527</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="16">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="3">
+      <c r="I21" s="17">
         <v>33.202831168831167</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="17">
         <v>94.081845047923323</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="17">
         <v>0.92035398230088494</v>
       </c>
-      <c r="M21" s="2">
+      <c r="L21" s="15"/>
+      <c r="M21" s="16">
         <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="N21" s="3">
+      <c r="N21" s="17">
         <v>42.926764252696458</v>
       </c>
-      <c r="O21" s="3">
+      <c r="O21" s="17">
         <v>116.6773716632443</v>
       </c>
-      <c r="P21" s="3">
+      <c r="P21" s="17">
         <v>0.94069529652351735</v>
       </c>
       <c r="R21" s="2">
@@ -7492,8 +7708,18 @@
       <c r="Z21" s="3">
         <v>0.7846153846153846</v>
       </c>
-    </row>
-    <row r="22" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB21" s="2">
+        <f t="shared" si="5"/>
+        <v>17</v>
+      </c>
+      <c r="AC21" s="3">
+        <v>43.204454792394252</v>
+      </c>
+      <c r="AD21" s="3">
+        <v>121.6349612403101</v>
+      </c>
+    </row>
+    <row r="22" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -7504,30 +7730,31 @@
       <c r="E22" s="3">
         <v>96.045970449966404</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="16">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I22" s="17">
         <v>32.722725274725278</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="17">
         <v>98.050199680511184</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="17">
         <v>0.92273730684326716</v>
       </c>
-      <c r="M22" s="2">
+      <c r="L22" s="15"/>
+      <c r="M22" s="16">
         <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N22" s="17">
         <v>40.889239856189008</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O22" s="17">
         <v>121.5879876796715</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P22" s="17">
         <v>0.94455852156057496</v>
       </c>
       <c r="R22" s="2">
@@ -7556,8 +7783,18 @@
       <c r="Z22" s="3">
         <v>0.79320987654320985</v>
       </c>
-    </row>
-    <row r="23" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB22" s="2">
+        <f t="shared" si="5"/>
+        <v>18</v>
+      </c>
+      <c r="AC22" s="3">
+        <v>42.760159099728369</v>
+      </c>
+      <c r="AD22" s="3">
+        <v>122.0356124031008</v>
+      </c>
+    </row>
+    <row r="23" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -7568,30 +7805,31 @@
       <c r="E23" s="3">
         <v>99.390738750839489</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="16">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I23" s="17">
         <v>33.003242757242766</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="17">
         <v>100.010231629393</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="17">
         <v>0.88435374149659862</v>
       </c>
-      <c r="M23" s="2">
+      <c r="L23" s="15"/>
+      <c r="M23" s="16">
         <f t="shared" si="2"/>
         <v>19</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N23" s="17">
         <v>40.596774524910117</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O23" s="17">
         <v>128.23845995893231</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P23" s="17">
         <v>0.96341463414634143</v>
       </c>
       <c r="R23" s="2">
@@ -7620,8 +7858,18 @@
       <c r="Z23" s="3">
         <v>0.79315707620528775</v>
       </c>
-    </row>
-    <row r="24" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB23" s="2">
+        <f t="shared" si="5"/>
+        <v>19</v>
+      </c>
+      <c r="AC23" s="3">
+        <v>43.424823438106323</v>
+      </c>
+      <c r="AD23" s="3">
+        <v>120.2225271317829</v>
+      </c>
+    </row>
+    <row r="24" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -7632,30 +7880,31 @@
       <c r="E24" s="3">
         <v>96.450214909335131</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="16">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="3">
+      <c r="I24" s="17">
         <v>32.781428571428577</v>
       </c>
-      <c r="J24" s="3">
+      <c r="J24" s="17">
         <v>98.881477635782744</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="17">
         <v>0.89485458612975399</v>
       </c>
-      <c r="M24" s="2">
+      <c r="L24" s="15"/>
+      <c r="M24" s="16">
         <f t="shared" si="2"/>
         <v>20</v>
       </c>
-      <c r="N24" s="3">
+      <c r="N24" s="17">
         <v>41.862013353877757</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="17">
         <v>124.09642710472281</v>
       </c>
-      <c r="P24" s="3">
+      <c r="P24" s="17">
         <v>0.93574297188755018</v>
       </c>
       <c r="R24" s="2">
@@ -7684,8 +7933,18 @@
       <c r="Z24" s="3">
         <v>0.73817034700315465</v>
       </c>
-    </row>
-    <row r="25" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB24" s="2">
+        <f t="shared" si="5"/>
+        <v>20</v>
+      </c>
+      <c r="AC24" s="3">
+        <v>43.703779588668993</v>
+      </c>
+      <c r="AD24" s="3">
+        <v>113.2233953488372</v>
+      </c>
+    </row>
+    <row r="25" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -7696,30 +7955,31 @@
       <c r="E25" s="3">
         <v>98.2770920080591</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="16">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="3">
+      <c r="I25" s="17">
         <v>33.32564035964036</v>
       </c>
-      <c r="J25" s="3">
+      <c r="J25" s="17">
         <v>97.871749201277964</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="17">
         <v>0.89887640449438211</v>
       </c>
-      <c r="M25" s="2">
+      <c r="L25" s="15"/>
+      <c r="M25" s="16">
         <f t="shared" si="2"/>
         <v>21</v>
       </c>
-      <c r="N25" s="3">
+      <c r="N25" s="17">
         <v>41.111782229070371</v>
       </c>
-      <c r="O25" s="3">
+      <c r="O25" s="17">
         <v>142.38030800821349</v>
       </c>
-      <c r="P25" s="3">
+      <c r="P25" s="17">
         <v>0.94331983805668007</v>
       </c>
       <c r="R25" s="2">
@@ -7748,8 +8008,18 @@
       <c r="Z25" s="3">
         <v>0.77708978328173373</v>
       </c>
-    </row>
-    <row r="26" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB25" s="2">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AC25" s="3">
+        <v>44.456162204113298</v>
+      </c>
+      <c r="AD25" s="3">
+        <v>113.77570542635659</v>
+      </c>
+    </row>
+    <row r="26" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -7760,30 +8030,31 @@
       <c r="E26" s="3">
         <v>97.128663532572176</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="16">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="3">
+      <c r="I26" s="17">
         <v>33.334709290709299</v>
       </c>
-      <c r="J26" s="3">
+      <c r="J26" s="17">
         <v>97.190958466453694</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="17">
         <v>0.89086859688195996</v>
       </c>
-      <c r="M26" s="2">
+      <c r="L26" s="15"/>
+      <c r="M26" s="16">
         <f t="shared" si="2"/>
         <v>22</v>
       </c>
-      <c r="N26" s="3">
+      <c r="N26" s="17">
         <v>41.633872624550598</v>
       </c>
-      <c r="O26" s="3">
+      <c r="O26" s="17">
         <v>118.5770431211499</v>
       </c>
-      <c r="P26" s="3">
+      <c r="P26" s="17">
         <v>0.95918367346938771</v>
       </c>
       <c r="R26" s="2">
@@ -7812,8 +8083,18 @@
       <c r="Z26" s="3">
         <v>0.81942336874051602</v>
       </c>
-    </row>
-    <row r="27" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB26" s="2">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="AC26" s="3">
+        <v>43.454850601474583</v>
+      </c>
+      <c r="AD26" s="3">
+        <v>115.80220155038759</v>
+      </c>
+    </row>
+    <row r="27" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -7824,30 +8105,31 @@
       <c r="E27" s="3">
         <v>96.354936198791123</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="16">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="3">
+      <c r="I27" s="17">
         <v>32.539228771228778</v>
       </c>
-      <c r="J27" s="3">
+      <c r="J27" s="17">
         <v>103.5235303514377</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="17">
         <v>0.91228070175438603</v>
       </c>
-      <c r="M27" s="2">
+      <c r="L27" s="15"/>
+      <c r="M27" s="16">
         <f t="shared" si="2"/>
         <v>23</v>
       </c>
-      <c r="N27" s="3">
+      <c r="N27" s="17">
         <v>41.263841807909607</v>
       </c>
-      <c r="O27" s="3">
+      <c r="O27" s="17">
         <v>132.73271047227931</v>
       </c>
-      <c r="P27" s="3">
+      <c r="P27" s="17">
         <v>0.93522267206477738</v>
       </c>
       <c r="R27" s="2">
@@ -7876,8 +8158,18 @@
       <c r="Z27" s="3">
         <v>0.78437500000000004</v>
       </c>
-    </row>
-    <row r="28" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB27" s="2">
+        <f t="shared" si="5"/>
+        <v>23</v>
+      </c>
+      <c r="AC27" s="3">
+        <v>44.039689561505618</v>
+      </c>
+      <c r="AD27" s="3">
+        <v>112.85266666666671</v>
+      </c>
+    </row>
+    <row r="28" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -7888,30 +8180,31 @@
       <c r="E28" s="3">
         <v>98.824002686366683</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="16">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="3">
+      <c r="I28" s="17">
         <v>32.904427572427579</v>
       </c>
-      <c r="J28" s="3">
+      <c r="J28" s="17">
         <v>101.8725559105431</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="17">
         <v>0.92070484581497791</v>
       </c>
-      <c r="M28" s="2">
+      <c r="L28" s="15"/>
+      <c r="M28" s="16">
         <f t="shared" si="2"/>
         <v>24</v>
       </c>
-      <c r="N28" s="3">
+      <c r="N28" s="17">
         <v>42.816718027734971</v>
       </c>
-      <c r="O28" s="3">
+      <c r="O28" s="17">
         <v>114.35016427104721</v>
       </c>
-      <c r="P28" s="3">
+      <c r="P28" s="17">
         <v>0.96523517382413082</v>
       </c>
       <c r="R28" s="2">
@@ -7940,8 +8233,18 @@
       <c r="Z28" s="3">
         <v>0.79384615384615387</v>
       </c>
-    </row>
-    <row r="29" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB28" s="2">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="AC28" s="3">
+        <v>43.756682188591377</v>
+      </c>
+      <c r="AD28" s="3">
+        <v>112.72755038759691</v>
+      </c>
+    </row>
+    <row r="29" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -7952,30 +8255,31 @@
       <c r="E29" s="3">
         <v>99.533089321692415</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="16">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="3">
+      <c r="I29" s="17">
         <v>32.49418781218781</v>
       </c>
-      <c r="J29" s="3">
+      <c r="J29" s="17">
         <v>98.991845047923334</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="17">
         <v>0.90507726269315669</v>
       </c>
-      <c r="M29" s="2">
+      <c r="L29" s="15"/>
+      <c r="M29" s="16">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N29" s="3">
+      <c r="N29" s="17">
         <v>41.201273754494103</v>
       </c>
-      <c r="O29" s="3">
+      <c r="O29" s="17">
         <v>138.04139630390139</v>
       </c>
-      <c r="P29" s="3">
+      <c r="P29" s="17">
         <v>0.93413173652694603</v>
       </c>
       <c r="R29" s="2">
@@ -8004,8 +8308,18 @@
       <c r="Z29" s="3">
         <v>0.80181543116490184</v>
       </c>
-    </row>
-    <row r="30" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB29" s="2">
+        <f t="shared" si="5"/>
+        <v>25</v>
+      </c>
+      <c r="AC29" s="3">
+        <v>43.747481567714402</v>
+      </c>
+      <c r="AD29" s="3">
+        <v>115.1509612403101</v>
+      </c>
+    </row>
+    <row r="30" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -8016,30 +8330,31 @@
       <c r="E30" s="3">
         <v>95.2527333781061</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="16">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="3">
+      <c r="I30" s="17">
         <v>32.954037962037972</v>
       </c>
-      <c r="J30" s="3">
+      <c r="J30" s="17">
         <v>98.983562300319505</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="17">
         <v>0.90549450549450561</v>
       </c>
-      <c r="M30" s="2">
+      <c r="L30" s="15"/>
+      <c r="M30" s="16">
         <f t="shared" si="2"/>
         <v>26</v>
       </c>
-      <c r="N30" s="3">
+      <c r="N30" s="17">
         <v>41.556938880328723</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O30" s="17">
         <v>117.37650924024641</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P30" s="17">
         <v>0.95918367346938771</v>
       </c>
       <c r="R30" s="2">
@@ -8068,8 +8383,18 @@
       <c r="Z30" s="3">
         <v>0.78627145085803429</v>
       </c>
-    </row>
-    <row r="31" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB30" s="2">
+        <f t="shared" si="5"/>
+        <v>26</v>
+      </c>
+      <c r="AC30" s="3">
+        <v>43.459840900271629</v>
+      </c>
+      <c r="AD30" s="3">
+        <v>122.9879069767442</v>
+      </c>
+    </row>
+    <row r="31" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -8080,30 +8405,31 @@
       <c r="E31" s="3">
         <v>94.601356615177977</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="16">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="3">
+      <c r="I31" s="17">
         <v>33.336481518481527</v>
       </c>
-      <c r="J31" s="3">
+      <c r="J31" s="17">
         <v>94.506948881789143</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="17">
         <v>0.91067538126361647</v>
       </c>
-      <c r="M31" s="2">
+      <c r="L31" s="15"/>
+      <c r="M31" s="16">
         <f t="shared" si="2"/>
         <v>27</v>
       </c>
-      <c r="N31" s="3">
+      <c r="N31" s="17">
         <v>41.975326142783778</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O31" s="17">
         <v>135.25613963039021</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P31" s="17">
         <v>0.93951612903225801</v>
       </c>
       <c r="R31" s="2">
@@ -8132,8 +8458,18 @@
       <c r="Z31" s="3">
         <v>0.80798771121351765</v>
       </c>
-    </row>
-    <row r="32" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB31" s="2">
+        <f t="shared" si="5"/>
+        <v>27</v>
+      </c>
+      <c r="AC31" s="3">
+        <v>43.291105937136187</v>
+      </c>
+      <c r="AD31" s="3">
+        <v>118.3451007751938</v>
+      </c>
+    </row>
+    <row r="32" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -8144,30 +8480,31 @@
       <c r="E32" s="3">
         <v>100.1417058428475</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="16">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="3">
+      <c r="I32" s="17">
         <v>33.27616183816184</v>
       </c>
-      <c r="J32" s="3">
+      <c r="J32" s="17">
         <v>96.509137380191689</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="17">
         <v>0.90337078651685387</v>
       </c>
-      <c r="M32" s="2">
+      <c r="L32" s="15"/>
+      <c r="M32" s="16">
         <f t="shared" si="2"/>
         <v>28</v>
       </c>
-      <c r="N32" s="3">
+      <c r="N32" s="17">
         <v>42.798166409861317</v>
       </c>
-      <c r="O32" s="3">
+      <c r="O32" s="17">
         <v>133.03772073921971</v>
       </c>
-      <c r="P32" s="3">
+      <c r="P32" s="17">
         <v>0.93861386138613856</v>
       </c>
       <c r="R32" s="2">
@@ -8196,8 +8533,18 @@
       <c r="Z32" s="3">
         <v>0.81860465116279069</v>
       </c>
-    </row>
-    <row r="33" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB32" s="2">
+        <f t="shared" si="5"/>
+        <v>28</v>
+      </c>
+      <c r="AC32" s="3">
+        <v>43.491470702367089</v>
+      </c>
+      <c r="AD32" s="3">
+        <v>114.3388837209302</v>
+      </c>
+    </row>
+    <row r="33" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -8208,30 +8555,31 @@
       <c r="E33" s="3">
         <v>94.03676292813968</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="16">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="3">
+      <c r="I33" s="17">
         <v>32.751874125874131</v>
       </c>
-      <c r="J33" s="3">
+      <c r="J33" s="17">
         <v>97.30373801916933</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="17">
         <v>0.91352549889135259</v>
       </c>
-      <c r="M33" s="2">
+      <c r="L33" s="15"/>
+      <c r="M33" s="16">
         <f t="shared" si="2"/>
         <v>29</v>
       </c>
-      <c r="N33" s="3">
+      <c r="N33" s="17">
         <v>40.75311248073961</v>
       </c>
-      <c r="O33" s="3">
+      <c r="O33" s="17">
         <v>131.2003080082136</v>
       </c>
-      <c r="P33" s="3">
+      <c r="P33" s="17">
         <v>0.95934959349593507</v>
       </c>
       <c r="R33" s="2">
@@ -8260,8 +8608,18 @@
       <c r="Z33" s="3">
         <v>0.82170542635658927</v>
       </c>
-    </row>
-    <row r="34" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB33" s="2">
+        <f t="shared" si="5"/>
+        <v>29</v>
+      </c>
+      <c r="AC33" s="3">
+        <v>43.60195964299573</v>
+      </c>
+      <c r="AD33" s="3">
+        <v>123.07263565891471</v>
+      </c>
+    </row>
+    <row r="34" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -8272,30 +8630,31 @@
       <c r="E34" s="3">
         <v>97.004472800537258</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="16">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="3">
+      <c r="I34" s="17">
         <v>32.983588411588421</v>
       </c>
-      <c r="J34" s="3">
+      <c r="J34" s="17">
         <v>96.090806709265181</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="17">
         <v>0.93216630196936545</v>
       </c>
-      <c r="M34" s="2">
+      <c r="L34" s="15"/>
+      <c r="M34" s="16">
         <f t="shared" si="2"/>
         <v>30</v>
       </c>
-      <c r="N34" s="3">
+      <c r="N34" s="17">
         <v>42.050441705187481</v>
       </c>
-      <c r="O34" s="3">
+      <c r="O34" s="17">
         <v>124.8905133470226</v>
       </c>
-      <c r="P34" s="3">
+      <c r="P34" s="17">
         <v>0.94610778443113763</v>
       </c>
       <c r="R34" s="2">
@@ -8324,8 +8683,18 @@
       <c r="Z34" s="3">
         <v>0.78063540090771555</v>
       </c>
-    </row>
-    <row r="35" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB34" s="2">
+        <f t="shared" si="5"/>
+        <v>30</v>
+      </c>
+      <c r="AC34" s="3">
+        <v>43.665242530073733</v>
+      </c>
+      <c r="AD34" s="3">
+        <v>112.6728682170542</v>
+      </c>
+    </row>
+    <row r="35" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -8336,30 +8705,31 @@
       <c r="E35" s="3">
         <v>93.270080591000664</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="16">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="3">
+      <c r="I35" s="17">
         <v>33.325026973026979</v>
       </c>
-      <c r="J35" s="3">
+      <c r="J35" s="17">
         <v>95.702140575079866</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="17">
         <v>0.89333333333333331</v>
       </c>
-      <c r="M35" s="2">
+      <c r="L35" s="15"/>
+      <c r="M35" s="16">
         <f t="shared" si="2"/>
         <v>31</v>
       </c>
-      <c r="N35" s="3">
+      <c r="N35" s="17">
         <v>40.980287621982527</v>
       </c>
-      <c r="O35" s="3">
+      <c r="O35" s="17">
         <v>137.59281314168371</v>
       </c>
-      <c r="P35" s="3">
+      <c r="P35" s="17">
         <v>0.93117408906882582</v>
       </c>
       <c r="R35" s="2">
@@ -8388,8 +8758,18 @@
       <c r="Z35" s="3">
         <v>0.77725118483412325</v>
       </c>
-    </row>
-    <row r="36" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB35" s="2">
+        <f t="shared" si="5"/>
+        <v>31</v>
+      </c>
+      <c r="AC35" s="3">
+        <v>43.876208769887469</v>
+      </c>
+      <c r="AD35" s="3">
+        <v>114.46843410852711</v>
+      </c>
+    </row>
+    <row r="36" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -8400,30 +8780,31 @@
       <c r="E36" s="3">
         <v>97.239603760913383</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="16">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="3">
+      <c r="I36" s="17">
         <v>32.57156843156843</v>
       </c>
-      <c r="J36" s="3">
+      <c r="J36" s="17">
         <v>99.028178913738017</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="17">
         <v>0.92139737991266379</v>
       </c>
-      <c r="M36" s="2">
+      <c r="L36" s="15"/>
+      <c r="M36" s="16">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="N36" s="3">
+      <c r="N36" s="17">
         <v>41.587170005136123</v>
       </c>
-      <c r="O36" s="3">
+      <c r="O36" s="17">
         <v>128.49227926078029</v>
       </c>
-      <c r="P36" s="3">
+      <c r="P36" s="17">
         <v>0.95353535353535357</v>
       </c>
       <c r="R36" s="2">
@@ -8452,8 +8833,18 @@
       <c r="Z36" s="3">
         <v>0.78603945371775419</v>
       </c>
-    </row>
-    <row r="37" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB36" s="2">
+        <f t="shared" si="5"/>
+        <v>32</v>
+      </c>
+      <c r="AC36" s="3">
+        <v>44.118727202173083</v>
+      </c>
+      <c r="AD36" s="3">
+        <v>112.714511627907</v>
+      </c>
+    </row>
+    <row r="37" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -8464,30 +8855,31 @@
       <c r="E37" s="3">
         <v>99.326984553391526</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="16">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="3">
+      <c r="I37" s="17">
         <v>32.763496503496512</v>
       </c>
-      <c r="J37" s="3">
+      <c r="J37" s="17">
         <v>101.5051837060703</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="17">
         <v>0.90868596881959918</v>
       </c>
-      <c r="M37" s="2">
+      <c r="L37" s="15"/>
+      <c r="M37" s="16">
         <f t="shared" si="2"/>
         <v>33</v>
       </c>
-      <c r="N37" s="3">
+      <c r="N37" s="17">
         <v>41.16887005649717</v>
       </c>
-      <c r="O37" s="3">
+      <c r="O37" s="17">
         <v>138.46248459958929</v>
       </c>
-      <c r="P37" s="3">
+      <c r="P37" s="17">
         <v>0.94523326572008126</v>
       </c>
       <c r="R37" s="2">
@@ -8516,8 +8908,18 @@
       <c r="Z37" s="3">
         <v>0.82949308755760376</v>
       </c>
-    </row>
-    <row r="38" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB37" s="2">
+        <f t="shared" si="5"/>
+        <v>33</v>
+      </c>
+      <c r="AC37" s="3">
+        <v>44.330349243306173</v>
+      </c>
+      <c r="AD37" s="3">
+        <v>111.1287751937984</v>
+      </c>
+    </row>
+    <row r="38" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -8528,30 +8930,31 @@
       <c r="E38" s="3">
         <v>103.0932505036937</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="16">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="3">
+      <c r="I38" s="17">
         <v>32.818027972027977</v>
       </c>
-      <c r="J38" s="3">
+      <c r="J38" s="17">
         <v>103.6220207667732</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="17">
         <v>0.87782805429864241</v>
       </c>
-      <c r="M38" s="2">
+      <c r="L38" s="15"/>
+      <c r="M38" s="16">
         <f t="shared" si="2"/>
         <v>34</v>
       </c>
-      <c r="N38" s="3">
+      <c r="N38" s="17">
         <v>40.397960965588091</v>
       </c>
-      <c r="O38" s="3">
+      <c r="O38" s="17">
         <v>128.31375770020529</v>
       </c>
-      <c r="P38" s="3">
+      <c r="P38" s="17">
         <v>0.95315682281059055</v>
       </c>
       <c r="R38" s="2">
@@ -8580,8 +8983,18 @@
       <c r="Z38" s="3">
         <v>0.79034690799396667</v>
       </c>
-    </row>
-    <row r="39" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB38" s="2">
+        <f t="shared" si="5"/>
+        <v>34</v>
+      </c>
+      <c r="AC38" s="3">
+        <v>43.668909584788508</v>
+      </c>
+      <c r="AD38" s="3">
+        <v>115.9584186046511</v>
+      </c>
+    </row>
+    <row r="39" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -8592,30 +9005,31 @@
       <c r="E39" s="3">
         <v>101.5870718603089</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="16">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="3">
+      <c r="I39" s="17">
         <v>32.714747252747259</v>
       </c>
-      <c r="J39" s="3">
+      <c r="J39" s="17">
         <v>99.725543130990417</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="17">
         <v>0.84834123222748814</v>
       </c>
-      <c r="M39" s="2">
+      <c r="L39" s="15"/>
+      <c r="M39" s="16">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
-      <c r="N39" s="3">
+      <c r="N39" s="17">
         <v>41.34043656908063</v>
       </c>
-      <c r="O39" s="3">
+      <c r="O39" s="17">
         <v>129.10381930184801</v>
       </c>
-      <c r="P39" s="3">
+      <c r="P39" s="17">
         <v>0.94262295081967218</v>
       </c>
       <c r="R39" s="2">
@@ -8644,8 +9058,18 @@
       <c r="Z39" s="3">
         <v>0.81957186544342508</v>
       </c>
-    </row>
-    <row r="40" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB39" s="2">
+        <f t="shared" si="5"/>
+        <v>35</v>
+      </c>
+      <c r="AC39" s="3">
+        <v>43.896313542879312</v>
+      </c>
+      <c r="AD39" s="3">
+        <v>115.75125581395351</v>
+      </c>
+    </row>
+    <row r="40" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -8656,30 +9080,31 @@
       <c r="E40" s="3">
         <v>97.55313633310945</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="16">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="3">
+      <c r="I40" s="17">
         <v>33.602579420579417</v>
       </c>
-      <c r="J40" s="3">
+      <c r="J40" s="17">
         <v>95.860183706070274</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="17">
         <v>0.87356321839080464</v>
       </c>
-      <c r="M40" s="2">
+      <c r="L40" s="15"/>
+      <c r="M40" s="16">
         <f t="shared" si="2"/>
         <v>36</v>
       </c>
-      <c r="N40" s="3">
+      <c r="N40" s="17">
         <v>42.403122752953259</v>
       </c>
-      <c r="O40" s="3">
+      <c r="O40" s="17">
         <v>123.6347843942505</v>
       </c>
-      <c r="P40" s="3">
+      <c r="P40" s="17">
         <v>0.95218295218295224</v>
       </c>
       <c r="R40" s="2">
@@ -8708,8 +9133,18 @@
       <c r="Z40" s="3">
         <v>0.76774193548387093</v>
       </c>
-    </row>
-    <row r="41" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB40" s="2">
+        <f t="shared" si="5"/>
+        <v>36</v>
+      </c>
+      <c r="AC40" s="3">
+        <v>43.502180830422972</v>
+      </c>
+      <c r="AD40" s="3">
+        <v>114.5008062015504</v>
+      </c>
+    </row>
+    <row r="41" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -8720,30 +9155,31 @@
       <c r="E41" s="3">
         <v>96.219798522498323</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="16">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="3">
+      <c r="I41" s="17">
         <v>33.294163836163847</v>
       </c>
-      <c r="J41" s="3">
+      <c r="J41" s="17">
         <v>96.13136581469648</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="17">
         <v>0.89624724061810157</v>
       </c>
-      <c r="M41" s="2">
+      <c r="L41" s="15"/>
+      <c r="M41" s="16">
         <f t="shared" si="2"/>
         <v>37</v>
       </c>
-      <c r="N41" s="3">
+      <c r="N41" s="17">
         <v>41.890580380071917</v>
       </c>
-      <c r="O41" s="3">
+      <c r="O41" s="17">
         <v>127.6810882956879</v>
       </c>
-      <c r="P41" s="3">
+      <c r="P41" s="17">
         <v>0.95774647887323949</v>
       </c>
       <c r="R41" s="2">
@@ -8772,8 +9208,18 @@
       <c r="Z41" s="3">
         <v>0.77429467084639492</v>
       </c>
-    </row>
-    <row r="42" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB41" s="2">
+        <f t="shared" si="5"/>
+        <v>37</v>
+      </c>
+      <c r="AC41" s="3">
+        <v>44.126612339930148</v>
+      </c>
+      <c r="AD41" s="3">
+        <v>113.9693023255814</v>
+      </c>
+    </row>
+    <row r="42" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -8784,30 +9230,31 @@
       <c r="E42" s="3">
         <v>97.743116185359298</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="16">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="3">
+      <c r="I42" s="17">
         <v>32.968829170829167</v>
       </c>
-      <c r="J42" s="3">
+      <c r="J42" s="17">
         <v>99.858905750798712</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="17">
         <v>0.87238979118329474</v>
       </c>
-      <c r="M42" s="2">
+      <c r="L42" s="15"/>
+      <c r="M42" s="16">
         <f t="shared" si="2"/>
         <v>38</v>
       </c>
-      <c r="N42" s="3">
+      <c r="N42" s="17">
         <v>42.025300462249618</v>
       </c>
-      <c r="O42" s="3">
+      <c r="O42" s="17">
         <v>125.90275154004109</v>
       </c>
-      <c r="P42" s="3">
+      <c r="P42" s="17">
         <v>0.9508196721311476</v>
       </c>
       <c r="R42" s="2">
@@ -8836,8 +9283,18 @@
       <c r="Z42" s="3">
         <v>0.80124223602484479</v>
       </c>
-    </row>
-    <row r="43" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB42" s="2">
+        <f t="shared" si="5"/>
+        <v>38</v>
+      </c>
+      <c r="AC42" s="3">
+        <v>43.355358944509113</v>
+      </c>
+      <c r="AD42" s="3">
+        <v>119.3431627906976</v>
+      </c>
+    </row>
+    <row r="43" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -8848,30 +9305,31 @@
       <c r="E43" s="3">
         <v>97.416400268636664</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="16">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="3">
+      <c r="I43" s="17">
         <v>32.843600399600398</v>
       </c>
-      <c r="J43" s="3">
+      <c r="J43" s="17">
         <v>98.517675718849844</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="17">
         <v>0.9002217294900221</v>
       </c>
-      <c r="M43" s="2">
+      <c r="L43" s="15"/>
+      <c r="M43" s="16">
         <f t="shared" si="2"/>
         <v>39</v>
       </c>
-      <c r="N43" s="3">
+      <c r="N43" s="17">
         <v>41.613790446841293</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O43" s="17">
         <v>121.5146406570842</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P43" s="17">
         <v>0.95121951219512191</v>
       </c>
       <c r="R43" s="2">
@@ -8900,8 +9358,18 @@
       <c r="Z43" s="3">
         <v>0.77672955974842761</v>
       </c>
-    </row>
-    <row r="44" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB43" s="2">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+      <c r="AC43" s="3">
+        <v>43.784695382227397</v>
+      </c>
+      <c r="AD43" s="3">
+        <v>113.6342015503876</v>
+      </c>
+    </row>
+    <row r="44" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -8912,30 +9380,31 @@
       <c r="E44" s="3">
         <v>98.837897918065821</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="16">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="3">
+      <c r="I44" s="17">
         <v>33.127262737262747</v>
       </c>
-      <c r="J44" s="3">
+      <c r="J44" s="17">
         <v>96.81063897763579</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="17">
         <v>0.91739130434782612</v>
       </c>
-      <c r="M44" s="2">
+      <c r="L44" s="15"/>
+      <c r="M44" s="16">
         <f t="shared" si="2"/>
         <v>40</v>
       </c>
-      <c r="N44" s="3">
+      <c r="N44" s="17">
         <v>40.634268104776588</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O44" s="17">
         <v>132.80765913757699</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P44" s="17">
         <v>0.946938775510204</v>
       </c>
       <c r="R44" s="2">
@@ -8964,8 +9433,18 @@
       <c r="Z44" s="3">
         <v>0.77588871715610508</v>
       </c>
-    </row>
-    <row r="45" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB44" s="2">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="AC44" s="3">
+        <v>44.737163368257669</v>
+      </c>
+      <c r="AD44" s="3">
+        <v>109.4500620155038</v>
+      </c>
+    </row>
+    <row r="45" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -8976,30 +9455,31 @@
       <c r="E45" s="3">
         <v>100.5845466756212</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="16">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="3">
+      <c r="I45" s="17">
         <v>32.614643356643363</v>
       </c>
-      <c r="J45" s="3">
+      <c r="J45" s="17">
         <v>100.4078833865815</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="17">
         <v>0.89887640449438211</v>
       </c>
-      <c r="M45" s="2">
+      <c r="L45" s="15"/>
+      <c r="M45" s="16">
         <f t="shared" si="2"/>
         <v>41</v>
       </c>
-      <c r="N45" s="3">
+      <c r="N45" s="17">
         <v>41.54017976373909</v>
       </c>
-      <c r="O45" s="3">
+      <c r="O45" s="17">
         <v>131.01845995893231</v>
       </c>
-      <c r="P45" s="3">
+      <c r="P45" s="17">
         <v>0.94628099173553715</v>
       </c>
       <c r="R45" s="2">
@@ -9028,8 +9508,18 @@
       <c r="Z45" s="3">
         <v>0.79375000000000007</v>
       </c>
-    </row>
-    <row r="46" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB45" s="2">
+        <f t="shared" si="5"/>
+        <v>41</v>
+      </c>
+      <c r="AC45" s="3">
+        <v>43.968172293364361</v>
+      </c>
+      <c r="AD45" s="3">
+        <v>111.95638759689921</v>
+      </c>
+    </row>
+    <row r="46" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -9040,30 +9530,31 @@
       <c r="E46" s="3">
         <v>101.0010611148422</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="16">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="3">
+      <c r="I46" s="17">
         <v>33.343020979020977</v>
       </c>
-      <c r="J46" s="3">
+      <c r="J46" s="17">
         <v>94.598490415335462</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="17">
         <v>0.88143176733780759</v>
       </c>
-      <c r="M46" s="2">
+      <c r="L46" s="15"/>
+      <c r="M46" s="16">
         <f t="shared" si="2"/>
         <v>42</v>
       </c>
-      <c r="N46" s="3">
+      <c r="N46" s="17">
         <v>41.595408320493071</v>
       </c>
-      <c r="O46" s="3">
+      <c r="O46" s="17">
         <v>123.5688090349076</v>
       </c>
-      <c r="P46" s="3">
+      <c r="P46" s="17">
         <v>0.95967741935483863</v>
       </c>
       <c r="R46" s="2">
@@ -9092,8 +9583,18 @@
       <c r="Z46" s="3">
         <v>0.80124223602484479</v>
       </c>
-    </row>
-    <row r="47" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB46" s="2">
+        <f t="shared" si="5"/>
+        <v>42</v>
+      </c>
+      <c r="AC46" s="3">
+        <v>43.86357392316647</v>
+      </c>
+      <c r="AD46" s="3">
+        <v>112.93046511627909</v>
+      </c>
+    </row>
+    <row r="47" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -9104,30 +9605,31 @@
       <c r="E47" s="3">
         <v>96.363955674949636</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="16">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="3">
+      <c r="I47" s="17">
         <v>33.083676323676329</v>
       </c>
-      <c r="J47" s="3">
+      <c r="J47" s="17">
         <v>94.647819488817902</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="17">
         <v>0.90582959641255612</v>
       </c>
-      <c r="M47" s="2">
+      <c r="L47" s="15"/>
+      <c r="M47" s="16">
         <f t="shared" si="2"/>
         <v>43</v>
       </c>
-      <c r="N47" s="3">
+      <c r="N47" s="17">
         <v>42.6520544427324</v>
       </c>
-      <c r="O47" s="3">
+      <c r="O47" s="17">
         <v>118.71581108829569</v>
       </c>
-      <c r="P47" s="3">
+      <c r="P47" s="17">
         <v>0.9327902240325866</v>
       </c>
       <c r="R47" s="2">
@@ -9156,8 +9658,18 @@
       <c r="Z47" s="3">
         <v>0.81860465116279069</v>
       </c>
-    </row>
-    <row r="48" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB47" s="2">
+        <f t="shared" si="5"/>
+        <v>43</v>
+      </c>
+      <c r="AC47" s="3">
+        <v>43.395269693441982</v>
+      </c>
+      <c r="AD47" s="3">
+        <v>120.3364496124031</v>
+      </c>
+    </row>
+    <row r="48" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -9168,30 +9680,31 @@
       <c r="E48" s="3">
         <v>96.194110141034244</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="16">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="3">
+      <c r="I48" s="17">
         <v>33.300607392607397</v>
       </c>
-      <c r="J48" s="3">
+      <c r="J48" s="17">
         <v>100.76310702875401</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="17">
         <v>0.88988764044943802</v>
       </c>
-      <c r="M48" s="2">
+      <c r="L48" s="15"/>
+      <c r="M48" s="16">
         <f t="shared" si="2"/>
         <v>44</v>
       </c>
-      <c r="N48" s="3">
+      <c r="N48" s="17">
         <v>41.511818181818178</v>
       </c>
-      <c r="O48" s="3">
+      <c r="O48" s="17">
         <v>109.6266324435318</v>
       </c>
-      <c r="P48" s="3">
+      <c r="P48" s="17">
         <v>0.95599999999999996</v>
       </c>
       <c r="R48" s="2">
@@ -9220,8 +9733,18 @@
       <c r="Z48" s="3">
         <v>0.78806907378335955</v>
       </c>
-    </row>
-    <row r="49" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB48" s="2">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="AC48" s="3">
+        <v>43.773395421032198</v>
+      </c>
+      <c r="AD48" s="3">
+        <v>117.9351472868217</v>
+      </c>
+    </row>
+    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -9232,30 +9755,31 @@
       <c r="E49" s="3">
         <v>96.968206850235063</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="16">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="3">
+      <c r="I49" s="17">
         <v>32.674797202797208</v>
       </c>
-      <c r="J49" s="3">
+      <c r="J49" s="17">
         <v>101.4149361022364</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="17">
         <v>0.89624724061810157</v>
       </c>
-      <c r="M49" s="2">
+      <c r="L49" s="15"/>
+      <c r="M49" s="16">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
-      <c r="N49" s="3">
+      <c r="N49" s="17">
         <v>42.097252182845423</v>
       </c>
-      <c r="O49" s="3">
+      <c r="O49" s="17">
         <v>142.9811088295688</v>
       </c>
-      <c r="P49" s="3">
+      <c r="P49" s="17">
         <v>0.93253968253968256</v>
       </c>
       <c r="R49" s="2">
@@ -9284,8 +9808,18 @@
       <c r="Z49" s="3">
         <v>0.79620853080568721</v>
       </c>
-    </row>
-    <row r="50" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB49" s="2">
+        <f t="shared" si="5"/>
+        <v>45</v>
+      </c>
+      <c r="AC49" s="3">
+        <v>42.605254171517267</v>
+      </c>
+      <c r="AD49" s="3">
+        <v>125.3234573643411</v>
+      </c>
+    </row>
+    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -9296,30 +9830,31 @@
       <c r="E50" s="3">
         <v>95.112108797850908</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="16">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="3">
+      <c r="I50" s="17">
         <v>33.339466533466542</v>
       </c>
-      <c r="J50" s="3">
+      <c r="J50" s="17">
         <v>93.227052715654949</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="17">
         <v>0.91832229580573943</v>
       </c>
-      <c r="M50" s="2">
+      <c r="L50" s="15"/>
+      <c r="M50" s="16">
         <f t="shared" si="2"/>
         <v>46</v>
       </c>
-      <c r="N50" s="3">
+      <c r="N50" s="17">
         <v>40.681268618387257</v>
       </c>
-      <c r="O50" s="3">
+      <c r="O50" s="17">
         <v>145.648932238193</v>
       </c>
-      <c r="P50" s="3">
+      <c r="P50" s="17">
         <v>0.92585170340681355</v>
       </c>
       <c r="R50" s="2">
@@ -9348,8 +9883,18 @@
       <c r="Z50" s="3">
         <v>0.79083969465648862</v>
       </c>
-    </row>
-    <row r="51" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB50" s="2">
+        <f t="shared" si="5"/>
+        <v>46</v>
+      </c>
+      <c r="AC50" s="3">
+        <v>44.037710516103992</v>
+      </c>
+      <c r="AD50" s="3">
+        <v>109.1608992248062</v>
+      </c>
+    </row>
+    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -9360,30 +9905,31 @@
       <c r="E51" s="3">
         <v>93.650114170584288</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="16">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="3">
+      <c r="I51" s="17">
         <v>33.239548451548451</v>
       </c>
-      <c r="J51" s="3">
+      <c r="J51" s="17">
         <v>95.216589456869002</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="17">
         <v>0.92105263157894746</v>
       </c>
-      <c r="M51" s="2">
+      <c r="L51" s="15"/>
+      <c r="M51" s="16">
         <f t="shared" si="2"/>
         <v>47</v>
       </c>
-      <c r="N51" s="3">
+      <c r="N51" s="17">
         <v>41.669352850539298</v>
       </c>
-      <c r="O51" s="3">
+      <c r="O51" s="17">
         <v>128.5404106776181</v>
       </c>
-      <c r="P51" s="3">
+      <c r="P51" s="17">
         <v>0.9346938775510204</v>
       </c>
       <c r="R51" s="2">
@@ -9412,8 +9958,18 @@
       <c r="Z51" s="3">
         <v>0.78382581648522553</v>
       </c>
-    </row>
-    <row r="52" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB51" s="2">
+        <f t="shared" si="5"/>
+        <v>47</v>
+      </c>
+      <c r="AC51" s="3">
+        <v>43.096041909196742</v>
+      </c>
+      <c r="AD51" s="3">
+        <v>127.15589147286821</v>
+      </c>
+    </row>
+    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -9424,30 +9980,31 @@
       <c r="E52" s="3">
         <v>100.5610275352585</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="16">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="3">
+      <c r="I52" s="17">
         <v>32.330719280719293</v>
       </c>
-      <c r="J52" s="3">
+      <c r="J52" s="17">
         <v>99.759744408945693</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="17">
         <v>0.90949227373068431</v>
       </c>
-      <c r="M52" s="2">
+      <c r="L52" s="15"/>
+      <c r="M52" s="16">
         <f t="shared" si="2"/>
         <v>48</v>
       </c>
-      <c r="N52" s="3">
+      <c r="N52" s="17">
         <v>42.313153569594242</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O52" s="17">
         <v>128.9450308008214</v>
       </c>
-      <c r="P52" s="3">
+      <c r="P52" s="17">
         <v>0.94117647058823539</v>
       </c>
       <c r="R52" s="2">
@@ -9476,8 +10033,18 @@
       <c r="Z52" s="3">
         <v>0.8168557536466774</v>
       </c>
-    </row>
-    <row r="53" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB52" s="2">
+        <f t="shared" si="5"/>
+        <v>48</v>
+      </c>
+      <c r="AC52" s="3">
+        <v>43.462572759022123</v>
+      </c>
+      <c r="AD52" s="3">
+        <v>116.93624806201549</v>
+      </c>
+    </row>
+    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -9488,30 +10055,31 @@
       <c r="E53" s="3">
         <v>96.358596373404978</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="16">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="3">
+      <c r="I53" s="17">
         <v>32.713758241758249</v>
       </c>
-      <c r="J53" s="3">
+      <c r="J53" s="17">
         <v>100.1563178913738</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K53" s="17">
         <v>0.91428571428571437</v>
       </c>
-      <c r="M53" s="2">
+      <c r="L53" s="15"/>
+      <c r="M53" s="16">
         <f t="shared" si="2"/>
         <v>49</v>
       </c>
-      <c r="N53" s="3">
+      <c r="N53" s="17">
         <v>41.538741653826413</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O53" s="17">
         <v>129.60850102669411</v>
       </c>
-      <c r="P53" s="3">
+      <c r="P53" s="17">
         <v>0.93737373737373741</v>
       </c>
       <c r="R53" s="2">
@@ -9540,8 +10108,18 @@
       <c r="Z53" s="3">
         <v>0.78387096774193554</v>
       </c>
-    </row>
-    <row r="54" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB53" s="2">
+        <f t="shared" si="5"/>
+        <v>49</v>
+      </c>
+      <c r="AC53" s="3">
+        <v>44.291505626697713</v>
+      </c>
+      <c r="AD53" s="3">
+        <v>111.8055813953488</v>
+      </c>
+    </row>
+    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -9552,30 +10130,31 @@
       <c r="E54" s="3">
         <v>100.1011820013432</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="16">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="3">
+      <c r="I54" s="17">
         <v>33.279206793206789</v>
       </c>
-      <c r="J54" s="3">
+      <c r="J54" s="17">
         <v>95.487915335463256</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K54" s="17">
         <v>0.93043478260869561</v>
       </c>
-      <c r="M54" s="2">
+      <c r="L54" s="15"/>
+      <c r="M54" s="16">
         <f t="shared" si="2"/>
         <v>50</v>
       </c>
-      <c r="N54" s="3">
+      <c r="N54" s="17">
         <v>42.707688751926042</v>
       </c>
-      <c r="O54" s="3">
+      <c r="O54" s="17">
         <v>117.4767145790555</v>
       </c>
-      <c r="P54" s="3">
+      <c r="P54" s="17">
         <v>0.95121951219512191</v>
       </c>
       <c r="R54" s="2">
@@ -9604,8 +10183,29 @@
       <c r="Z54" s="3">
         <v>0.81031866464339908</v>
       </c>
-    </row>
-    <row r="56" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB54" s="2">
+        <f t="shared" si="5"/>
+        <v>50</v>
+      </c>
+      <c r="AC54" s="3">
+        <v>44.229868063639891</v>
+      </c>
+      <c r="AD54" s="3">
+        <v>112.03973643410851</v>
+      </c>
+    </row>
+    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="H55" s="15"/>
+      <c r="I55" s="15"/>
+      <c r="J55" s="15"/>
+      <c r="K55" s="15"/>
+      <c r="L55" s="15"/>
+      <c r="M55" s="15"/>
+      <c r="N55" s="15"/>
+      <c r="O55" s="15"/>
+      <c r="P55" s="15"/>
+    </row>
+    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -9617,33 +10217,34 @@
         <f>AVERAGE(E5:E54)</f>
         <v>97.598678173270599</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="3">
+      <c r="I56" s="17">
         <f>AVERAGE(I5:I54)</f>
         <v>32.973438401598408</v>
       </c>
-      <c r="J56" s="3">
+      <c r="J56" s="17">
         <f>AVERAGE(J5:J54)</f>
         <v>98.379571405750809</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56" s="17">
         <f>AVERAGE(K5:K54)</f>
         <v>0.89928343770783348</v>
       </c>
-      <c r="M56" s="2" t="s">
+      <c r="L56" s="15"/>
+      <c r="M56" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="N56" s="3">
+      <c r="N56" s="17">
         <f>AVERAGE(N5:N54)</f>
         <v>41.676103954802265</v>
       </c>
-      <c r="O56" s="3">
+      <c r="O56" s="17">
         <f>AVERAGE(O5:O54)</f>
         <v>128.0171979466119</v>
       </c>
-      <c r="P56" s="3">
+      <c r="P56" s="17">
         <f>AVERAGE(P5:P54)</f>
         <v>0.94508022479194187</v>
       </c>
@@ -9677,8 +10278,19 @@
         <f>AVERAGE(Z5:Z54)</f>
         <v>0.79467782527036457</v>
       </c>
-    </row>
-    <row r="57" spans="3:26" x14ac:dyDescent="0.25">
+      <c r="AB56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AC56" s="3">
+        <f>AVERAGE(AC5:AC54)</f>
+        <v>43.641598603026779</v>
+      </c>
+      <c r="AD56" s="3">
+        <f>AVERAGE(AD5:AD54)</f>
+        <v>116.28809426356592</v>
+      </c>
+    </row>
+    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -9690,33 +10302,34 @@
         <f>_xlfn.STDEV.S(E5:E54)</f>
         <v>2.5439019153472042</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="3">
+      <c r="I57" s="17">
         <f>_xlfn.STDEV.S(I5:I54)</f>
         <v>0.29863893743100534</v>
       </c>
-      <c r="J57" s="3">
+      <c r="J57" s="17">
         <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>2.7722317733107955</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57" s="17">
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>1.7116157402485069E-2</v>
       </c>
-      <c r="M57" s="2" t="s">
+      <c r="L57" s="15"/>
+      <c r="M57" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="N57" s="3">
+      <c r="N57" s="17">
         <f>_xlfn.STDEV.S(N5:N54)</f>
         <v>0.70394240200137581</v>
       </c>
-      <c r="O57" s="3">
+      <c r="O57" s="17">
         <f>_xlfn.STDEV.S(O5:O54)</f>
         <v>8.177697174742022</v>
       </c>
-      <c r="P57" s="3">
+      <c r="P57" s="17">
         <f>_xlfn.STDEV.S(P5:P54)</f>
         <v>1.0308949808780091E-2</v>
       </c>
@@ -9749,6 +10362,17 @@
       <c r="Z57" s="3">
         <f>_xlfn.STDEV.S(Z5:Z54)</f>
         <v>1.9067980952349326E-2</v>
+      </c>
+      <c r="AB57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AC57" s="3">
+        <f>_xlfn.STDEV.S(AC5:AC54)</f>
+        <v>0.42557014512045621</v>
+      </c>
+      <c r="AD57" s="3">
+        <f>_xlfn.STDEV.S(AD5:AD54)</f>
+        <v>4.1512051854914294</v>
       </c>
     </row>
   </sheetData>
@@ -9761,8 +10385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AL57"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Y44" sqref="Y44"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Z28" sqref="Z28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9787,10 +10411,12 @@
         <v>4</v>
       </c>
       <c r="E3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="1"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="15"/>
       <c r="N3" s="1" t="s">
         <v>33</v>
       </c>
@@ -9808,14 +10434,14 @@
       <c r="E4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="16"/>
+      <c r="I4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="16" t="s">
         <v>9</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="16" t="s">
         <v>5</v>
       </c>
       <c r="N4" s="2"/>
@@ -9858,16 +10484,16 @@
       <c r="E5" s="4">
         <v>2.6872809770650489E-2</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="16">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="18">
         <v>7.3054991303972178E-4</v>
       </c>
-      <c r="J5" s="4">
+      <c r="J5" s="18">
         <v>7.9053139800706277E-3</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="17">
         <v>0.91938997821350776</v>
       </c>
       <c r="N5" s="2">
@@ -9915,17 +10541,17 @@
       <c r="E6" s="4">
         <v>2.8297882858074969E-2</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="16">
         <f>H5+1</f>
         <v>2</v>
       </c>
-      <c r="I6" s="4">
+      <c r="I6" s="18">
         <v>7.2775903938616905E-4</v>
       </c>
-      <c r="J6" s="4">
+      <c r="J6" s="18">
         <v>9.2527687092204304E-3</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="17">
         <v>0.86877828054298634</v>
       </c>
       <c r="N6" s="2">
@@ -9975,17 +10601,17 @@
       <c r="E7" s="4">
         <v>2.6811164812730631E-2</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="16">
         <f t="shared" ref="H7:H54" si="1">H6+1</f>
         <v>3</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="18">
         <v>7.273619363185876E-4</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="18">
         <v>7.3582175788381677E-3</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="17">
         <v>0.91150442477876115</v>
       </c>
       <c r="N7" s="2">
@@ -10035,17 +10661,17 @@
       <c r="E8" s="4">
         <v>2.8402875125575131E-2</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="16">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="I8" s="4">
+      <c r="I8" s="18">
         <v>7.6874518698567134E-4</v>
       </c>
-      <c r="J8" s="4">
+      <c r="J8" s="18">
         <v>7.3056744941661263E-3</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="17">
         <v>0.90308370044052877</v>
       </c>
       <c r="N8" s="2">
@@ -10095,17 +10721,17 @@
       <c r="E9" s="4">
         <v>2.5853134642315759E-2</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="16">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="I9" s="4">
+      <c r="I9" s="18">
         <v>7.859219696341852E-4</v>
       </c>
-      <c r="J9" s="4">
+      <c r="J9" s="18">
         <v>7.0367067724706692E-3</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="17">
         <v>0.89977728285077951</v>
       </c>
       <c r="N9" s="2">
@@ -10155,17 +10781,17 @@
       <c r="E10" s="4">
         <v>3.0369313080958471E-2</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="16">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="I10" s="4">
+      <c r="I10" s="18">
         <v>7.3747736420139533E-4</v>
       </c>
-      <c r="J10" s="4">
+      <c r="J10" s="18">
         <v>7.1854959711028519E-3</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="17">
         <v>0.91352549889135259</v>
       </c>
       <c r="N10" s="2">
@@ -10215,17 +10841,17 @@
       <c r="E11" s="4">
         <v>2.9039274741696479E-2</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="16">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="I11" s="4">
+      <c r="I11" s="18">
         <v>7.8089912875852895E-4</v>
       </c>
-      <c r="J11" s="4">
+      <c r="J11" s="18">
         <v>6.854203064220527E-3</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="17">
         <v>0.92341356673960617</v>
       </c>
       <c r="N11" s="2">
@@ -10275,17 +10901,17 @@
       <c r="E12" s="4">
         <v>2.7928201559299069E-2</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="16">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="I12" s="4">
+      <c r="I12" s="18">
         <v>7.6610083060762145E-4</v>
       </c>
-      <c r="J12" s="4">
+      <c r="J12" s="18">
         <v>7.200023382403423E-3</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="17">
         <v>0.89485458612975399</v>
       </c>
       <c r="N12" s="2">
@@ -10335,17 +10961,17 @@
       <c r="E13" s="4">
         <v>2.8141538016755889E-2</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="16">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="I13" s="4">
+      <c r="I13" s="18">
         <v>7.5875659833013779E-4</v>
       </c>
-      <c r="J13" s="4">
+      <c r="J13" s="18">
         <v>8.1272663705131594E-3</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="17">
         <v>0.89686098654708535</v>
       </c>
       <c r="N13" s="2">
@@ -10395,17 +11021,17 @@
       <c r="E14" s="4">
         <v>2.687925624265711E-2</v>
       </c>
-      <c r="H14" s="2">
+      <c r="H14" s="16">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="18">
         <v>7.6286475085775274E-4</v>
       </c>
-      <c r="J14" s="4">
+      <c r="J14" s="18">
         <v>5.8779181857611506E-3</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="17">
         <v>0.92872570194384452</v>
       </c>
       <c r="N14" s="2">
@@ -10455,17 +11081,17 @@
       <c r="E15" s="4">
         <v>2.882085174650945E-2</v>
       </c>
-      <c r="H15" s="2">
+      <c r="H15" s="16">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="I15" s="4">
+      <c r="I15" s="18">
         <v>7.6916773795141218E-4</v>
       </c>
-      <c r="J15" s="4">
+      <c r="J15" s="18">
         <v>7.3442704364819261E-3</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="17">
         <v>0.88487584650112872</v>
       </c>
       <c r="N15" s="2">
@@ -10515,17 +11141,17 @@
       <c r="E16" s="4">
         <v>2.975635506976828E-2</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="16">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="18">
         <v>7.855095300392629E-4</v>
       </c>
-      <c r="J16" s="4">
+      <c r="J16" s="18">
         <v>6.9174305577748927E-3</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="17">
         <v>0.90380313199105144</v>
       </c>
       <c r="N16" s="2">
@@ -10575,17 +11201,17 @@
       <c r="E17" s="4">
         <v>2.734510818016956E-2</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="16">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="18">
         <v>7.6525442447802179E-4</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="18">
         <v>7.2336422848631636E-3</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="17">
         <v>0.8868778280542986</v>
       </c>
       <c r="N17" s="2">
@@ -10635,17 +11261,17 @@
       <c r="E18" s="4">
         <v>2.549298724019286E-2</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="16">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="I18" s="4">
+      <c r="I18" s="18">
         <v>7.8926878666558823E-4</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="18">
         <v>6.4125798325584023E-3</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="17">
         <v>0.90350877192982448</v>
       </c>
       <c r="N18" s="2">
@@ -10695,17 +11321,17 @@
       <c r="E19" s="4">
         <v>2.4181809072906651E-2</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="16">
         <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="I19" s="4">
+      <c r="I19" s="18">
         <v>7.5940094435271953E-4</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="18">
         <v>6.6864778170868814E-3</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="17">
         <v>0.90350877192982448</v>
       </c>
       <c r="N19" s="2">
@@ -10755,17 +11381,17 @@
       <c r="E20" s="4">
         <v>2.5848474995463978E-2</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="16">
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="18">
         <v>7.6131344616830402E-4</v>
       </c>
-      <c r="J20" s="4">
+      <c r="J20" s="18">
         <v>8.7204799770255574E-3</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="17">
         <v>0.90869565217391302</v>
       </c>
       <c r="N20" s="2">
@@ -10806,17 +11432,17 @@
       <c r="E21" s="4">
         <v>2.6240046834724091E-2</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H21" s="16">
         <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="I21" s="4">
+      <c r="I21" s="18">
         <v>7.8121892797452901E-4</v>
       </c>
-      <c r="J21" s="4">
+      <c r="J21" s="18">
         <v>6.0070753920913921E-3</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="17">
         <v>0.92747252747252751</v>
       </c>
       <c r="N21" s="2">
@@ -10857,17 +11483,17 @@
       <c r="E22" s="4">
         <v>2.8783177102295769E-2</v>
       </c>
-      <c r="H22" s="2">
+      <c r="H22" s="16">
         <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="18">
         <v>7.6053012558254538E-4</v>
       </c>
-      <c r="J22" s="4">
+      <c r="J22" s="18">
         <v>5.9287342890273157E-3</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="17">
         <v>0.90380313199105144</v>
       </c>
       <c r="N22" s="2">
@@ -10908,17 +11534,17 @@
       <c r="E23" s="4">
         <v>2.481079967838417E-2</v>
       </c>
-      <c r="H23" s="2">
+      <c r="H23" s="16">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="18">
         <v>7.8077372390414714E-4</v>
       </c>
-      <c r="J23" s="4">
+      <c r="J23" s="18">
         <v>5.5152953518202517E-3</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="17">
         <v>0.89795918367346927</v>
       </c>
       <c r="N23" s="2">
@@ -10959,17 +11585,17 @@
       <c r="E24" s="4">
         <v>2.6490374757372689E-2</v>
       </c>
-      <c r="H24" s="2">
+      <c r="H24" s="16">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I24" s="4">
+      <c r="I24" s="18">
         <v>7.5733659537335408E-4</v>
       </c>
-      <c r="J24" s="4">
+      <c r="J24" s="18">
         <v>7.6325203402343913E-3</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="17">
         <v>0.8928571428571429</v>
       </c>
       <c r="N24" s="2">
@@ -11010,17 +11636,17 @@
       <c r="E25" s="4">
         <v>2.8047402593543391E-2</v>
       </c>
-      <c r="H25" s="2">
+      <c r="H25" s="16">
         <f t="shared" si="1"/>
         <v>21</v>
       </c>
-      <c r="I25" s="4">
+      <c r="I25" s="18">
         <v>7.363428607739201E-4</v>
       </c>
-      <c r="J25" s="4">
+      <c r="J25" s="18">
         <v>7.1744372537360917E-3</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="17">
         <v>0.91973969631236441</v>
       </c>
       <c r="N25" s="2">
@@ -11061,17 +11687,17 @@
       <c r="E26" s="4">
         <v>2.5780589083182689E-2</v>
       </c>
-      <c r="H26" s="2">
+      <c r="H26" s="16">
         <f t="shared" si="1"/>
         <v>22</v>
       </c>
-      <c r="I26" s="4">
+      <c r="I26" s="18">
         <v>6.8354247055653979E-4</v>
       </c>
-      <c r="J26" s="4">
+      <c r="J26" s="18">
         <v>7.3295536475015974E-3</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="17">
         <v>0.93275488069414314</v>
       </c>
       <c r="N26" s="2">
@@ -11112,17 +11738,17 @@
       <c r="E27" s="4">
         <v>2.5570233238790499E-2</v>
       </c>
-      <c r="H27" s="2">
+      <c r="H27" s="16">
         <f t="shared" si="1"/>
         <v>23</v>
       </c>
-      <c r="I27" s="4">
+      <c r="I27" s="18">
         <v>7.4185821596320161E-4</v>
       </c>
-      <c r="J27" s="4">
+      <c r="J27" s="18">
         <v>8.6338343217365766E-3</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="17">
         <v>0.9111111111111112</v>
       </c>
       <c r="N27" s="2">
@@ -11163,17 +11789,17 @@
       <c r="E28" s="4">
         <v>2.8819020744889162E-2</v>
       </c>
-      <c r="H28" s="2">
+      <c r="H28" s="16">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="I28" s="4">
+      <c r="I28" s="18">
         <v>7.5523591306526493E-4</v>
       </c>
-      <c r="J28" s="4">
+      <c r="J28" s="18">
         <v>7.608370092279119E-3</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="17">
         <v>0.91703056768558955</v>
       </c>
       <c r="N28" s="2">
@@ -11214,17 +11840,17 @@
       <c r="E29" s="4">
         <v>3.0057788823361881E-2</v>
       </c>
-      <c r="H29" s="2">
+      <c r="H29" s="16">
         <f t="shared" si="1"/>
         <v>25</v>
       </c>
-      <c r="I29" s="4">
+      <c r="I29" s="18">
         <v>7.9871536622971851E-4</v>
       </c>
-      <c r="J29" s="4">
+      <c r="J29" s="18">
         <v>6.761408844259925E-3</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="17">
         <v>0.9126637554585153</v>
       </c>
       <c r="N29" s="2">
@@ -11265,17 +11891,17 @@
       <c r="E30" s="4">
         <v>3.036462570137707E-2</v>
       </c>
-      <c r="H30" s="2">
+      <c r="H30" s="16">
         <f t="shared" si="1"/>
         <v>26</v>
       </c>
-      <c r="I30" s="4">
+      <c r="I30" s="18">
         <v>7.1965998048706555E-4</v>
       </c>
-      <c r="J30" s="4">
+      <c r="J30" s="18">
         <v>9.724471229207313E-3</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="17">
         <v>0.89342403628117906</v>
       </c>
       <c r="N30" s="2">
@@ -11316,17 +11942,17 @@
       <c r="E31" s="4">
         <v>2.6176243985086022E-2</v>
       </c>
-      <c r="H31" s="2">
+      <c r="H31" s="16">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="I31" s="4">
+      <c r="I31" s="18">
         <v>7.6634011989119486E-4</v>
       </c>
-      <c r="J31" s="4">
+      <c r="J31" s="18">
         <v>7.7077774262973037E-3</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="17">
         <v>0.90909090909090906</v>
       </c>
       <c r="N31" s="2">
@@ -11367,17 +11993,17 @@
       <c r="E32" s="4">
         <v>2.77923234996077E-2</v>
       </c>
-      <c r="H32" s="2">
+      <c r="H32" s="16">
         <f t="shared" si="1"/>
         <v>28</v>
       </c>
-      <c r="I32" s="4">
+      <c r="I32" s="18">
         <v>7.2252445291465153E-4</v>
       </c>
-      <c r="J32" s="4">
+      <c r="J32" s="18">
         <v>7.8745270776356315E-3</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="17">
         <v>0.90507726269315669</v>
       </c>
       <c r="N32" s="2">
@@ -11418,17 +12044,17 @@
       <c r="E33" s="4">
         <v>3.1133483508790579E-2</v>
       </c>
-      <c r="H33" s="2">
+      <c r="H33" s="16">
         <f t="shared" si="1"/>
         <v>29</v>
       </c>
-      <c r="I33" s="4">
+      <c r="I33" s="18">
         <v>7.6799249131884488E-4</v>
       </c>
-      <c r="J33" s="4">
+      <c r="J33" s="18">
         <v>7.6842849530559722E-3</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="17">
         <v>0.8783783783783784</v>
       </c>
       <c r="N33" s="2">
@@ -11469,17 +12095,17 @@
       <c r="E34" s="4">
         <v>2.667409849898604E-2</v>
       </c>
-      <c r="H34" s="2">
+      <c r="H34" s="16">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="I34" s="4">
+      <c r="I34" s="18">
         <v>7.6217233168613969E-4</v>
       </c>
-      <c r="J34" s="4">
+      <c r="J34" s="18">
         <v>6.4886574628806939E-3</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="17">
         <v>0.90949227373068431</v>
       </c>
       <c r="N34" s="2">
@@ -11520,17 +12146,17 @@
       <c r="E35" s="4">
         <v>2.6440087674392359E-2</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H35" s="16">
         <f t="shared" si="1"/>
         <v>31</v>
       </c>
-      <c r="I35" s="4">
+      <c r="I35" s="18">
         <v>7.7048272847028948E-4</v>
       </c>
-      <c r="J35" s="4">
+      <c r="J35" s="18">
         <v>7.5063549336500442E-3</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="17">
         <v>0.91428571428571437</v>
       </c>
       <c r="N35" s="2">
@@ -11571,17 +12197,17 @@
       <c r="E36" s="4">
         <v>2.8551800829002751E-2</v>
       </c>
-      <c r="H36" s="2">
+      <c r="H36" s="16">
         <f t="shared" si="1"/>
         <v>32</v>
       </c>
-      <c r="I36" s="4">
+      <c r="I36" s="18">
         <v>7.5648264479976344E-4</v>
       </c>
-      <c r="J36" s="4">
+      <c r="J36" s="18">
         <v>6.7478526077371969E-3</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="17">
         <v>0.8928571428571429</v>
       </c>
       <c r="N36" s="2">
@@ -11622,17 +12248,17 @@
       <c r="E37" s="4">
         <v>2.6971365282784019E-2</v>
       </c>
-      <c r="H37" s="2">
+      <c r="H37" s="16">
         <f t="shared" si="1"/>
         <v>33</v>
       </c>
-      <c r="I37" s="4">
+      <c r="I37" s="18">
         <v>7.082102114009919E-4</v>
       </c>
-      <c r="J37" s="4">
+      <c r="J37" s="18">
         <v>9.7256589092136487E-3</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="17">
         <v>0.91390728476821192</v>
       </c>
       <c r="N37" s="2">
@@ -11673,17 +12299,17 @@
       <c r="E38" s="4">
         <v>2.8085421339488811E-2</v>
       </c>
-      <c r="H38" s="2">
+      <c r="H38" s="16">
         <f t="shared" si="1"/>
         <v>34</v>
       </c>
-      <c r="I38" s="4">
+      <c r="I38" s="18">
         <v>7.4792561910549287E-4</v>
       </c>
-      <c r="J38" s="4">
+      <c r="J38" s="18">
         <v>7.7813951245616977E-3</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="17">
         <v>0.88741721854304645</v>
       </c>
       <c r="N38" s="2">
@@ -11724,17 +12350,17 @@
       <c r="E39" s="4">
         <v>2.77635868504937E-2</v>
       </c>
-      <c r="H39" s="2">
+      <c r="H39" s="16">
         <f t="shared" si="1"/>
         <v>35</v>
       </c>
-      <c r="I39" s="4">
+      <c r="I39" s="18">
         <v>7.6621782936206885E-4</v>
       </c>
-      <c r="J39" s="4">
+      <c r="J39" s="18">
         <v>8.399670319009029E-3</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="17">
         <v>0.8868778280542986</v>
       </c>
       <c r="N39" s="2">
@@ -11775,17 +12401,17 @@
       <c r="E40" s="4">
         <v>2.7218575965366941E-2</v>
       </c>
-      <c r="H40" s="2">
+      <c r="H40" s="16">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="I40" s="4">
+      <c r="I40" s="18">
         <v>7.185744618904324E-4</v>
       </c>
-      <c r="J40" s="4">
+      <c r="J40" s="18">
         <v>7.9736007370085089E-3</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="17">
         <v>0.88392857142857129</v>
       </c>
       <c r="N40" s="2">
@@ -11826,17 +12452,17 @@
       <c r="E41" s="4">
         <v>2.9723421719144799E-2</v>
       </c>
-      <c r="H41" s="2">
+      <c r="H41" s="16">
         <f t="shared" si="1"/>
         <v>37</v>
       </c>
-      <c r="I41" s="4">
+      <c r="I41" s="18">
         <v>7.839989790524158E-4</v>
       </c>
-      <c r="J41" s="4">
+      <c r="J41" s="18">
         <v>7.0495461085633877E-3</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="17">
         <v>0.89485458612975399</v>
       </c>
       <c r="N41" s="2">
@@ -11877,17 +12503,17 @@
       <c r="E42" s="4">
         <v>2.5739825124919659E-2</v>
       </c>
-      <c r="H42" s="2">
+      <c r="H42" s="16">
         <f t="shared" si="1"/>
         <v>38</v>
       </c>
-      <c r="I42" s="4">
+      <c r="I42" s="18">
         <v>7.9131292119946021E-4</v>
       </c>
-      <c r="J42" s="4">
+      <c r="J42" s="18">
         <v>6.4134340741896414E-3</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="17">
         <v>0.92810457516339873</v>
       </c>
       <c r="N42" s="2">
@@ -11928,17 +12554,17 @@
       <c r="E43" s="4">
         <v>2.6779323254488101E-2</v>
       </c>
-      <c r="H43" s="2">
+      <c r="H43" s="16">
         <f t="shared" si="1"/>
         <v>39</v>
       </c>
-      <c r="I43" s="4">
+      <c r="I43" s="18">
         <v>7.6983747451217824E-4</v>
       </c>
-      <c r="J43" s="4">
+      <c r="J43" s="18">
         <v>6.5858596888496096E-3</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="17">
         <v>0.90134529147982068</v>
       </c>
       <c r="N43" s="2">
@@ -11979,17 +12605,17 @@
       <c r="E44" s="4">
         <v>2.401601120272474E-2</v>
       </c>
-      <c r="H44" s="2">
+      <c r="H44" s="16">
         <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="I44" s="4">
+      <c r="I44" s="18">
         <v>7.4798897065226039E-4</v>
       </c>
-      <c r="J44" s="4">
+      <c r="J44" s="18">
         <v>8.0029016577502742E-3</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="17">
         <v>0.91666666666666663</v>
       </c>
       <c r="N44" s="2">
@@ -12030,17 +12656,17 @@
       <c r="E45" s="4">
         <v>2.8005137930539891E-2</v>
       </c>
-      <c r="H45" s="2">
+      <c r="H45" s="16">
         <f t="shared" si="1"/>
         <v>41</v>
       </c>
-      <c r="I45" s="4">
+      <c r="I45" s="18">
         <v>7.574657934107964E-4</v>
       </c>
-      <c r="J45" s="4">
+      <c r="J45" s="18">
         <v>7.715341570947872E-3</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="17">
         <v>0.89438202247191023</v>
       </c>
       <c r="N45" s="2">
@@ -12081,17 +12707,17 @@
       <c r="E46" s="4">
         <v>3.0798913894152791E-2</v>
       </c>
-      <c r="H46" s="2">
+      <c r="H46" s="16">
         <f t="shared" si="1"/>
         <v>42</v>
       </c>
-      <c r="I46" s="4">
+      <c r="I46" s="18">
         <v>7.512336681669389E-4</v>
       </c>
-      <c r="J46" s="4">
+      <c r="J46" s="18">
         <v>7.4137011303850222E-3</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="17">
         <v>0.8669724770642202</v>
       </c>
       <c r="N46" s="2">
@@ -12132,17 +12758,17 @@
       <c r="E47" s="4">
         <v>2.8537236460197641E-2</v>
       </c>
-      <c r="H47" s="2">
+      <c r="H47" s="16">
         <f t="shared" si="1"/>
         <v>43</v>
       </c>
-      <c r="I47" s="4">
+      <c r="I47" s="18">
         <v>7.4976945885124927E-4</v>
       </c>
-      <c r="J47" s="4">
+      <c r="J47" s="18">
         <v>6.9376780017463054E-3</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="17">
         <v>0.92841648590021697</v>
       </c>
       <c r="N47" s="2">
@@ -12183,17 +12809,17 @@
       <c r="E48" s="4">
         <v>2.8668062253393911E-2</v>
       </c>
-      <c r="H48" s="2">
+      <c r="H48" s="16">
         <f t="shared" si="1"/>
         <v>44</v>
       </c>
-      <c r="I48" s="4">
+      <c r="I48" s="18">
         <v>7.7089214564833868E-4</v>
       </c>
-      <c r="J48" s="4">
+      <c r="J48" s="18">
         <v>6.9732516634904828E-3</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="17">
         <v>0.91228070175438603</v>
       </c>
       <c r="N48" s="2">
@@ -12234,17 +12860,17 @@
       <c r="E49" s="4">
         <v>2.8005740654497211E-2</v>
       </c>
-      <c r="H49" s="2">
+      <c r="H49" s="16">
         <f t="shared" si="1"/>
         <v>45</v>
       </c>
-      <c r="I49" s="4">
+      <c r="I49" s="18">
         <v>7.5565282313349875E-4</v>
       </c>
-      <c r="J49" s="4">
+      <c r="J49" s="18">
         <v>6.8725771875219567E-3</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="17">
         <v>0.88127853881278551</v>
       </c>
       <c r="N49" s="2">
@@ -12285,17 +12911,17 @@
       <c r="E50" s="4">
         <v>2.612216900567654E-2</v>
       </c>
-      <c r="H50" s="2">
+      <c r="H50" s="16">
         <f t="shared" si="1"/>
         <v>46</v>
       </c>
-      <c r="I50" s="4">
+      <c r="I50" s="18">
         <v>7.7598594294192612E-4</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="18">
         <v>6.4286134856099157E-3</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="17">
         <v>0.92139737991266379</v>
       </c>
       <c r="N50" s="2">
@@ -12336,17 +12962,17 @@
       <c r="E51" s="4">
         <v>2.9210147704990919E-2</v>
       </c>
-      <c r="H51" s="2">
+      <c r="H51" s="16">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="I51" s="4">
+      <c r="I51" s="18">
         <v>8.1245259152935411E-4</v>
       </c>
-      <c r="J51" s="4">
+      <c r="J51" s="18">
         <v>6.9663434976151867E-3</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="17">
         <v>0.89333333333333331</v>
       </c>
       <c r="N51" s="2">
@@ -12387,17 +13013,17 @@
       <c r="E52" s="4">
         <v>2.8592664583893521E-2</v>
       </c>
-      <c r="H52" s="2">
+      <c r="H52" s="16">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="I52" s="4">
+      <c r="I52" s="18">
         <v>7.5938456207537669E-4</v>
       </c>
-      <c r="J52" s="4">
+      <c r="J52" s="18">
         <v>7.237472228691851E-3</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="17">
         <v>0.90423162583518935</v>
       </c>
       <c r="N52" s="2">
@@ -12438,17 +13064,17 @@
       <c r="E53" s="4">
         <v>2.8166956626693759E-2</v>
       </c>
-      <c r="H53" s="2">
+      <c r="H53" s="16">
         <f t="shared" si="1"/>
         <v>49</v>
       </c>
-      <c r="I53" s="4">
+      <c r="I53" s="18">
         <v>7.1914394072859896E-4</v>
       </c>
-      <c r="J53" s="4">
+      <c r="J53" s="18">
         <v>7.9042481584177902E-3</v>
       </c>
-      <c r="K53" s="3">
+      <c r="K53" s="17">
         <v>0.90748898678414092</v>
       </c>
       <c r="N53" s="2">
@@ -12489,17 +13115,17 @@
       <c r="E54" s="4">
         <v>2.8923390865649719E-2</v>
       </c>
-      <c r="H54" s="2">
+      <c r="H54" s="16">
         <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I54" s="4">
+      <c r="I54" s="18">
         <v>7.3873382439944735E-4</v>
       </c>
-      <c r="J54" s="4">
+      <c r="J54" s="18">
         <v>8.4813349173732417E-3</v>
       </c>
-      <c r="K54" s="3">
+      <c r="K54" s="17">
         <v>0.89639639639639634</v>
       </c>
       <c r="N54" s="2">
@@ -12532,8 +13158,10 @@
     <row r="55" spans="3:23" x14ac:dyDescent="0.25">
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
-      <c r="I55" s="5"/>
-      <c r="J55" s="5"/>
+      <c r="H55" s="15"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="19"/>
+      <c r="K55" s="15"/>
       <c r="O55" s="5"/>
       <c r="P55" s="5"/>
       <c r="U55" s="5"/>
@@ -12551,18 +13179,18 @@
         <f>AVERAGE(E5:E54)</f>
         <v>2.7662021688572166E-2</v>
       </c>
-      <c r="H56" s="2" t="s">
+      <c r="H56" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="I56" s="4">
+      <c r="I56" s="18">
         <f>AVERAGE(I5:I54)</f>
         <v>7.5724683509654145E-4</v>
       </c>
-      <c r="J56" s="4">
+      <c r="J56" s="18">
         <f>AVERAGE(J5:J54)</f>
         <v>7.3721250619730857E-3</v>
       </c>
-      <c r="K56" s="3">
+      <c r="K56" s="17">
         <f>AVERAGE(K5:K54)</f>
         <v>0.90376923389460639</v>
       </c>
@@ -12609,18 +13237,18 @@
         <f>_xlfn.STDEV.S(E5:E54)</f>
         <v>1.6698090965107128E-3</v>
       </c>
-      <c r="H57" s="2" t="s">
+      <c r="H57" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="I57" s="4">
+      <c r="I57" s="18">
         <f>_xlfn.STDEV.S(I5:I54)</f>
         <v>2.4824291707019717E-5</v>
       </c>
-      <c r="J57" s="4">
+      <c r="J57" s="18">
         <f>_xlfn.STDEV.S(J5:J54)</f>
         <v>8.999383576214589E-4</v>
       </c>
-      <c r="K57" s="3">
+      <c r="K57" s="17">
         <f>_xlfn.STDEV.S(K5:K54)</f>
         <v>1.5395698477376924E-2</v>
       </c>

</xml_diff>

<commit_message>
single model on balanced dataset (mse)
</commit_message>
<xml_diff>
--- a/migforecasting/underground/tests on superdataset/test-13.xlsx
+++ b/migforecasting/underground/tests on superdataset/test-13.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="pos vs neg" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="37">
   <si>
     <t>train (MAE)</t>
   </si>
@@ -6343,7 +6343,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AD57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="AH18" sqref="AH18"/>
     </sheetView>
   </sheetViews>
@@ -10385,8 +10385,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:AL57"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Z28" sqref="Z28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10401,6 +10401,8 @@
     <col min="20" max="20" width="9.7109375" customWidth="1"/>
     <col min="21" max="21" width="13" customWidth="1"/>
     <col min="22" max="22" width="13.42578125" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" customWidth="1"/>
+    <col min="28" max="28" width="13" customWidth="1"/>
     <col min="36" max="36" width="16.140625" customWidth="1"/>
     <col min="37" max="37" width="15.85546875" customWidth="1"/>
     <col min="38" max="38" width="14" customWidth="1"/>
@@ -10425,6 +10427,10 @@
         <v>34</v>
       </c>
       <c r="V3" s="1"/>
+      <c r="Z3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB3" s="1"/>
     </row>
     <row r="4" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
@@ -10464,6 +10470,13 @@
       <c r="W4" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="Z4" s="2"/>
+      <c r="AA4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB4" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="AJ4" s="2" t="s">
         <v>10</v>
       </c>
@@ -10519,6 +10532,15 @@
       </c>
       <c r="W5" s="3">
         <v>0.81230769230769229</v>
+      </c>
+      <c r="Z5" s="2">
+        <v>1</v>
+      </c>
+      <c r="AA5" s="4">
+        <v>5.1911747277417174E-3</v>
+      </c>
+      <c r="AB5" s="4">
+        <v>3.7289262492994912E-2</v>
       </c>
       <c r="AJ5" s="6" t="s">
         <v>12</v>
@@ -10580,6 +10602,16 @@
       <c r="W6" s="3">
         <v>0.79179810725552047</v>
       </c>
+      <c r="Z6" s="2">
+        <f>Z5+1</f>
+        <v>2</v>
+      </c>
+      <c r="AA6" s="4">
+        <v>5.2141855584596922E-3</v>
+      </c>
+      <c r="AB6" s="4">
+        <v>4.0009702819772799E-2</v>
+      </c>
       <c r="AJ6" s="6" t="s">
         <v>13</v>
       </c>
@@ -10640,6 +10672,16 @@
       <c r="W7" s="3">
         <v>0.79939209726443772</v>
       </c>
+      <c r="Z7" s="2">
+        <f t="shared" ref="Z7:Z54" si="4">Z6+1</f>
+        <v>3</v>
+      </c>
+      <c r="AA7" s="4">
+        <v>5.180859693226029E-3</v>
+      </c>
+      <c r="AB7" s="4">
+        <v>3.8074174329044252E-2</v>
+      </c>
       <c r="AJ7" s="6" t="s">
         <v>14</v>
       </c>
@@ -10700,6 +10742,16 @@
       <c r="W8" s="3">
         <v>0.78988941548183256</v>
       </c>
+      <c r="Z8" s="2">
+        <f t="shared" si="4"/>
+        <v>4</v>
+      </c>
+      <c r="AA8" s="4">
+        <v>5.468373495288773E-3</v>
+      </c>
+      <c r="AB8" s="4">
+        <v>3.15431174781119E-2</v>
+      </c>
       <c r="AJ8" s="6" t="s">
         <v>15</v>
       </c>
@@ -10760,6 +10812,16 @@
       <c r="W9" s="3">
         <v>0.8160741885625965</v>
       </c>
+      <c r="Z9" s="2">
+        <f t="shared" si="4"/>
+        <v>5</v>
+      </c>
+      <c r="AA9" s="4">
+        <v>5.1031278821172098E-3</v>
+      </c>
+      <c r="AB9" s="4">
+        <v>4.0175649122820442E-2</v>
+      </c>
       <c r="AJ9" s="6" t="s">
         <v>16</v>
       </c>
@@ -10820,6 +10882,16 @@
       <c r="W10" s="3">
         <v>0.74763406940063082</v>
       </c>
+      <c r="Z10" s="2">
+        <f t="shared" si="4"/>
+        <v>6</v>
+      </c>
+      <c r="AA10" s="4">
+        <v>5.2784055957786208E-3</v>
+      </c>
+      <c r="AB10" s="4">
+        <v>4.2036394828651368E-2</v>
+      </c>
       <c r="AJ10" s="6" t="s">
         <v>17</v>
       </c>
@@ -10880,6 +10952,16 @@
       <c r="W11" s="3">
         <v>0.7828843106180664</v>
       </c>
+      <c r="Z11" s="2">
+        <f t="shared" si="4"/>
+        <v>7</v>
+      </c>
+      <c r="AA11" s="4">
+        <v>5.27454555385221E-3</v>
+      </c>
+      <c r="AB11" s="4">
+        <v>4.1285351829287553E-2</v>
+      </c>
       <c r="AJ11" s="6" t="s">
         <v>18</v>
       </c>
@@ -10940,6 +11022,16 @@
       <c r="W12" s="3">
         <v>0.77300613496932535</v>
       </c>
+      <c r="Z12" s="2">
+        <f t="shared" si="4"/>
+        <v>8</v>
+      </c>
+      <c r="AA12" s="4">
+        <v>5.2925715366095721E-3</v>
+      </c>
+      <c r="AB12" s="4">
+        <v>3.8607968163734678E-2</v>
+      </c>
       <c r="AJ12" s="6" t="s">
         <v>19</v>
       </c>
@@ -11000,6 +11092,16 @@
       <c r="W13" s="3">
         <v>0.80503144654088055</v>
       </c>
+      <c r="Z13" s="2">
+        <f t="shared" si="4"/>
+        <v>9</v>
+      </c>
+      <c r="AA13" s="4">
+        <v>5.4537412613167068E-3</v>
+      </c>
+      <c r="AB13" s="4">
+        <v>3.4528929775381328E-2</v>
+      </c>
       <c r="AJ13" s="6" t="s">
         <v>20</v>
       </c>
@@ -11060,6 +11162,16 @@
       <c r="W14" s="3">
         <v>0.79503105590062106</v>
       </c>
+      <c r="Z14" s="2">
+        <f t="shared" si="4"/>
+        <v>10</v>
+      </c>
+      <c r="AA14" s="4">
+        <v>5.8130660688287912E-3</v>
+      </c>
+      <c r="AB14" s="4">
+        <v>3.2412609188747783E-2</v>
+      </c>
       <c r="AJ14" s="6" t="s">
         <v>21</v>
       </c>
@@ -11120,6 +11232,16 @@
       <c r="W15" s="3">
         <v>0.80804953560371506</v>
       </c>
+      <c r="Z15" s="2">
+        <f t="shared" si="4"/>
+        <v>11</v>
+      </c>
+      <c r="AA15" s="4">
+        <v>5.6025011087142296E-3</v>
+      </c>
+      <c r="AB15" s="4">
+        <v>3.3466712529964887E-2</v>
+      </c>
       <c r="AJ15" s="6" t="s">
         <v>22</v>
       </c>
@@ -11180,6 +11302,16 @@
       <c r="W16" s="3">
         <v>0.7869362363919129</v>
       </c>
+      <c r="Z16" s="2">
+        <f t="shared" si="4"/>
+        <v>12</v>
+      </c>
+      <c r="AA16" s="4">
+        <v>5.4034423904782232E-3</v>
+      </c>
+      <c r="AB16" s="4">
+        <v>3.4399042336621152E-2</v>
+      </c>
       <c r="AJ16" s="6" t="s">
         <v>23</v>
       </c>
@@ -11240,6 +11372,16 @@
       <c r="W17" s="3">
         <v>0.79999999999999993</v>
       </c>
+      <c r="Z17" s="2">
+        <f t="shared" si="4"/>
+        <v>13</v>
+      </c>
+      <c r="AA17" s="4">
+        <v>5.2581342885430751E-3</v>
+      </c>
+      <c r="AB17" s="4">
+        <v>4.2876616713096491E-2</v>
+      </c>
       <c r="AJ17" s="6" t="s">
         <v>24</v>
       </c>
@@ -11300,6 +11442,16 @@
       <c r="W18" s="3">
         <v>0.74882995319812795</v>
       </c>
+      <c r="Z18" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="AA18" s="4">
+        <v>5.2671522738366363E-3</v>
+      </c>
+      <c r="AB18" s="4">
+        <v>3.7045971579997158E-2</v>
+      </c>
       <c r="AJ18" s="6" t="s">
         <v>25</v>
       </c>
@@ -11360,6 +11512,16 @@
       <c r="W19" s="3">
         <v>0.75968992248062017</v>
       </c>
+      <c r="Z19" s="2">
+        <f t="shared" si="4"/>
+        <v>15</v>
+      </c>
+      <c r="AA19" s="4">
+        <v>5.1706973629096617E-3</v>
+      </c>
+      <c r="AB19" s="4">
+        <v>4.0310097637199907E-2</v>
+      </c>
       <c r="AJ19" s="7" t="s">
         <v>26</v>
       </c>
@@ -11420,6 +11582,16 @@
       <c r="W20" s="3">
         <v>0.81298299845440491</v>
       </c>
+      <c r="Z20" s="2">
+        <f t="shared" si="4"/>
+        <v>16</v>
+      </c>
+      <c r="AA20" s="4">
+        <v>5.4670301867762042E-3</v>
+      </c>
+      <c r="AB20" s="4">
+        <v>3.2025653440341521E-2</v>
+      </c>
     </row>
     <row r="21" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C21" s="2">
@@ -11471,6 +11643,16 @@
       <c r="W21" s="3">
         <v>0.79198767334360565</v>
       </c>
+      <c r="Z21" s="2">
+        <f t="shared" si="4"/>
+        <v>17</v>
+      </c>
+      <c r="AA21" s="4">
+        <v>5.041479712558394E-3</v>
+      </c>
+      <c r="AB21" s="4">
+        <v>4.218228158604679E-2</v>
+      </c>
     </row>
     <row r="22" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C22" s="2">
@@ -11522,6 +11704,16 @@
       <c r="W22" s="3">
         <v>0.79746835443037978</v>
       </c>
+      <c r="Z22" s="2">
+        <f t="shared" si="4"/>
+        <v>18</v>
+      </c>
+      <c r="AA22" s="4">
+        <v>5.424090178761126E-3</v>
+      </c>
+      <c r="AB22" s="4">
+        <v>3.7239089494750542E-2</v>
+      </c>
     </row>
     <row r="23" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C23" s="2">
@@ -11573,6 +11765,16 @@
       <c r="W23" s="3">
         <v>0.78834355828220848</v>
       </c>
+      <c r="Z23" s="2">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="AA23" s="4">
+        <v>5.5196800914131686E-3</v>
+      </c>
+      <c r="AB23" s="4">
+        <v>3.2777826682756493E-2</v>
+      </c>
     </row>
     <row r="24" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C24" s="2">
@@ -11624,6 +11826,16 @@
       <c r="W24" s="3">
         <v>0.7835365853658538</v>
       </c>
+      <c r="Z24" s="2">
+        <f t="shared" si="4"/>
+        <v>20</v>
+      </c>
+      <c r="AA24" s="4">
+        <v>5.3013429000414248E-3</v>
+      </c>
+      <c r="AB24" s="4">
+        <v>4.0414566519607342E-2</v>
+      </c>
     </row>
     <row r="25" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C25" s="2">
@@ -11675,6 +11887,16 @@
       <c r="W25" s="3">
         <v>0.79273827534039343</v>
       </c>
+      <c r="Z25" s="2">
+        <f t="shared" si="4"/>
+        <v>21</v>
+      </c>
+      <c r="AA25" s="4">
+        <v>5.3427424014135657E-3</v>
+      </c>
+      <c r="AB25" s="4">
+        <v>3.618736686420973E-2</v>
+      </c>
     </row>
     <row r="26" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C26" s="2">
@@ -11726,6 +11948,16 @@
       <c r="W26" s="3">
         <v>0.7736757624398074</v>
       </c>
+      <c r="Z26" s="2">
+        <f t="shared" si="4"/>
+        <v>22</v>
+      </c>
+      <c r="AA26" s="4">
+        <v>5.2340150580500533E-3</v>
+      </c>
+      <c r="AB26" s="4">
+        <v>3.7772602686318678E-2</v>
+      </c>
     </row>
     <row r="27" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C27" s="2">
@@ -11777,6 +12009,16 @@
       <c r="W27" s="3">
         <v>0.77862595419847325</v>
       </c>
+      <c r="Z27" s="2">
+        <f t="shared" si="4"/>
+        <v>23</v>
+      </c>
+      <c r="AA27" s="4">
+        <v>5.1169344717237331E-3</v>
+      </c>
+      <c r="AB27" s="4">
+        <v>4.2146481891007059E-2</v>
+      </c>
     </row>
     <row r="28" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C28" s="2">
@@ -11828,6 +12070,16 @@
       <c r="W28" s="3">
         <v>0.81047765793528515</v>
       </c>
+      <c r="Z28" s="2">
+        <f t="shared" si="4"/>
+        <v>24</v>
+      </c>
+      <c r="AA28" s="4">
+        <v>5.2495054542448863E-3</v>
+      </c>
+      <c r="AB28" s="4">
+        <v>3.8206870208343451E-2</v>
+      </c>
     </row>
     <row r="29" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C29" s="2">
@@ -11879,6 +12131,16 @@
       <c r="W29" s="3">
         <v>0.84274809160305331</v>
       </c>
+      <c r="Z29" s="2">
+        <f t="shared" si="4"/>
+        <v>25</v>
+      </c>
+      <c r="AA29" s="4">
+        <v>5.4625795406965947E-3</v>
+      </c>
+      <c r="AB29" s="4">
+        <v>3.3970448276033599E-2</v>
+      </c>
     </row>
     <row r="30" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C30" s="2">
@@ -11930,6 +12192,16 @@
       <c r="W30" s="3">
         <v>0.78980891719745228</v>
       </c>
+      <c r="Z30" s="2">
+        <f t="shared" si="4"/>
+        <v>26</v>
+      </c>
+      <c r="AA30" s="4">
+        <v>5.5194584439677181E-3</v>
+      </c>
+      <c r="AB30" s="4">
+        <v>3.7378100179754278E-2</v>
+      </c>
     </row>
     <row r="31" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C31" s="2">
@@ -11981,6 +12253,16 @@
       <c r="W31" s="3">
         <v>0.82170542635658927</v>
       </c>
+      <c r="Z31" s="2">
+        <f t="shared" si="4"/>
+        <v>27</v>
+      </c>
+      <c r="AA31" s="4">
+        <v>5.5495457232637149E-3</v>
+      </c>
+      <c r="AB31" s="4">
+        <v>3.1297516777640352E-2</v>
+      </c>
     </row>
     <row r="32" spans="3:38" x14ac:dyDescent="0.25">
       <c r="C32" s="2">
@@ -12032,8 +12314,18 @@
       <c r="W32" s="3">
         <v>0.80373831775700932</v>
       </c>
-    </row>
-    <row r="33" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z32" s="2">
+        <f t="shared" si="4"/>
+        <v>28</v>
+      </c>
+      <c r="AA32" s="4">
+        <v>5.5077782644669506E-3</v>
+      </c>
+      <c r="AB32" s="4">
+        <v>4.2105325526634457E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C33" s="2">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -12083,8 +12375,18 @@
       <c r="W33" s="3">
         <v>0.7951070336391437</v>
       </c>
-    </row>
-    <row r="34" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z33" s="2">
+        <f t="shared" si="4"/>
+        <v>29</v>
+      </c>
+      <c r="AA33" s="4">
+        <v>5.4490850418254756E-3</v>
+      </c>
+      <c r="AB33" s="4">
+        <v>3.2878530087935003E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C34" s="2">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -12134,8 +12436,18 @@
       <c r="W34" s="3">
         <v>0.81776416539050534</v>
       </c>
-    </row>
-    <row r="35" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z34" s="2">
+        <f t="shared" si="4"/>
+        <v>30</v>
+      </c>
+      <c r="AA34" s="4">
+        <v>5.3039774358518707E-3</v>
+      </c>
+      <c r="AB34" s="4">
+        <v>4.0712688069284068E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C35" s="2">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -12185,8 +12497,18 @@
       <c r="W35" s="3">
         <v>0.800632911392405</v>
       </c>
-    </row>
-    <row r="36" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z35" s="2">
+        <f t="shared" si="4"/>
+        <v>31</v>
+      </c>
+      <c r="AA35" s="4">
+        <v>5.3688114109919621E-3</v>
+      </c>
+      <c r="AB35" s="4">
+        <v>3.2744975134607383E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C36" s="2">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -12236,8 +12558,18 @@
       <c r="W36" s="3">
         <v>0.7801857585139319</v>
       </c>
-    </row>
-    <row r="37" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z36" s="2">
+        <f t="shared" si="4"/>
+        <v>32</v>
+      </c>
+      <c r="AA36" s="4">
+        <v>5.2471898872556424E-3</v>
+      </c>
+      <c r="AB36" s="4">
+        <v>3.7208707989786413E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C37" s="2">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -12287,8 +12619,18 @@
       <c r="W37" s="3">
         <v>0.76623376623376627</v>
       </c>
-    </row>
-    <row r="38" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z37" s="2">
+        <f t="shared" si="4"/>
+        <v>33</v>
+      </c>
+      <c r="AA37" s="4">
+        <v>5.2342271973812339E-3</v>
+      </c>
+      <c r="AB37" s="4">
+        <v>3.7238410216032927E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C38" s="2">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -12338,8 +12680,18 @@
       <c r="W38" s="3">
         <v>0.78713629402756502</v>
       </c>
-    </row>
-    <row r="39" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z38" s="2">
+        <f t="shared" si="4"/>
+        <v>34</v>
+      </c>
+      <c r="AA38" s="4">
+        <v>5.2655104371927136E-3</v>
+      </c>
+      <c r="AB38" s="4">
+        <v>3.8214392377676931E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C39" s="2">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -12389,8 +12741,18 @@
       <c r="W39" s="3">
         <v>0.77388535031847139</v>
       </c>
-    </row>
-    <row r="40" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z39" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="AA39" s="4">
+        <v>5.3294397660726776E-3</v>
+      </c>
+      <c r="AB39" s="4">
+        <v>3.4714095179805511E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C40" s="2">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -12440,8 +12802,18 @@
       <c r="W40" s="3">
         <v>0.77588871715610508</v>
       </c>
-    </row>
-    <row r="41" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z40" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="AA40" s="4">
+        <v>5.325833668107279E-3</v>
+      </c>
+      <c r="AB40" s="4">
+        <v>3.8117873029251438E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C41" s="2">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -12491,8 +12863,18 @@
       <c r="W41" s="3">
         <v>0.78516228748068007</v>
       </c>
-    </row>
-    <row r="42" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z41" s="2">
+        <f t="shared" si="4"/>
+        <v>37</v>
+      </c>
+      <c r="AA41" s="4">
+        <v>5.4478537952985864E-3</v>
+      </c>
+      <c r="AB41" s="4">
+        <v>3.6167233375428633E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C42" s="2">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -12542,8 +12924,18 @@
       <c r="W42" s="3">
         <v>0.79443585780525494</v>
       </c>
-    </row>
-    <row r="43" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z42" s="2">
+        <f t="shared" si="4"/>
+        <v>38</v>
+      </c>
+      <c r="AA42" s="4">
+        <v>5.2765339452991913E-3</v>
+      </c>
+      <c r="AB42" s="4">
+        <v>3.7476804174930212E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C43" s="2">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -12593,8 +12985,18 @@
       <c r="W43" s="3">
         <v>0.79812206572769939</v>
       </c>
-    </row>
-    <row r="44" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z43" s="2">
+        <f t="shared" si="4"/>
+        <v>39</v>
+      </c>
+      <c r="AA43" s="4">
+        <v>5.3306063923264004E-3</v>
+      </c>
+      <c r="AB43" s="4">
+        <v>3.9127465273078837E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C44" s="2">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -12644,8 +13046,18 @@
       <c r="W44" s="3">
         <v>0.79938744257274119</v>
       </c>
-    </row>
-    <row r="45" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z44" s="2">
+        <f t="shared" si="4"/>
+        <v>40</v>
+      </c>
+      <c r="AA44" s="4">
+        <v>5.4225217959446396E-3</v>
+      </c>
+      <c r="AB44" s="4">
+        <v>3.115448937054368E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C45" s="2">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -12695,8 +13107,18 @@
       <c r="W45" s="3">
         <v>0.80751173708920188</v>
       </c>
-    </row>
-    <row r="46" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z45" s="2">
+        <f t="shared" si="4"/>
+        <v>41</v>
+      </c>
+      <c r="AA45" s="4">
+        <v>5.2318905146100684E-3</v>
+      </c>
+      <c r="AB45" s="4">
+        <v>4.1342842286630592E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C46" s="2">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -12746,8 +13168,18 @@
       <c r="W46" s="3">
         <v>0.80989180834621333</v>
       </c>
-    </row>
-    <row r="47" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z46" s="2">
+        <f t="shared" si="4"/>
+        <v>42</v>
+      </c>
+      <c r="AA46" s="4">
+        <v>5.3057993177645472E-3</v>
+      </c>
+      <c r="AB46" s="4">
+        <v>3.5930833587261388E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C47" s="2">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -12797,8 +13229,18 @@
       <c r="W47" s="3">
         <v>0.77934272300469476</v>
       </c>
-    </row>
-    <row r="48" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z47" s="2">
+        <f t="shared" si="4"/>
+        <v>43</v>
+      </c>
+      <c r="AA47" s="4">
+        <v>5.522080114134317E-3</v>
+      </c>
+      <c r="AB47" s="4">
+        <v>3.2453708552701022E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C48" s="2">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -12848,8 +13290,18 @@
       <c r="W48" s="3">
         <v>0.76265822784810133</v>
       </c>
-    </row>
-    <row r="49" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z48" s="2">
+        <f t="shared" si="4"/>
+        <v>44</v>
+      </c>
+      <c r="AA48" s="4">
+        <v>5.2161367539720971E-3</v>
+      </c>
+      <c r="AB48" s="4">
+        <v>4.0356156507227049E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C49" s="2">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -12899,8 +13351,18 @@
       <c r="W49" s="3">
         <v>0.798165137614679</v>
       </c>
-    </row>
-    <row r="50" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z49" s="2">
+        <f t="shared" si="4"/>
+        <v>45</v>
+      </c>
+      <c r="AA49" s="4">
+        <v>5.4366776615265098E-3</v>
+      </c>
+      <c r="AB49" s="4">
+        <v>3.2899570011463639E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C50" s="2">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -12950,8 +13412,18 @@
       <c r="W50" s="3">
         <v>0.78525641025641035</v>
       </c>
-    </row>
-    <row r="51" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z50" s="2">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="AA50" s="4">
+        <v>5.3271645640347214E-3</v>
+      </c>
+      <c r="AB50" s="4">
+        <v>4.1365252540332888E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C51" s="2">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -13001,8 +13473,18 @@
       <c r="W51" s="3">
         <v>0.79815100154083207</v>
       </c>
-    </row>
-    <row r="52" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z51" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="AA51" s="4">
+        <v>5.0482037532829354E-3</v>
+      </c>
+      <c r="AB51" s="4">
+        <v>4.5024587581712433E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C52" s="2">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -13052,8 +13534,18 @@
       <c r="W52" s="3">
         <v>0.78759689922480625</v>
       </c>
-    </row>
-    <row r="53" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z52" s="2">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="AA52" s="4">
+        <v>5.2478846032914519E-3</v>
+      </c>
+      <c r="AB52" s="4">
+        <v>3.8185897780785648E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C53" s="2">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -13103,8 +13595,18 @@
       <c r="W53" s="3">
         <v>0.78260869565217395</v>
       </c>
-    </row>
-    <row r="54" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z53" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="AA53" s="4">
+        <v>5.2417863278543843E-3</v>
+      </c>
+      <c r="AB53" s="4">
+        <v>3.693099772576542E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C54" s="2">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -13154,8 +13656,18 @@
       <c r="W54" s="3">
         <v>0.81039755351681964</v>
       </c>
-    </row>
-    <row r="55" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z54" s="2">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="AA54" s="4">
+        <v>5.2340891366356194E-3</v>
+      </c>
+      <c r="AB54" s="4">
+        <v>3.8096639259442448E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="3:28" x14ac:dyDescent="0.25">
       <c r="D55" s="5"/>
       <c r="E55" s="5"/>
       <c r="H55" s="15"/>
@@ -13166,8 +13678,10 @@
       <c r="P55" s="5"/>
       <c r="U55" s="5"/>
       <c r="V55" s="5"/>
-    </row>
-    <row r="56" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5"/>
+    </row>
+    <row r="56" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C56" s="2" t="s">
         <v>2</v>
       </c>
@@ -13224,8 +13738,19 @@
         <f>AVERAGE(W5:W54)</f>
         <v>0.79199827166065406</v>
       </c>
-    </row>
-    <row r="57" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="Z56" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA56" s="4">
+        <f>AVERAGE(AA5:AA54)</f>
+        <v>5.3304292949146606E-3</v>
+      </c>
+      <c r="AB56" s="4">
+        <f>AVERAGE(AB5:AB54)</f>
+        <v>3.7322157621411098E-2</v>
+      </c>
+    </row>
+    <row r="57" spans="3:28" x14ac:dyDescent="0.25">
       <c r="C57" s="2" t="s">
         <v>3</v>
       </c>
@@ -13281,6 +13806,17 @@
       <c r="W57" s="3">
         <f>_xlfn.STDEV.S(W5:W54)</f>
         <v>1.8275731132312845E-2</v>
+      </c>
+      <c r="Z57" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA57" s="4">
+        <f>_xlfn.STDEV.S(AA5:AA54)</f>
+        <v>1.4805935773898901E-4</v>
+      </c>
+      <c r="AB57" s="4">
+        <f>_xlfn.STDEV.S(AB5:AB54)</f>
+        <v>3.5363409602866859E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>